<commit_message>
Snugget_load is case sensitive on table/shapefile names
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets.xlsx
+++ b/disasterinfosite/data/snuggets.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinda/seattle-ready/disasterinfosite/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="snuggets.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -1126,9 +1131,6 @@
     <t>&lt;p&gt;&lt;b&gt;Due to the steeper slopes&amp;#44; this area has an increased chance for shallow landslides here&lt;/b&gt;.  Landslides tend to happen when the ground is wet from lots of rain OR from ground shaking caused by earthquakes.  Scroll down to historical events to see if any landslide activity has been documented in your area. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;map&lt;/a&gt;)&lt;/p&gt;</t>
   </si>
   <si>
-    <t>LSLD_steepgradezone</t>
-  </si>
-  <si>
     <t>&lt;p&gt;A &lt;b&gt;LOW CHANCE&lt;/b&gt; (5%) exists of a magnitude 7+ earthquake on the Seattle Fault in the next 50 years&amp;#44; but if it does it will be damaging. &lt;b&gt;Moderate shaking will be felt by nearly everyone. Doors will swing&amp;#44; pictures on walls will rattle&amp;#44; and small objects could fall. Damage will be slight&lt;/b&gt;. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(map)&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -1160,6 +1162,9 @@
   </si>
   <si>
     <t>&lt;p&gt;Are the steep slopes nearby unvegetated? Has it been raining for days? &lt;b&gt;If yes&amp;#44; the steep slopes make it more likely for a landslide to happen here&lt;/b&gt;. Keep an eye out for unstable areas. Especially roads that have been blocked by fallen debris or washed out. &lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;(map)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lsld_steepgradezone</t>
   </si>
 </sst>
 </file>
@@ -2999,10 +3004,10 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J187" sqref="J187"/>
+      <selection pane="bottomRight" activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -3010,7 +3015,7 @@
     <col min="8" max="8" width="53.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3036,7 +3041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3059,7 +3064,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3105,10 +3110,10 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3128,10 +3133,10 @@
         <v>50</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3151,10 +3156,10 @@
         <v>60</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3174,10 +3179,10 @@
         <v>70</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3197,10 +3202,10 @@
         <v>80</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3220,13 +3225,13 @@
         <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3246,10 +3251,10 @@
         <v>50</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3269,10 +3274,10 @@
         <v>60</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3292,13 +3297,13 @@
         <v>70</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3321,7 +3326,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3344,7 +3349,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -3390,7 +3395,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -3413,7 +3418,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -3436,10 +3441,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3490,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3508,7 +3513,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -3531,7 +3536,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -3554,7 +3559,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3600,7 +3605,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3623,7 +3628,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -3646,10 +3651,10 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -3672,7 +3677,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -3695,7 +3700,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -3718,7 +3723,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -3741,7 +3746,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -3764,10 +3769,10 @@
         <v>343</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -3787,13 +3792,13 @@
         <v>47</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3833,7 +3838,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -3853,10 +3858,10 @@
         <v>314</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3876,7 +3881,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -3896,7 +3901,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -3916,7 +3921,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3936,7 +3941,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3956,7 +3961,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3976,7 +3981,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -3996,7 +4001,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -4016,7 +4021,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4036,7 +4041,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="13" customHeight="1">
+    <row r="54" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -4056,7 +4061,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4076,7 +4081,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -4096,7 +4101,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -4116,7 +4121,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -4136,7 +4141,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -4156,7 +4161,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -4176,7 +4181,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -4196,7 +4201,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4216,7 +4221,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -4236,7 +4241,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4256,7 +4261,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4276,7 +4281,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4296,7 +4301,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4316,7 +4321,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4336,7 +4341,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -4356,7 +4361,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -4376,7 +4381,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4396,7 +4401,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -4416,7 +4421,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4436,7 +4441,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4456,7 +4461,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4476,7 +4481,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -4496,7 +4501,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4516,7 +4521,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -4536,7 +4541,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -4556,7 +4561,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4576,7 +4581,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4596,7 +4601,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4616,7 +4621,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4656,7 +4661,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4676,7 +4681,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4696,7 +4701,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4716,7 +4721,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4736,7 +4741,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4756,7 +4761,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4776,7 +4781,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4796,7 +4801,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4816,7 +4821,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4836,7 +4841,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4856,7 +4861,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4876,7 +4881,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4896,7 +4901,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -4916,7 +4921,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -4936,7 +4941,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -4956,7 +4961,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -4976,7 +4981,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4996,7 +5001,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -5016,7 +5021,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -5036,7 +5041,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -5056,7 +5061,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -5076,7 +5081,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -5096,7 +5101,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -5116,7 +5121,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -5136,7 +5141,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -5156,10 +5161,10 @@
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>54</v>
       </c>
@@ -5179,15 +5184,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="12" customFormat="1">
+    <row r="112" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E112" s="13"/>
       <c r="H112" s="14"/>
     </row>
-    <row r="113" spans="1:8" s="12" customFormat="1">
+    <row r="113" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E113" s="13"/>
       <c r="H113" s="14"/>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -5210,7 +5215,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -5233,7 +5238,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -5256,7 +5261,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -5279,7 +5284,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -5302,7 +5307,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -5325,7 +5330,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -5348,7 +5353,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -5371,10 +5376,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -5397,7 +5402,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -5420,7 +5425,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -5443,7 +5448,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -5466,7 +5471,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -5489,7 +5494,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -5512,7 +5517,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -5535,7 +5540,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -5558,10 +5563,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>8</v>
       </c>
@@ -5584,7 +5589,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -5607,7 +5612,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -5630,7 +5635,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -5653,7 +5658,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -5676,7 +5681,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -5699,7 +5704,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -5722,7 +5727,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -5745,7 +5750,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -5768,7 +5773,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -5791,7 +5796,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -5814,7 +5819,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -5837,7 +5842,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -5860,7 +5865,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -5883,7 +5888,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -5906,10 +5911,10 @@
         <v>247</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>8</v>
       </c>
@@ -5932,7 +5937,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -5955,7 +5960,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -5978,7 +5983,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -6001,7 +6006,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -6024,10 +6029,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
         <v>8</v>
       </c>
@@ -6047,10 +6052,10 @@
         <v>147</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -6073,10 +6078,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -6096,7 +6101,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -6116,7 +6121,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -6136,10 +6141,10 @@
         <v>248</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -6162,7 +6167,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -6185,7 +6190,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -6208,7 +6213,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -6231,7 +6236,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -6254,7 +6259,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -6277,7 +6282,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -6300,7 +6305,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -6369,7 +6374,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -6392,7 +6397,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -6412,10 +6417,10 @@
         <v>91</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -6438,7 +6443,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -6461,7 +6466,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -6484,10 +6489,10 @@
         <v>263</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>54</v>
       </c>
@@ -6507,15 +6512,15 @@
         <v>264</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="12" customFormat="1">
+    <row r="179" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E179" s="13"/>
       <c r="H179" s="14"/>
     </row>
-    <row r="180" spans="1:8" s="12" customFormat="1">
+    <row r="180" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E180" s="13"/>
       <c r="H180" s="14"/>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -6523,7 +6528,7 @@
         <v>9</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>106</v>
@@ -6538,7 +6543,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>8</v>
       </c>
@@ -6546,7 +6551,7 @@
         <v>9</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D182" s="15" t="s">
         <v>106</v>
@@ -6561,7 +6566,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>8</v>
       </c>
@@ -6569,7 +6574,7 @@
         <v>9</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D183" s="15" t="s">
         <v>106</v>
@@ -6584,7 +6589,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -6592,7 +6597,7 @@
         <v>9</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>106</v>
@@ -6607,7 +6612,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>8</v>
       </c>
@@ -6615,7 +6620,7 @@
         <v>9</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D185" s="15" t="s">
         <v>106</v>
@@ -6630,7 +6635,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>8</v>
       </c>
@@ -6638,7 +6643,7 @@
         <v>9</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D186" s="15" t="s">
         <v>106</v>
@@ -6653,7 +6658,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -6661,7 +6666,7 @@
         <v>9</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D187" s="15" t="s">
         <v>106</v>
@@ -6676,7 +6681,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>8</v>
       </c>
@@ -6684,7 +6689,7 @@
         <v>9</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>106</v>
@@ -6699,7 +6704,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>8</v>
       </c>
@@ -6707,7 +6712,7 @@
         <v>9</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>106</v>
@@ -6722,14 +6727,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C190" s="8"/>
       <c r="D190" s="15"/>
       <c r="E190"/>
       <c r="F190" s="8"/>
       <c r="H190" s="8"/>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>8</v>
       </c>
@@ -6737,7 +6742,7 @@
         <v>12</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D191" s="15" t="s">
         <v>106</v>
@@ -6752,7 +6757,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>8</v>
       </c>
@@ -6760,7 +6765,7 @@
         <v>12</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D192" s="15" t="s">
         <v>106</v>
@@ -6772,10 +6777,10 @@
         <v>80</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>8</v>
       </c>
@@ -6783,7 +6788,7 @@
         <v>12</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D193" s="15" t="s">
         <v>106</v>
@@ -6795,10 +6800,10 @@
         <v>80</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>8</v>
       </c>
@@ -6806,7 +6811,7 @@
         <v>12</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D194" s="15" t="s">
         <v>106</v>
@@ -6818,10 +6823,10 @@
         <v>80</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>8</v>
       </c>
@@ -6829,7 +6834,7 @@
         <v>12</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D195" s="15" t="s">
         <v>106</v>
@@ -6841,10 +6846,10 @@
         <v>80</v>
       </c>
       <c r="H195" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>8</v>
       </c>
@@ -6852,7 +6857,7 @@
         <v>12</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D196" s="15" t="s">
         <v>106</v>
@@ -6864,10 +6869,10 @@
         <v>80</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>8</v>
       </c>
@@ -6875,7 +6880,7 @@
         <v>12</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D197" s="15" t="s">
         <v>106</v>
@@ -6887,10 +6892,10 @@
         <v>80</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>8</v>
       </c>
@@ -6898,7 +6903,7 @@
         <v>12</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D198" s="15" t="s">
         <v>106</v>
@@ -6910,10 +6915,10 @@
         <v>80</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>8</v>
       </c>
@@ -6921,7 +6926,7 @@
         <v>12</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D199" s="15" t="s">
         <v>106</v>
@@ -6933,15 +6938,15 @@
         <v>80</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C200" s="8"/>
       <c r="D200" s="15"/>
       <c r="E200"/>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
         <v>8</v>
       </c>
@@ -6961,12 +6966,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>8</v>
       </c>
@@ -6989,10 +6994,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>48</v>
       </c>
@@ -7012,7 +7017,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>48</v>
       </c>
@@ -7032,7 +7037,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>48</v>
       </c>
@@ -7052,7 +7057,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>48</v>
       </c>
@@ -7072,10 +7077,10 @@
         <v>344</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>54</v>
       </c>
@@ -7095,7 +7100,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>54</v>
       </c>
@@ -7115,7 +7120,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>54</v>
       </c>
@@ -7135,7 +7140,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>54</v>
       </c>
@@ -7155,7 +7160,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>54</v>
       </c>
@@ -7175,7 +7180,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>54</v>
       </c>
@@ -7195,7 +7200,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>54</v>
       </c>
@@ -7215,7 +7220,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>54</v>
       </c>
@@ -7235,7 +7240,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>54</v>
       </c>
@@ -7255,7 +7260,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>54</v>
       </c>
@@ -7275,15 +7280,15 @@
         <v>281</v>
       </c>
     </row>
-    <row r="220" spans="1:8" s="12" customFormat="1">
+    <row r="220" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E220" s="13"/>
       <c r="H220" s="14"/>
     </row>
-    <row r="221" spans="1:8" s="12" customFormat="1">
+    <row r="221" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E221" s="13"/>
       <c r="H221" s="14"/>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>8</v>
       </c>
@@ -7329,7 +7334,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -7352,7 +7357,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -7375,7 +7380,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>8</v>
       </c>
@@ -7398,10 +7403,10 @@
         <v>286</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D227" s="6"/>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>8</v>
       </c>
@@ -7424,7 +7429,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>8</v>
       </c>
@@ -7447,7 +7452,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>8</v>
       </c>
@@ -7470,7 +7475,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>8</v>
       </c>
@@ -7493,10 +7498,10 @@
         <v>289</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D232" s="6"/>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="8" t="s">
         <v>8</v>
       </c>
@@ -7516,10 +7521,10 @@
         <v>316</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D234" s="6"/>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>8</v>
       </c>
@@ -7539,10 +7544,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D236" s="6"/>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>48</v>
       </c>
@@ -7559,7 +7564,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>48</v>
       </c>
@@ -7576,7 +7581,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>48</v>
       </c>
@@ -7593,10 +7598,10 @@
         <v>291</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D240" s="6"/>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>48</v>
       </c>
@@ -7613,10 +7618,10 @@
         <v>317</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D242" s="6"/>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>54</v>
       </c>
@@ -7633,15 +7638,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="244" spans="1:8" s="12" customFormat="1">
+    <row r="244" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E244" s="13"/>
       <c r="H244" s="14"/>
     </row>
-    <row r="245" spans="1:8" s="12" customFormat="1">
+    <row r="245" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E245" s="13"/>
       <c r="H245" s="14"/>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>8</v>
       </c>
@@ -7664,10 +7669,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D247" s="7"/>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>8</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>8</v>
       </c>
@@ -7713,7 +7718,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>8</v>
       </c>
@@ -7736,7 +7741,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>8</v>
       </c>
@@ -7759,10 +7764,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D252" s="7"/>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>8</v>
       </c>
@@ -7785,10 +7790,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D254" s="7"/>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>48</v>
       </c>
@@ -7808,7 +7813,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>48</v>
       </c>
@@ -7828,7 +7833,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>48</v>
       </c>
@@ -7848,7 +7853,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>48</v>
       </c>
@@ -7868,10 +7873,10 @@
         <v>301</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D259" s="7"/>
     </row>
-    <row r="260" spans="1:8" ht="16" customHeight="1">
+    <row r="260" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>54</v>
       </c>
@@ -7891,15 +7896,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="261" spans="1:8" s="12" customFormat="1">
+    <row r="261" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E261" s="13"/>
       <c r="H261" s="14"/>
     </row>
-    <row r="262" spans="1:8" s="12" customFormat="1">
+    <row r="262" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E262" s="13"/>
       <c r="H262" s="14"/>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>8</v>
       </c>
@@ -7919,10 +7924,10 @@
         <v>302</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D264" s="9"/>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>8</v>
       </c>
@@ -7942,10 +7947,10 @@
         <v>303</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D266" s="9"/>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="8" t="s">
         <v>8</v>
       </c>
@@ -7965,12 +7970,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="D268" s="9"/>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>8</v>
       </c>
@@ -7990,10 +7995,10 @@
         <v>305</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D270" s="9"/>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>48</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>48</v>
       </c>
@@ -8027,7 +8032,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>48</v>
       </c>
@@ -8044,7 +8049,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>48</v>
       </c>
@@ -8061,10 +8066,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D275" s="9"/>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>54</v>
       </c>
@@ -8081,15 +8086,15 @@
         <v>318</v>
       </c>
     </row>
-    <row r="277" spans="1:8" s="12" customFormat="1">
+    <row r="277" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E277" s="13"/>
       <c r="H277" s="14"/>
     </row>
-    <row r="278" spans="1:8" s="12" customFormat="1">
+    <row r="278" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E278" s="13"/>
       <c r="H278" s="14"/>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>8</v>
       </c>
@@ -8109,10 +8114,10 @@
         <v>319</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D280" s="10"/>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>8</v>
       </c>
@@ -8132,10 +8137,10 @@
         <v>320</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D282" s="10"/>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>8</v>
       </c>
@@ -8155,10 +8160,10 @@
         <v>309</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D284" s="10"/>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>8</v>
       </c>
@@ -8178,10 +8183,10 @@
         <v>310</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D286" s="10"/>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>48</v>
       </c>
@@ -8198,7 +8203,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>48</v>
       </c>
@@ -8215,7 +8220,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>48</v>
       </c>
@@ -8232,7 +8237,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>48</v>
       </c>
@@ -8249,10 +8254,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D291" s="10"/>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>54</v>
       </c>
@@ -8272,10 +8277,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added and tested Russian snuggets
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets.xlsx
+++ b/disasterinfosite/data/snuggets.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="1010">
   <si>
     <t>section</t>
   </si>
@@ -11787,6 +11787,721 @@
   </si>
   <si>
     <t>text-cn</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;ВЫСОКАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (84%) того&amp;#44; что в ближайшие 50 лет в этом районе произойдет глубокофокусное землетрясение магнитудой более 6&amp;#44;5. Толчки будут ощущаться такие же&amp;#44; как и при землетрясении Nisqually магнитудой 6&amp;#44;8&amp;#44; которое произошло в 2001 г. Почти все жители этого района почувствуют легкое дрожание.  &lt;b&gt;Будут раскачиваться двери&amp;#44; шататься картины&amp;#44; небольшие предметы могут падать. Разрушения будут незначительными.&lt;/b&gt;  &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;ВЫСОКАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (84%) того&amp;#44; что в ближайшие 50 лет в этом районе произойдет глубокофокусное землетрясение магнитудой более 6&amp;#44;5. Толчки будут ощущаться такие же&amp;#44; как и при землетрясении Nisqually магнитудой 6&amp;#44;8&amp;#44; которое произошло в 2001 г. &lt;b&gt;Из-за значительного дрожания в этом районе будет сложно ходить. С полок попадают книги&amp;#44; стеклянная посуда и другие предметы. Откроются дверцы шкафов и ящики комодов&lt;/b&gt;. Разрушатся дымоходы и некачественно построенные здания. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;ВЫСОКАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (84%) того&amp;#44; что в ближайшие 50 лет в этом районе произойдет глубокофокусное землетрясение магнитудой более 6&amp;#44;5. Толчки будут ощущаться такие же&amp;#44; как и при землетрясении Nisqually магнитудой 6&amp;#44;8&amp;#44; которое произошло в 2001 г. &lt;b&gt;Из-за очень сильного дрожания в этом районе будет трудно устоять на ногах. Мебель начнет двигаться&amp;#44; с полок попадает множество предметов.&lt;/b&gt; Сильно разрушаться некачественно построенные здания. Степень разрушения нормальных зданий будет легкой или умеренной. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует&lt;b&gt;МИНИМАЛЬНАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (5%) того&amp;#44; что в ближайшие 50 лет в зоне Seattle Fault произойдет землетрясение магнитудой более 7. Но если оно произойдет&amp;#44; его последствия будут разрушительны. &lt;b&gt;Почти все жители почувствуют умеренные толчки. Будут раскачиваться двери&amp;#44; шататься картины&amp;#44; небольшие предметы могут падать. Разрушения будут незначительными.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует&lt;b&gt;МИНИМАЛЬНАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (5%) того&amp;#44; что в ближайшие 50 лет в зоне Seattle Fault произойдет землетрясение магнитудой более 7. Но если оно произойдет&amp;#44; его последствия будут разрушительны. Из-за сильного дрожания будет сложно ходить. &lt;b&gt;С полок попадают книги&amp;#44; стеклянная посуда и другие предметы. Разрушатся дымоходы и некачественно построенные здания.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует&lt;b&gt;МИНИМАЛЬНАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (5%) того&amp;#44; что в ближайшие 50 лет в зоне Seattle Fault произойдет землетрясение магнитудой более 7. Но если оно произойдет&amp;#44; его последствия будут разрушительны. &lt;b&gt;Из-за сильных толчков будет трудно устоять на ногах. Мебель начнет двигаться&amp;#44; попадают предметы&lt;/b&gt;. Плохо построенные здания подвергнутся значительным разрушениям&amp;#44; у зданий с хорошим фундаментом будут наблюдаться умеренные повреждения. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(карта) &lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует&lt;b&gt;МИНИМАЛЬНАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (5%) того&amp;#44; что в ближайшие 50 лет в зоне Seattle Fault произойдет землетрясение магнитудой более 7. Но если оно произойдет&amp;#44; его последствия будут разрушительны. &lt;b&gt;Из-за сильных толчков будет трудно устоять на ногах или вести автомобиль. Перевернется тяжелая мебель. Части &lt;a href="http://www.seattle.gov/dpd/codesrules/changestocode/unreinforcedmasonrybuildings/whatwhy/" target=_blank&gt;зданий с неармированной каменной кладкой&lt;/a&gt; разрушатся&amp;#44; каркасные дома сойдут с фундамента&lt;/b&gt;. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует&lt;b&gt;МИНИМАЛЬНАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (5%) того&amp;#44; что в ближайшие 50 лет в зоне Seattle Fault произойдет землетрясение магнитудой более 7. Но если оно произойдет&amp;#44; его последствия будут разрушительны. &lt;b&gt;Из-за сильнейших толчков среди людей быстро распространиться паника. В земле образуются трещины. На крутых склонах произойдут оползни&amp;#44; насыщенная влагой почва пострадает от разжижения.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;УМЕРЕННАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (10–30%) того&amp;#44; что в ближайшие 50 лет на северо-западе произойдет землетрясение магнитудой более 8&amp;#44; подобное Каскадии. &lt;b&gt; Если же это произойдет&amp;#44; жители района почувствуют умеренные толчки&amp;#44; которые будут повторяться в течение всего нескольких минут. Незакрепленные предметы попадают с полок. Дверцы шкафов будут раскачиваться из стороны в сторону&lt;/b&gt;. На многие дни и недели жители останутся без электричества и воды. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;УМЕРЕННАЯ ВЕРОЯТНОСТЬ&lt;b&gt; (10–30 %) того&amp;#44; что в ближайшие 50 лет на северо-западе произойдет землетрясение магнитудой более 8&amp;#44; подобное Каскадии. &lt;b&gt;Если же это произойдет&amp;#44; жители района почувствуют сильные толчки&amp;#44; которые будут повторяться в течение всего нескольких минут. Будет трудно ходить. Разрушиться множество зданий с неармированной каменной кладкой&amp;#44; пострадают люди&lt;/b&gt;. На многие дни и недели жители останутся без электричества и воды. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Существует &lt;b&gt;УМЕРЕННАЯ ВЕРОЯТНОСТЬ&lt;/b&gt; (10–30%) того&amp;#44; что в ближайшие 50 лет на северо-западе произойдет землетрясение магнитудой более 8&amp;#44; подобное Каскадии.&lt;b&gt; Если же это произойдет&amp;#44; жители района почувствуют очень сильные толчки&amp;#44; которые будут повторяться в течение всего нескольких минут. Будет трудно устоять на ногах&amp;#44; пострадает много людей. Улицы засыплет грудами обрушившихся кирпичей и битого стекла.&lt;/b&gt; На многие дни и недели жители останутся без электричества и воды. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Вы находитесь &lt;b&gt;в зоне ВЫСОКОГО риска возникновения цунами&lt;/b&gt;. Через несколько десятков минут после землетрясения вода поднимется на уровень выше головы. Как только прекратятся толчки&amp;#44; НЕМЕДЛЕННО ЭВАКУИРУЙТЕСЬ в более возвышенную местность. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Вы находитесь &lt;b&gt;в зоне ВЫСОКОГО риска возникновения цунами&lt;/b&gt;. Через несколько десятков минут после землетрясения вода поднимется на уровень от колен до головы. Как только прекратятся толчки&amp;#44; НЕМЕДЛЕННО ЭВАКУИРУЙТЕСЬ в более возвышенную местность.&lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Вы находитесь &lt;b&gt;в зоне ВЫСОКОГО риска возникновения цунами&lt;/b&gt;. Вода поднимется примерно до уровня колен&amp;#44; но скорость ее потока будет достаточно сильной&amp;#44; чтобы сбить человека с ног. Всего несколько десятков минут будет на то&amp;#44; чтобы ЭВАКУИРОВАТЬСЯ в более возвышенную местность. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Вы находитесь вне зоны высокого риска возникновения цунами&amp;#44; обозначенной на карте&lt;/b&gt;&amp;#44; но радиус распространения волн цунами может варьироваться от случая к случаю. Живете ли вы или работаете в низкой местности (около 9 м над уровнем моря) вблизи океана? Если да&amp;#44; НЕМЕДЛЕННО ЭВАКУИРУЙТЕСЬ в более возвышенную местность после прекращения сильных толчков. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Если вы находитесь в радиусе 0&amp;#44;4 км от берега&lt;/b&gt;. Если вы находитесь в низкой местности (около 9 м над уровнем моря)&amp;#44; то существует риск возникновения цунами&amp;#44; которое последует за землетрясением. Немедленно переходите на возвышенность. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Если во время землетрясения вы находитесь в лодке&amp;#44; то можете почувствовать прохождение быстро движущихся волн цунами. Будьте готовы к этому. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(карта)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ВЫСОКАЯ&lt;/b&gt;&lt;br&gt;Из-за толчков почва станет очень неустойчивой&amp;#44; будет подобна зыбучим пескам. На улице сквозь трещины дорог могут прорываться потоки воды с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: УМЕРЕННАЯ – ВЫСОКАЯ&lt;/b&gt;&lt;br&gt;Содрогающаяся от толчков почва станет неустойчивой. Ее способность удерживать дома&amp;#44; транспортные средства и другие объекты уменьшится. На улице сквозь трещины дорог могут прорываться потоки воды с песком.  &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: НИЗКАЯ – УМЕРЕННАЯ&lt;/b&gt;&lt;br&gt;В этом районе существует риск возникновения разжижения грунтов. Из-за толчков почва может стать неустойчивой. Дороги могут покрыться трещинами и разрушиться.&lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: НИЗКАЯ&lt;/b&gt;&lt;br&gt;В этом районе возникновение разжижения грунтов маловероятно&amp;#44; если только толчки не будут сильные. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ОЧЕНЬ НИЗКАЯ–НИЗКАЯ&lt;/b&gt;&lt;br&gt;В этом районе возникновение разжижения грунтов маловероятно&amp;#44; если только толчки не будут очень сильные. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ОЧЕНЬ НИЗКАЯ&lt;/b&gt;&lt;br&gt;В этом районе возникновение разжижения грунтов маловероятно&amp;#44; если только толчки не будут очень сильные. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ОТСУТСТВУЕТ&lt;/b&gt;&lt;br&gt;Район находится в материковой зоне&amp;#44; под почвой и осадочными породами — скалистый грунт. Он не подвержен разжижению. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ОТСУТСТВУЕТ&lt;/b&gt;&lt;br&gt;Этот район расположен в торфяной местности. Торф — темная горная порода&amp;#44; похожая на почву&amp;#44; которая состоит из органических веществ. Торф может деформироваться&amp;#44; но разжижению он не подвержен. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность возникновения: ОТСУТСТВУЕТ&lt;/b&gt;&lt;br&gt;Эта местность состоит изо льда и не подвержена разжижению. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;ОЧЕНЬ НИЗКАЯ ПЛОТНОСТЬ ЗАСТРОЙКИ: от 0 до 10 зданий с неармированной каменной кладкой в радиусе 0&amp;#44;4 км.&lt;/b&gt;&lt;br&gt;В таких зданиях сильные толчки землетрясений разрушат кирпичные стены или крыши. Улицы будут захламлены их завалами. Узнайте&amp;#44; где расположены  &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;ближайшие к вам&lt;/a&gt; здания с неармированной каменной кладкой и были ли они реконструированы. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;НИЗКАЯ ПЛОТНОСТЬ ЗАСТРОЙКИ: от 10 до 25 зданий с неармированной каменной кладкой в радиусе 0&amp;#44;4 км.&lt;/b&gt;&lt;br&gt;В таких зданиях сильные толчки землетрясений разрушат кирпичные стены или крыши. Улицы будут захламлены их завалами. Узнайте&amp;#44; где расположены  &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;ближайшие к вам&lt;/a&gt; здания с неармированной каменной кладкой и были ли они реконструированы. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;УМЕРЕННАЯ ПЛОТНОСТЬ ЗАСТРОЙКИ: от 25 до 50 зданий с неармированной каменной кладкой в радиусе 0&amp;#44;4 км.&lt;/b&gt;&lt;br&gt;В таких зданиях сильные толчки землетрясений разрушат кирпичные стены или крыши. Улицы будут захламлены их завалами. Узнайте&amp;#44; где расположены &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;ближайшие к вам&lt;/a&gt; здания с неармированной каменной кладкой и были ли они реконструированы. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;ВЫСОКАЯ ПЛОТНОСТЬ ЗАСТРОЙКИ: от 50 до 100 зданий с неармированной каменной кладкой в радиусе 0&amp;#44;4 км.&lt;/b&gt;&lt;br&gt;Если во время землетрясения вы находитесь в здании с неармированной каменной кладкой&amp;#44; то нужно «Лечь&amp;#44; защититься и не двигаться». Сильные толчки землетрясений разрушат кирпичные стены или крыши таких зданий. Улицы будут захламлены их завалами. Узнайте&amp;#44; где расположены &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;ближайшие к вам&lt;/a&gt; здания с неармированной каменной кладкой и были ли они реконструированы. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;ОЧЕНЬ ВЫСОКАЯ ПЛОТНОСТЬ ЗАСТРОЙКИ: от 100 до 250 зданий с неармированной каменной кладкой в радиусе 0&amp;#44;4 км.&lt;/b&gt;&lt;br&gt;Если во время землетрясения вы находитесь в здании с неармированной каменной кладкой&amp;#44; то нужно «Лечь&amp;#44; защититься и не двигаться». Сильные толчки землетрясений разрушат кирпичные стены или крыши таких зданий. Улицы будут захламлены их завалами. Узнайте&amp;#44; где расположены &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;ближайшие к вам&lt;/a&gt; здания с неармированной каменной кладкой и были ли они реконструированы. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Землетрясения предсказать невозможно&amp;#44; поэтому&amp;#44; если вы чувствуете толчки&amp;#44; — лягте&amp;#44; защититесь и не двигайтесь. Сейчас для жителей Западного побережья разрабатывается система предварительного оповещения. Вы можете узнать больше &lt;a href=http://earthquake.usgs.gov/research/earlywarning/ target="_blank"&gt;здесь&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;РЕПЕТИЦИЯ&lt;/b&gt; - будьте бдительны и повторяйте про себя следующие команды: «Лечь&amp;#44; защититься и не двигаться».&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПЛАН&lt;/b&gt; - составьте домашний план эвакуации (&lt;a href=http://www.fema.gov/media-library-data/0e3ef555f66e22ab832e284f826c2e9e/FEMA_plan_parent_508_071513.pdf target="_blank"&gt;для взрослых&lt;/a&gt; и &lt;a href=http://www.fema.gov/media-library-data/a260e5fb242216dc62ae380946806677/FEMA_plan_child_508_071513.pdf target="_blank"&gt;для детей&lt;/a&gt;) и соберите &lt;a href=http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf target="_blank"&gt;набор для выживания&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДГОТОВКА&lt;/b&gt; - прикрепите предметы&amp;#44; которые могут упасть&amp;#44; и запомните&amp;#44; где выключаются вода&amp;#44; газ&amp;#44; электричество.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;ЕСЛИ ВЫ ВНУТРИ ДОМА — ОСТАВАЙТЕСЬ ТАМ!&lt;/b&gt; Укройтесь под прочным письменным или кухонным столом вдали от объектов&amp;#44; которые могут на вас упасть&amp;#44; и не двигайтесь. НЕ выбегайте наружу&amp;#44; пока не прекратятся толчки. &lt;/li&gt;&lt;li&gt;&lt;b&gt;ЕСЛИ ВЫ НА УЛИЦЕ — ВЫЙДИТЕ НА ОТКРЫТУЮ МЕСТНОСТЬ&amp;#44; &lt;/b&gt; которая находится вдали от зданий&amp;#44; линий электропередач&amp;#44; дымоходов и других предметов&amp;#44; которые могут на вас упасть. &lt;/li&gt;&lt;li&gt;&lt;b&gt;ЕСЛИ ВЫ ВЕДЕТЕ АВТОМОБИЛЬ — ОСТОРОЖНО ОСТАНОВИТЕСЬ &lt;/b&gt; (не под мостом&amp;#44; не на переходе&amp;#44; не возле линий электропередач и т. п.) и ОСТАВАЙТЕСЬ ВНУТРИ.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ЕСЛИ ВЫ ВБЛИЗИ ОКЕАНА &lt;/b&gt; - следуйте рекомендациям&amp;#44; названным выше&amp;#44; пока не прекратятся толчки. Затем &lt;b&gt;ОТПРАВЛЯЙТЕСЬ НА БОЛЕЕ ВОЗВЫШЕННУЮ МЕСТНОСТЬ&lt;/b&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/EQ_during.jpg" alt="This is a panel of four cartoon images showing what to do during an earthquake if inside&amp;#44; outside&amp;#44; driving&amp;#44; or near the ocean." title="During Earthquake Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;ПОДГОТОВЬТЕСЬ К АФТЕРШОКАМ &lt;/b&gt; (повторные толчки&amp;#44; следующие за главным могут вызвать больше разрушений&amp;#44; чем первоначальный). &lt;ul&gt;&lt;li&gt;Телефонные линии будут перегружены; &lt;b&gt;для поддержания связи с семьей рекомендуется отправлять СМС.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;Проверяйте&amp;#44; есть ли у кого травмы.&lt;/li&gt;&lt;li&gt;Когда вы уже в безопасности&amp;#44; &lt;b&gt;проверьте новости &lt;/b&gt; о чрезвычайной ситуации по радиоприемнику батарейного питания&amp;#44; телевизору&amp;#44; соцсетям. Проверьте сообщения&amp;#44; которые поступают на мобильный телефон.&lt;/li&gt;&lt;li&gt;Группа реагирования на чрезвычайные ситуации будет занята. Поэтому в последующие за землетрясением дни и часы  &lt;b&gt;обращайтесь за поддержкой к друзьям и соседям.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;Если необходимо&amp;#44; регулируйте потребление коммунальных ресурсов&lt;/b&gt;. Подробно о том&amp;#44; когда и как &lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target="_blank"&gt; регулировать потребление газа и воды после землетрясения&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Morgan Junction Park Hub &lt;br&gt;Месторасположение центра: At Morgan Junction Park&amp;#44; &lt;br&gt;6413 California Ave SW&amp;#44; Seattle&amp;#44; WA 98118 &lt;br&gt;Заведующий центром: Cindi Barker&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:cindiLbarker@gmail.com" target="_top"&gt;cindiLbarker@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-933-6968&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/west-seattle/" target=_blank&gt;http://seattleemergencyhubs.org/west-seattle&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;North Highland Park Hub &lt;br&gt;Месторасположение центра: The Highland Park Improvement Club &lt;br&gt;1116 SW Holden St&lt;br&gt;Заведующий центром:требуются волонтеры &lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;South Park Neighborhood Center &lt;br&gt;Месторасположение центра: 8201 10th Ave S&lt;br&gt;Заведующий центром: Dagmar Cronn&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:cronn@oakland.edu" target="_top"&gt;cronn@oakland.edu&lt;/a&gt;&lt;br&gt;Телефон: 206-327-1828&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt; &lt;br&gt;description: Meet by the blue box in the park&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Pigeon Point Hub &lt;br&gt;Месторасположение центра: The intersection of 20th Ave SW &amp; SW Genesee St&amp;#44; Seattle&amp;#44; WA 98106 &lt;br&gt;NW corner of the Park&amp;#44; just north of the school.&lt;br&gt;Заведующий центром: Wade Harper&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:wade.harper@outlook.com" target="_top"&gt;wade.harper@outlook.com&lt;/a&gt;&lt;br&gt;Телефон: 206-455-5407&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Hiawatha Playfield/Community Center (Admiral Hub) &lt;br&gt;Месторасположение центра: At California Ave SW &amp; SW Lander St&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Заведующий центром: Paul Stancik&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:pstancik@mindspring.com" target="_top"&gt;pstancik@mindspring.com&lt;/a&gt;&lt;br&gt;Телефон:будет определен &lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Fauntleroy Church Hub &lt;br&gt;Месторасположение центра: Fauntleroy Church&amp;#44; 9140 California Ave SW&lt;br&gt;Заведующий центром: Gordon Wiehler&lt;br&gt;Адрес электронной почты:: &lt;a href="mailto:gmwinv@Comcast.net" target="_top"&gt;gmwinv@Comcast.net&lt;/a&gt;&lt;br&gt;Телефон:: 206-577-4292&lt;br&gt;Веб-сайт:&lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Providence/Mount St. Vincent&amp;#44; parking lot (Fairmount Hub) &lt;br&gt;Месторасположение центра: At SW Hudson St &amp; 35th Ave SW&amp;#44; Seattle&amp;#44; WA 98126 &lt;br&gt; (meet at the SE parking lot under the flag pole )&lt;br&gt;Заведующий центром: Sharonn Meeks&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:smeeks50@comcast.net" target="_top"&gt;smeeks50@comcast.net&lt;/a&gt;&lt;br&gt;Телефон: 206-938-1007&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Neighborhood House (High Point Hub) &lt;br&gt;Месторасположение центра: At 6400 Sylvan Way SW (note that east of 35th Ave SW&amp;#44; SW Morgan Street becomes Sylvan Way SW). Neighborhood House is next to Lanham Place SW. Meet at the amphitheater. &lt;br&gt;Заведующий центром: Heather Hutchison&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:heather.hutchison@manage" target="_top"&gt;heather.hutchison@manage&lt;/a&gt;&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Ercolini Park Hub &lt;br&gt;Месторасположение центра: At 48th Ave SW &amp; SW Alaska St.&amp;#44; in the park&lt;br&gt;Заведующий центром: Jon Wright&lt;br&gt;Адрес электронной почты:&lt;a href="mailto:ercolini@westseattlebeprepared.org" target="_top"&gt;ercolini@westseattlebeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;EC Hughes Playground (Olympic Heights Hub) &lt;br&gt;Месторасположение центра: At 29th Ave SW &amp; SW Holden St&amp;#44; Seattle&amp;#44; WA 98126&amp;#44; at the NE corner of Hughes Playground.&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Salvation Army&amp;#44; parking lot (South Highland Park Hub) &lt;br&gt;Месторасположение центра: At 9050 16th Ave SW (near SW Barton St.)&amp;#44; the Salvation Army parking lot is the gathering place for this hub.&lt;br&gt;Заведующий центром: требуются волонтеры &lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;North Delridge P-Patch Hub &lt;br&gt;Месторасположение центра: At the P-Patch&amp;#44; located at 5078 25th Ave SW&amp;#44; Seattle&amp;#44; WA&lt;br&gt;Заведующий центром: Jay McNally&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:Newcarissa@gmail.com" target="_top"&gt;Newcarissa@gmail.com &lt;/a&gt;&lt;br&gt;Телефон: 206-484-6613&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Hope Lutheran Church (Alaska Junction Hub) &lt;br&gt;Месторасположение центра: 4456 42nd Ave SW&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Alki Community Center (Alki Hub) &lt;br&gt;Месторасположение центра: At 59th Ave SW &amp; SW Stevens St&amp;#44; Seattle&amp;#44; WA 98116. This is adjacent to Whale Tail Park&amp;#44; near the west edge of the playfield. North side of Alki Playfield&lt;br&gt;Заведующий центром: Tony Fragada (98126)&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:tfragada@yahoo.com" target="_top"&gt;tfragada@yahoo.com&lt;/a&gt; &lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Maa Nyei Lai Ndeic P-Patch Hub &lt;br&gt;Месторасположение центра: 4913 Columbia Dr S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Заведующий центром: Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Hillman City P-Patch Hub &lt;br&gt;Месторасположение центра: 4613 S Lucile St&amp;#44; Seattle&amp;#44; WA 98118 (Corner of South Lucile &amp; 46th Ave South)&lt;br&gt;Заведующий центром: Joanne Tilton&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:Jtilton22@comcast.net" target="_top"&gt;Jtilton22@comcast.net&lt;/a&gt;&lt;br&gt;Телефон: 206-650-2071&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Judkins P-Patch Hub &lt;br&gt;Месторасположение центра: 24th Avenue S &amp; S Norman Street Seattle&amp;#44; WA 98112 (Meeting Location: P-Patch entrance off Norman &amp; 24th Ave S.)&lt;br&gt;Заведующий центром: Jen Ellis&lt;br&gt;Адрес электронной почты:   &lt;a href="mailto:JenniferEllis.206@gmail.com" target="_top"&gt;JenniferEllis.206@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-276-4982&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Fisher Pavilion Hub &lt;br&gt;Месторасположение центра: 2nd Ave N &amp; Thomas St&lt;br&gt;Заведующий центром: MIQA Be Prepared&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт:  &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Interbay Fishermen's Terminal Hub &lt;br&gt;Месторасположение центра: Interbay Fishermen's Terminal&lt;br&gt;Заведующий центром: MIQA Be Prepared&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Eastlake Hub &lt;br&gt;Месторасположение центра: Rogers Playfield&lt;br&gt;Заведующий центром: Amy O'Donnell&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:eastlake.hub@gmail.com" target="_top"&gt;eastlake.hub@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Madison Park Hub &lt;br&gt;Месторасположение центра: 42nd Ave E and E Howe St (at the north side of tennis courts)&lt;br&gt;Заведующий центром: John Madrid&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:johnmadrid@hotmail.com" target="_top"&gt;johnmadrid@hotmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-498-1880&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Sunrise P-Patch Hub &lt;br&gt;Месторасположение центра: 33rd Ave S &amp; S Oregon St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Aaron Deitz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:aarondietz@gmail.com" target="_top"&gt;aarondietz@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-694-3966&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Snoqualmie P-Patch Hub &lt;br&gt;Месторасположение центра: 4549 13th Ave S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Заведующий центром: Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;New Holly Youth &amp; Family P-Patch Hub &lt;br&gt;Месторасположение центра: 32nd Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;New Holly Power P-Patch Hub &lt;br&gt;Месторасположение центра: 7123 S Holly Park Dr&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;New Holly Lucky Garden Hub &lt;br&gt;Месторасположение центра: S Holly St &amp; Shaffer Ave S&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;New Holly 29 P-Patch Hub &lt;br&gt;Месторасположение центра: 29th Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;John C. Little P-Patch Hub &lt;br&gt;Месторасположение центра: 6961 37th Ave S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Dakota P-Patch Hub &lt;br&gt;Месторасположение центра: 2902 S Dakota St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Beacon Food Forest Hub &lt;br&gt; Месторасположение центра:: 15th Ave S &amp; S Dakota St&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Ethiopian Community in Seattle &lt;br&gt;Месторасположение центра: 8323 Rainier Ave S (meet at main building)&lt;br&gt;Заведующий центром: Kassa Kachara&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:kabiso_kass@yahoo.com" target="_top"&gt;kabiso_kass@yahoo.com&lt;/a&gt;&lt;br&gt;Телефон: 206-325-0304&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Angel Morgan P-Patch (Angel Morgan Hub) &lt;br&gt;Месторасположение центра: 3956 S Morgan St&amp;#44; Seattle&amp;#44; WA 98118 (The P Patch is located at 42nd Ave S &amp; S Morgan Street)&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Thistle P-Patch Hub &lt;br&gt;Месторасположение центра: Martin Luther King Jr Way S &amp; S Cloverdale St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;New Holly Rockery &amp; Market Hub &lt;br&gt;Месторасположение центра: S Holly Park Dr &amp; Rockery Dr S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Заведующий центром: Contact Debbie Goetz&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Телефон: 206-684-0517&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Lakewood Seward Park Hub &lt;br&gt;Месторасположение центра: Lakewood Seward Park Community Club - 4916 S. Angeline Street&lt;br&gt;Заведующий центром: Aaron Evanson&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:aaronevanson@gmail.com" target="_top"&gt;aaronevanson@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206.660.3822&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Rainier Beach Community Club Hub &lt;br&gt;Месторасположение центра: Rainier Beach Community Club - VFW Hall &amp;#44; 6038 S. Pilgrim&amp;#44; Seattle  WA  98118&lt;br&gt;Заведующий центром: Ron Angeles&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:ranestoba@comcast.net" target="_top"&gt;ranestoba@comcast.net&lt;/a&gt;&lt;br&gt;Телефон: 206-721-5326 and 206-351-0813&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Queen Anne Bowl &lt;br&gt;Месторасположение центра: 2806 3rd Ave W&lt;br&gt;Заведующий центром: Chris Saether&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:csaether@msn.com" target="_top"&gt;csaether@msn.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Interbay Athletic Complex &lt;br&gt;Месторасположение центра: 3027 17th Ave W&lt;br&gt;Заведующий центром: MIQA Be Prepared&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Magnolia Manor Park &lt;br&gt; Месторасположение центра: 3500 28th Ave W&lt;br&gt;Заведующий центром: MIQA Be Prepared&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Magnolia Metropolitan Market&lt;br&gt;Месторасположение центра: 3830 34th Ave W&lt;br&gt;Заведующий центром: MIQA Be Prepared&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;West Queen Anne Playfield Hub &lt;br&gt;Месторасположение центра: 150 W Blaine St&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен &lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;West Magnolia Playfield Hub &lt;br&gt;Месторасположение центра: 32nd Ave W &amp; W Smith St&amp;#44; South Playfield&amp;#44; Southwest corner&lt;br&gt;Заведующий центром: Frank Gaul&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:ftgaul@gmail.com" target="_top"&gt;ftgaul@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-499-8690&lt;br&gt;Веб-сайт: &lt;a href="http://www.miqabeprepared.org/" target=_blank&gt;http://www.miqabeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Ballard Commons Hub &lt;br&gt;Месторасположение центра: NW 57th &amp; 22nd Ave NW&lt;br&gt;Заведующий центром: Colin Getty&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:k7biowa@gmail.com" target="_top"&gt;k7biowa@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Lower Woodland Playfields Hub &lt;br&gt;Месторасположение центра: Green Lake Way N &amp; N 50th St&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Ravenna Hub &lt;br&gt; Месторасположение центра: 6535 Ravenna Ave NE (Ravenna-Eckstein Community Center parking lot)&lt;br&gt;Заведующий центром: David Ward&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:booksgalore22@gmail.com" target="_top"&gt;booksgalore22@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-523-1161&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Victory Heights Hub &lt;br&gt;Месторасположение центра: Victory Heights Park (1737 NE 106th St)&lt;br&gt;Заведующий центром: Ann Forrest&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:aaforrest@hotmail.com" target="_top"&gt;aaforrest@hotmail.com&lt;/a&gt;&lt;br&gt;Телефон: (360)550-2234&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Epic Life Church Hub &lt;br&gt;Месторасположение центра: Epic Life Church - 10503 Stone Ave N&amp;#44; Seattle&amp;#44; WA 98133&lt;br&gt;Заведующий центром: Larry Chaney&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:larry@epiclifechurch.org" target="_top"&gt;larry@epiclifechurch.org&lt;/a&gt;&lt;br&gt;Телефон: 425-218-8849&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Crown Hill Park Hub &lt;br&gt;Месторасположение центра: NW 92nd &amp; 14th Ave NW&lt;br&gt;Заведующий центром: Dennis Galvin&lt;br&gt;Адрес электронной почты:  &lt;a href="mailto:short.harp@gmail.com" target="_top"&gt;short.harp@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Shilshole Marina Hub &lt;br&gt;Месторасположение центра: Shilshole Marina&amp;#44; 7001 Seaview Ave NW&lt;br&gt;Заведующий центром: Jim Doub&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:jim@portagebaymarine.com" target="_top"&gt;jim@portagebaymarine.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Loyal Heights Playfield Hub&lt;br&gt;Месторасположение центра: NW 77th &amp;amp; 21st Ave NW (2101 NW 77th St&amp;#44; Loyal Heights CC basketball half court)&lt;br&gt;Заведующий центром: Cheryl Dyer&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:cheryldy@msn.com" target="_top"&gt;cheryldy@msn.com&lt;/a&gt;&lt;br&gt;Телефон: 206-784-3724&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Kirke Park Hub&lt;br&gt;Месторасположение центра: 7028 9th Ave NW&lt;br&gt;Заведующий центром: Hugh Kelso&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:HKelso@mac.com" target="_top"&gt;HKelso@mac.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Gilman Park Hub &lt;br&gt;Месторасположение центра: NW 54th &amp;amp; 9th Ave NW&lt;br&gt;Заведующий центром: Linda Frank&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:lindabfrank@gmail.com" target="_top"&gt;lindabfrank@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Ross Playground Hub &lt;br&gt;Месторасположение центра: 4320 4th Ave NW&lt;br&gt;Заведующий центром: Leslie Matthis&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:leslie.matthis@gmail.comv" target="_top"&gt;leslie.matthis@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206.783.1500&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Phinney Neighborhood Center Hub &lt;br&gt;Месторасположение центра: Phinney Neighborhood Center: 6532 Phinney Avenue North&amp;#44; Seattle&amp;#44; WA  98103 (Meeting Place: Phinney Center upper parking area)&lt;br&gt;Заведующий центром: David Baum&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:phinneyhub@gmail.com" target="_top"&gt;phinneyhub@gmail.com &lt;/a&gt;&lt;br&gt;Телефон: 206-913-1021&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Meridian Playfield/Good Shepherd Center Hub &lt;br&gt;Месторасположение центра: 4649 Sunnyside Ave. N&lt;br&gt;Заведующий центром: Brian Shapiro&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:bshapiro@objectarts.net" target="_top"&gt;bshapiro@objectarts.net&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;History House of Greater Seattle Hub &lt;br&gt;Месторасположение центра: 790 N 34th St&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Greenwood Senior Center Hub &lt;br&gt;Месторасположение центра: Greenwood Senior Center: 525 N 85th  Street&amp;#44; Seattle&amp;#44; WA  98103&lt;br&gt;Заведующий центром: Kelly Kasper&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:kelly@ht2consulting.com" target="_top"&gt;kelly@ht2consulting.com&lt;/a&gt;&lt;br&gt;Телефон: 206-397-4283&lt;br&gt;Co-Captain: Noel Frame&lt;br&gt;Co-Captain Адрес электронной почты: &lt;a href="mailto:noel@noelframe.com" target="_top"&gt;noel@noelframe.com&lt;/a&gt; &lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Green Lake Playfield &amp; Community Center Hub &lt;br&gt;Месторасположение центра: 7201 Green Lake Dr N&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Bagley Elementary Hub &lt;br&gt;Месторасположение центра: 7821 Stone Ave N&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Телефон: будет определен&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Maple Leaf Park Hub &lt;br&gt;Месторасположение центра: 1020 NE 82nd St&lt;br&gt;Заведующий центром: Lori Phipps&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:lphipps01@gmail.com" target="_top"&gt;lphipps01@gmail.com&lt;/a&gt;&lt;br&gt;Телефон: 206-947-0309&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Hunter Farm Hub &lt;br&gt;Месторасположение центра: 7730 35th Ave NE&lt;br&gt;Заведующий центром: требуются волонтеры&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Веб-сайт:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;University Heights Center &lt;br&gt;Месторасположение центра: NE 50th Street and University Way NE&lt;br&gt;Заведующий центром: Ray Munger&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:ray@uheightscenter.org" target="_top"&gt;ray@uheightscenter.org&lt;/a&gt;&lt;br&gt;Телефон: 206-527-4278&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Lake City Way SR 522/Fred Meyer Hub &lt;br&gt;Месторасположение центра: 13000 Lake City Way NE (SE corner of lower parking lot)&lt;br&gt;Заведующий центром: Sandy Motzer (98125)&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:sandymotzer@aol.com" target="_top"&gt;sandymotzer@aol.com&lt;/a&gt;&lt;br&gt;Телефон: 206-819-8056&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Luther Memorial Lutheran Church Hub &lt;br&gt;Месторасположение центра: 13047 Greenwood Ave N&lt;br&gt;Заведующий центром: Dale Johnson&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Телефон: 206-362-2980&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Общественные центры помощи в случае возникновения чрезвычайных ситуаций — это места&amp;#44; в которых после бедствия могут собираться соседи с тем&amp;#44; чтобы помогать друг другу. &lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ:&lt;center&gt;&lt;b&gt;Grace Lutheran Church Hub &lt;br&gt; Месторасположение центра: 11051 Phinney Ave N (Greenwood Avenue N &amp; N 112th Street)&lt;br&gt;Заведующий центром: Dale Johnson&lt;br&gt;Адрес электронной почты: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Телефон: 206-362-2980&lt;br&gt;Веб-сайт: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;С 1870 г. в штате Вашингтон произошло 15 мощных землетрясений (магнитудой более 5). Согласно местным преданиям&amp;#44; в 1700 г. здесь также произошло сильнейшее землетрясение (магнитудой более 8)&amp;#44; за которым последовало цунами. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/historical_EQs2.jpg" alt="This is an Image showing the sizes of historical earthquakes in Washington. It shows a magnitude(M) 6.5 in 1949 which is 316 times smaller than M9&amp;#44; M6.9 in 2001 which is 160 times smaller than M9&amp;#44; M7.1 in 1965 which is 79 times smaller than M9&amp;#44; and M9 in 1700." title="Relative sizes of notable earthquakes in Washington State"&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Существует высокая вероятность наводнения в этом районе. Он расположен в зоне поймы реки&amp;#44; в которой вероятность возникновения наводнения составляет раз на сто лет&lt;/b&gt;. Это означает&amp;#44; что существует 25 %-я вероятность того&amp;#44; что в ближайшие 30 лет этот район будет затоплен &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&lt;/a&gt;&amp;#44; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Существует высокая вероятность наводнения в этом районе&lt;/b&gt;. Он расположен в зоне поймы реки&amp;#44; в которой вероятность возникновения наводнения составляет раз на сто лет. Это означает&amp;#44; что существует 25 %-я вероятность того&amp;#44; что в ближайшие 30 лет этот район будет затоплен &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&lt;/a&gt;&amp;#44; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе возникновение наводнения маловероятно&lt;/b&gt;. Во время наводнений и сильных штормов уровень воды в реке может подняться незначительно.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе возникновение наводнения маловероятно&lt;/b&gt;. Во время наводнений и сильных штормов уровень воды в водохранилище может подняться незначительно. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Во время наводнения переходить мосты может быть опасно&lt;/b&gt;. Если у вас есть подозрения&amp;#44; что мост пострадал во время наводнения&amp;#44; переходите по нему осторожно и сообщите о его повреждении в Центр оповещения о наводнении&amp;#44; позвонив по номеру 206-296-82-00 или по номеру 800-945-92-63. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Этот район находится вне зон высокого риска возникновения наводнений&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;. НО&amp;#44; если вы живете возле ручья или небольшой реки&amp;#44; знайте&amp;#44; что в них тоже может произойти наводнение. Для получения более подробной информации посетите  &lt;a href=http://www.kingcounty.gov/depts/dnrp/wlr/sections-programs/river-floodplain-section.aspx target=_blank&gt;веб-сайт&amp;#44; посвященный противопаводочным мероприятиям&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;В прошлом&amp;#44; когда на Сиэтл обрушивались сильные ливни&amp;#44; этот район был затоплен&lt;/b&gt;. Это может произойти снова&amp;#44; если в результате сильного шторма водные бассейны выйдут из берегов. Прокрутите вниз&amp;#44; чтобы узнать&amp;#44; как подготовиться. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Дождь&amp;#44; талые воды&amp;#44; или то и другое вместе вызывают быстрое повышение уровня воды. Паводковые воды переполняют берега рек&amp;#44; затапливают близлежащие районы и разрушают дороги.  &lt;b&gt;Этот район расположен в зоне поймы реки&amp;#44; где вероятность возникновения наводнения составляет раз на пятьсот лет. Если это произойдет&amp;#44; он будет затоплен&lt;/b&gt;. Существует 6 %-я вероятность того&amp;#44; что в ближайшие 30 лет произойдет наводнение подобного масштаба. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Находящиеся вблизи ручьи&amp;#44; небольшие и крупные реки выходят из берегов. Из-за этого некоторые дороги становятся непроходимыми &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&lt;/a&gt;&amp;#44; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе возникновение наводнения маловероятно&lt;/b&gt;. Из-за сильных штормов уровень воды в близлежащих ручьях&amp;#44; небольших и крупных реках может подняться. Из-за проливных дождей на улицах могут образоваться лужи со стоячей водой. Если вы обнаружили в своей местности наводнение&amp;#44; сообщите об этом в Центр оповещения о наводнении округа Кинг&amp;#44; позвонив по номеру 206-296-82-00 или по номеру 800-945-92-63. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Этот район&amp;#44; расположенный в городской зоне&amp;#44; подвержен наводнениям&lt;/b&gt;. Чем сильнее шторм&amp;#44; тем сильнее наводнение в этом районе. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует высокая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Сидар&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует высокая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Грин-Ривер&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует высокая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Рейджинг-Ривер &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует высокая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Сноквалми&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует высокая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Толт&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует умеренная вероятность того&amp;#44; что в будущем в этом районе будет русло реки Сидар&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует умеренная вероятность того&amp;#44; что в будущем в этом районе будет русло реки Грин-Ривер&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует умеренная вероятность того&amp;#44; что в будущем в этом районе будет русло реки Рейджинг-Ривер &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует умеренная вероятность того&amp;#44; что в будущем в этом районе будет русло реки Сноквалми&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует умеренная вероятность того&amp;#44; что в будущем в этом районе будет русло реки Толт&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует низкая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Грин-Ривер&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует низкая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Сноквалми&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. Чаще всего это происходит во время и после наводнения. &lt;b&gt;Существует низкая вероятность того&amp;#44; что в будущем в этом районе будет русло реки Толт. &lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Как и многое другое&amp;#44; реки следуют пути наименьшего сопротивления и меняют свое русло с течением времени. &lt;b&gt;Пока еще не было проведено исследования&amp;#44; которое бы подтверждало существование вероятности того&amp;#44; что река переместит свое русло в этом районе. Тем не менее&amp;#44; помните о том&amp;#44; что это может произойти.&lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Здесь показана внутренняя часть текущего русла реки. С течением времени расположение русла может меняться. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Прорывы дамбы случаются очень редко. Тем не менее&amp;#44; если произойдет прорыв &lt;a href=https://goo.gl/maps/X2HGtZX6Kyz target=_blank&gt;дамбы George Culmback&lt;/a&gt; или &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;дамбы на реке Толт&lt;/a&gt;&amp;#44; этот район может затопить &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&lt;/a&gt;&amp;#44; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.</t>
+  </si>
+  <si>
+    <t>Прорывы дамбы случаются очень редко. Тем не менее&amp;#44; если произойдет прорыв &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;дамбы на озере Янгс&amp;#44;&lt;/a&gt; существует риск возникновения наводнения в этом районе &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&amp;#44;&lt;/a&gt; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.</t>
+  </si>
+  <si>
+    <t>Прорывы дамбы случаются очень редко. Тем не менее&amp;#44; если произойдет прорыв &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;дамбы на озере Янгс&amp;#44;&lt;/a&gt; существует умеренный риск возникновения наводнения в этом районе &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&amp;#44;&lt;/a&gt; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.</t>
+  </si>
+  <si>
+    <t>Прорывы дамбы случаются очень редко. Тем не менее&amp;#44; если произойдет прорыв &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;дамбы на озере Янгс&amp;#44;&lt;/a&gt; существует высокий риск возникновения наводнения в этом районе &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&amp;#44;&lt;/a&gt; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон. Прорывы дамбы случаются очень редко.</t>
+  </si>
+  <si>
+    <t>Прорывы дамбы случаются очень редко. Тем не менее&amp;#44; если произойдет прорыв &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;дамбы на реке Толт&amp;#44;&lt;/a&gt; этот район может затопить &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(карта)&lt;/a&gt;. Подпишетесь&amp;#44; чтобы получать оповещения о наводнениях &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;по электронной почте или на телефон в виде СМС&amp;#44;&lt;/a&gt; или загрузите &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;приложение&amp;#44; оповещающее о наводнениях&amp;#44;&lt;/a&gt; на смартфон.</t>
+  </si>
+  <si>
+    <t>Ожидается&amp;#44; что в ближайшие 50 лет возрастет количество сильных штормов с дождями и снегом. Повышение уровня воды рек приведет к большему количеству наводнений осенью и зимой. Щелкните изображение&amp;#44; чтобы узнать больше.&lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Rivers.jpg" alt="Climate Change Rivers Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Идет сильный дождь или дождь&amp;#44; который не прекращается в течение многих дней? Высокая температура вызвала стремительное таяние снега в горах? Уровень воды в местных реках поднялся? Вероятность возникновения наводнения может возрасти. Проверяйте прогноз погоды&amp;#44; чтобы не пропустить оповещений о происходящих катаклизмах.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;СОСТАВЬТЕ ПЛАН&lt;/b&gt; - составьте план действий в случае наводнения. &lt;b&gt;Заранее подготовьте все ценные вещи&lt;/b&gt; (свидетельства о рождении&amp;#44; важные документы&amp;#44; фотографии и т. п.). Приобретите страховку от наводнения&amp;#44; если нужно.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДГОТОВЬТЕСЬ&lt;/b&gt; - переместите ценные вещи и предметы бытовой химии на верхние этажи и &lt;b&gt;узнайте&amp;#44; как отключить&lt;/b&gt; (&lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target=_blank&gt;воду&amp;#44; газ и электричество&lt;/a&gt;).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;ПЕРЕД ЭВАКУАЦИЕЙ&lt;/b&gt; - соберите предметы первой необходимости (теплая одежда&amp;#44; фонарик&amp;#44; мобильный телефон&amp;#44; переносное радио и т. п.). Если есть время и необходимость&amp;#44; отключите газ&amp;#44; воду&amp;#44; электричество.&lt;/li&gt;&lt;li&gt;&lt;b&gt;СЛУШАЙТЕ НОВОСТИ&lt;/b&gt; - при соответствующих рекомендациях эвакуируйтесь в более возвышенные места.&lt;/li&gt;&lt;li&gt;&lt;b&gt;НЕ ПОДВЕРГАЙТЕ СЕБЯ РИСКАМ - НЕ переходите вброд через потоки воды и не ведите автомобиль.&lt;/b&gt; Движущиеся потоки воды высотой всего 15 см могут сбить человека с ног&amp;#44; а высотой 61 см — снести с дороги автомобиль.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Flood_during.jpg" alt="This is a panel of four cartoon images showing what to do during an a flood collect essentials&amp;#44; get to high ground&amp;#44; avoid water&amp;#44; and shutt off utilities." title="During Flood Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Если ваш дом затопило&amp;#44; &lt;b&gt;входить в него следует осторожно&amp;#44; поскольку возможно повреждение конструкции&lt;/b&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Позаботьтесь о том&amp;#44; чтобы специалист проверил газ&amp;#44; воду&amp;#44; электричество &lt;/b&gt; перед тем&amp;#44; как вы их включите.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Задокументируйте информацию об ущербе:&lt;/b&gt; сфотографируйте разрушения и составьте смету затрат на ремонт. &lt;li&gt;Узнайте больше &lt;a href=http://www.kingcounty.gov/services/environment/water-and-land/flooding/prepare.aspx target=_blank&gt;здесь&lt;/a&gt;&lt;/b&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Russell Road Park &lt;br&gt; на перекрестке Russell Rd. и S. 240th St.&lt;br&gt; Kent&amp;#44; WA&amp;#44; 98032 &lt;br&gt;  Заполнять мешки песком нужно самостоятельно.&lt;br&gt; Время работы: пн–пт с 8:00 - 16:00 &lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&amp;#44;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt;Public Works Shops &lt;br&gt;1155 East North Bend Way &lt;br&gt; North Bend&amp;#44; WA 98045&lt;br&gt; мешки песком и песком&lt;br&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; 33100 NE 45th Street &lt;br&gt; Carnation&amp;#44; WA 98014 &lt;br&gt;Время работы: пн–пт с 8:00 - 16:30 &lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Meadowbrook Community Center&lt;br&gt;10517 35th Ave. NE &lt;br&gt; Seattle&amp;#44; WA 98125&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; 1305 C St. SW &lt;br&gt; Auburn&amp;#44; WA 98001&lt;br&gt; Время работы: пн–пт с 6:30 - 16:00&lt;br&gt;мешки песком и песком --&gt;253-931-3048&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Kent City Public Works&lt;br&gt; 5821 S. 240th St. &lt;br&gt; Kent&amp;#44; WA 98032&lt;br&gt; Время работы: пн–пт с 8:00 - 16:00 &lt;br&gt;мешки песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Tahoma School District &lt;br&gt; 23015 SE 216th Way&lt;br&gt; Maple Valley&amp;#44; WA 98038&lt;br&gt; 8:00 - 17:00&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Pacific City Park &lt;br&gt; 600 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Pacific/Algona Community Center &lt;br&gt; 100 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047 &lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; City Property @ &lt;br&gt; Railroad Avenue SE и SE King Street &lt;br&gt; Snoqualmie&amp;#44; WA 98065&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Preston-Snoqualmie Trail parking lot &lt;br&gt; Lake Alice Road SE и SE 56th Place &lt;br&gt; Fall City&amp;#44; WA 98024&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; 14701 Main St. NE &lt;br&gt; Duvall&amp;#44; WA 98019&lt;br&gt;мешки песком и песком--&gt;425-788-3332&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Haller Lake Neighborhood &lt;br&gt; 12551 Ashworth Ave N.&lt;br&gt; Seattle&amp;#44; WA 98133&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; South Park Neighborhood &lt;br&gt; 731 S. Sullivan &lt;br&gt; Seattle&amp;#44; WA 98108&lt;br&gt;мешки песком и песком&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Приготовьтесь к наводнению: приобретите и заполните мешки с песком. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;p&gt;БЛИЖАЙШИЕ К ВАМ ЦЕНТРЫ ВЫДАЧИ МЕШКОВ С ПЕСКОМ  &lt;center&gt;&lt;b&gt; Delridge Community Center &lt;br&gt; 4501 Delridge Way SW &lt;br&gt; Seattle&amp;#44; WA 98106&lt;br&gt;мешки песком и песком &lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Так как в округе Кинг много рек&amp;#44; наводнение — обычное явление во время ливней или быстрого таяния снега. &lt;b&gt;Чаще всего наводнение происходит в период между ноябрем и февралем&lt;/b&gt;&amp;#44; но оно может произойти в любую минуту&amp;#44; если для этого есть подходящие условия.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Это местность с пологими откосами&amp;#44; возникновение оползней здесь маловероятно&lt;/b&gt;. Оползни обычно происходят вследствие переувлажнения земли от большого количества осадков ИЛИ же их вызывают толчки землетрясений. Прокрутите вниз до заголовка «исторические события»&amp;#44; чтобы узнать&amp;#44; были ли зафиксированы оползни в вашем районе. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Из-за крутых склонов в этом районе существует большая вероятность возникновения оползней по сравнению с районом с пологими склонами&lt;/b&gt;. Оползни обычно происходят вследствие переувлажнения земли от большого количества осадков ИЛИ же их вызывают толчки землетрясений. Прокрутите вниз до заголовка «исторические события»&amp;#44; чтобы узнать&amp;#44; были ли зафиксированы оползни в вашем районе. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе возникновение оползня маловероятно&amp;#44; но он может произойти в соседнем районе&amp;#44; который расположен в местности с крутыми склонами&amp;#44; если для этого есть подходящие условия. &lt;/b&gt; Обращайте внимание на районы с неустойчивой почвой. Особенно на дороги&amp;#44; заблокированные обломками горных пород или размытые потоками воды. &lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Находящиеся поблизости крутые склоны лишены растительности? Дождь не прекращается в течение многих дней? &lt;b&gt;Если да&amp;#44; то вероятность возникновения оползня в этом районе выше&amp;#44; так как здесь крутые склоны&lt;/b&gt;. Обращайте внимание на районы с неустойчивой почвой. Особенно на дороги&amp;#44; заблокированные обломками горных пород или размытые потоками воды.  (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Часто оползни наблюдают вдоль высоких крутых океанических берегов&amp;#44; которые размываются волнами. &lt;b&gt;С 1913 г. уровень воды в заливе Пьюджет повысился на 20 см&lt;/b&gt;! При повышении уровня воды вероятность возникновения береговой эрозии возрастает. Избыточное количество осадков в результате сильных штормов также может привести к размыву крутых склонов&amp;#44; что в свою очередь вызовет больше оползней в округе Кинг. Щелкните изображение&amp;#44; чтобы узнать больше.&lt;br&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storms Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Слышен треск ломающихся деревьев&amp;#44; грохот столкновения огромных валунов или же гул земли? В рельефе обнаружились трещины или же с холмов движется масса земли&amp;#44; камней&amp;#44; растительности? Возможно&amp;#44; это оползень. Перейдите в местность с устойчивой почвой.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;ОЦЕНКА&lt;/b&gt; - узнайте&amp;#44; может ли случиться в районе вашего проживания оползень. Для этого &lt;b&gt;&lt;b&gt;обратитесь к инженерам-геотехникам&lt;/b&gt;. Они оценят риск возникновения оползня и/или разработают профилактические мероприятия&amp;#44; направленные на снижение риска возникновения оползня.&lt;/li&gt;&lt;li&gt;&lt;b&gt;УМЕНЬШЕНИЕ РИСКА&lt;/b&gt; -  высадите растения вдоль склонов холмов и/или соорудите поддерживающие стены для&lt;b&gt; их укрепления.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;3. ПОДГОТОВКА&lt;/b&gt; - &lt;b&gt;соберите набор для выживания и составьте домашний план эвакуации &lt;/b&gt;&amp;#44; в котором должно быть по крайней мере два эвакуационных маршрута.&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Самый верный путь остаться невредимыми — не подходить близко в движущемуся оползню или грязевому потоку.&lt;/b&gt; Специалисты геологической службы США также рекомендуют следующее: &lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;&lt;b&gt;БУДЬТЕ БДИТЕЛЬНЫ - обращайте внимание на необычные звуки&lt;/b&gt;. Резко барабанящий дождь может таить в себе чрезвычайную опасность&amp;#44; особенно если до этого в течение длительного времени шли проливные дожди и на улице сыро.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДУМАЙТЕ О ТОМ&amp;#44; ЧТОБЫ ПОКИНУТЬ ДОМ&lt;/b&gt; - если вы находитесь в районах&amp;#44; которые подвержены оползням и грязевым потокам&amp;#44; рассмотрите вариант отъезда&amp;#44; если это безопасно. Если же вы решили остаться дома&amp;#44; то&amp;#44; если это возможно&amp;#44; поднимитесь на второй этаж.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ОБРАЩАЙТЕ ВНИМАНИЕ НА УРОВЕНЬ ВОДЫ&lt;/b&gt; - если вы находитесь недалеко от ручья или у русла реки&amp;#44; &lt;b&gt;обращайте внимание на резкое увеличение или уменьшение уровня воды&amp;#44; а также на ее помутнение&lt;/b&gt;. Это могут быть признаки движущегося выше по течению оползня. РЕАГИРУЙТЕ БЫСТРО! Спасайте свою жизнь&amp;#44; а не имущество.&lt;/li&gt;&lt;/ul&gt; Больше советов от Геологической служба США о том&amp;#44; как вести себя во время оползня можно найти &lt;a href=http://landslides.usgs.gov/learn/prepare.php target=_blank&gt;здесь&lt;/a&gt;. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Landslide_during.jpg" alt="This is a panel of three cartoon images showing what to do during an a landslide. Stay Alert&amp;#44; Leave the area&amp;#44; and Don't Delay." title="During Landslide Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;БУДЬТЕ ГОТОВЫ К НАВОДНЕНИЮ (оползни часто загромождают реки&amp;#44; в результате чего те выходят из берегов)&lt;/b&gt;.&lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;Держитесь подальше от потоков оползня. За главным оползнем могут последовать и другие.&lt;/li&gt;&lt;li&gt;Когда опасность миновала&amp;#44; проверьте&amp;#44; есть ли травмированные или попавшие под завалы люди.&lt;/li&gt;&lt;li&gt;Проверьте&amp;#44; не повреждены ли газопроводы&amp;#44; трубопроводы или линии энергоснабжения. Если да&amp;#44; то сообщите об этом в соответствующую службу.&lt;/li&gt;&lt;li&gt;Узнавайте актуальную информацию из местных СМИ или по радио NOAA Weather Radio.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Подробную информацию по &lt;a href=http://www.dnr.wa.gov/programs-and-services/geology/geologic-hazards/landslides#some-historic-landslides-in-washington-state target=_blank&gt;оползням&lt;/a&gt; и &lt;a href=http://file.dnr.wa.gov/publications/ger_fs_landslide_hazards.pdf target=_blank&gt;рискам возникновения оползней&lt;/a&gt;. можно узнать на веб-странице Департамента природных ресурсов. Доступную информацию по оползням в вашем районе можно найти на сайтах города Сиэтл и округа Кинг.&lt;br&gt;&lt;br&gt;&lt;a href=http://www.seattle.gov/dpd/aboutus/whoweare/emergencymanagement target=_blank&gt;&lt;b&gt;округ Кинг&lt;/b&gt;&lt;/a&gt; &lt;br&gt; &lt;a href=http://www.kingcounty.gov/services/environment/water-and-land/landslides.aspx target=_blank&gt;&lt;b&gt;город Сиэтл&lt;/b&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе оползни не были обнаружены&lt;/b&gt; (&lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;отчет за 2016 г&lt;/a&gt;). Чаще всего оползни встречаются на голых&amp;#44; крутых склонах холмов&amp;#44; то есть там&amp;#44; где свободно проходит поток воды. Если ваше жилье находится ниже подобных районов&amp;#44; помните&amp;#44; что вы подвержены риску (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg=en target=_blank&gt;карта&lt;/a&gt;). Более подробную информацию о слоях горных пород можно найти на&lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;  электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе оползни не были обнаружены&lt;/b&gt;. Подробную информацию можно найти в &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;отчете за 2016 г.&lt;/a&gt; и на &lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;карте&lt;/a&gt;. Более подробную информацию о слоях горных пород можно найти на&lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt; электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Согласно исследованию по оползням&amp;#44; проведенному в 1995 г. для города Сиэтл&amp;#44;&lt;b&gt; в этом районе оползни не были обнаружены &lt;/b&gt; (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;карта&lt;/a&gt;).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе пока не проводили исследованный&amp;#44;&lt;/b&gt; посвященных происходящим в прошлом оползням (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Однажды в прошлом &lt;b&gt;В ЭТОМ РАЙОНЕ БЫЛ ОПОЛЗЕНЬ&lt;/b&gt; (см. &lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;отчет за 2016 г.&lt;/a&gt;) и (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;). То&amp;#44; что в этом районе происходили оползни в прошлом&amp;#44; необязательно может свидетельствовать о вероятности возникновения оползней в будущем. Для того&amp;#44; чтобы узнать&amp;#44; существует ли еще вероятность возникновения оползней&amp;#44; нужно привлечь специалистов-геотехников&amp;#44; которые проведут оценку местности. Более подробную информацию о слоях горных пород можно найти на &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Однажды в прошлом &lt;b&gt;В ЭТОМ РАЙОНЕ БЫЛ ОПОЛЗЕНЬ &lt;/b&gt; (см. &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;отчет за 2016 г.&lt;/a&gt;) и (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;). То&amp;#44; что в этом районе происходили оползни в прошлом&amp;#44; необязательно может свидетельствовать о вероятности возникновения оползней в будущем. Для того&amp;#44; чтобы узнать&amp;#44; существует ли еще вероятность возникновения оползней&amp;#44; нужно привлечь специалистов-геотехников&amp;#44; которые проведут оценку местности. Более подробную информацию о слоях горных пород можно найти на &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Однажды в прошлом &lt;b&gt;В ЭТОМ РАЙОНЕ БЫЛ ОПОЛЗЕНЬ И ОБВАЛ&lt;/b&gt; (см. &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;отчет за 2016 г.&lt;/a&gt;) и (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;). То&amp;#44; что в этом районе происходили оползни в прошлом&amp;#44; необязательно может свидетельствовать о вероятности возникновения оползней в будущем. Для того&amp;#44; чтобы узнать&amp;#44; существует ли еще вероятность возникновения оползней&amp;#44; нужно привлечь специалистов-геотехников&amp;#44; которые проведут оценку местности. Более подробную информацию о прослойках горных пород можно найти на &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt; электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Однажды в прошлом &lt;b&gt;В ЭТОМ РАЙОНЕ БЫЛ ОПОЛЗЕНЬ И ОБВАЛ&lt;/b&gt; (см. &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;отчет за 2016 г.&lt;/a&gt;) и (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;). То&amp;#44; что в этом районе происходили оползни в прошлом&amp;#44; необязательно может свидетельствовать о вероятности возникновения оползней в будущем. Для того&amp;#44; чтобы узнать&amp;#44; существует ли еще вероятность возникновения оползней&amp;#44; нужно привлечь специалистов-геотехников&amp;#44; которые проведут оценку местности. Более подробную информацию о прослойках горных пород можно найти на &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;электронной карте округа Кинг&lt;/a&gt; (в легенде карты должен быть установлен флажок «оползни»).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Согласно исследованию по оползням&amp;#44; проведенному в 1995 г. для города Сиэтл&amp;#44; &lt;b&gt;В ЭТОМ РАЙОНЕ БЫЛ ОПОЛЗЕНЬ &lt;/b&gt;(&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;карта&lt;/a&gt;). То&amp;#44; что в этом районе происходили оползни в прошлом&amp;#44; необязательно может свидетельствовать о вероятности возникновения оползней в будущем. Для того&amp;#44; чтобы узнать&amp;#44; существует ли еще вероятность возникновения оползней&amp;#44; нужно привлечь специалистов-геотехников&amp;#44; которые проведут оценку местности.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе существует очень высокий риск возникновения лесного пожара&lt;/b&gt;. Он расположен между жилыми поселениями и лесом. Территория западного Вашингтона подвержена умеренному риску возникновения лесных пожаров. Тем не менее&amp;#44; в восточной части округа Кинг лесные пожары происходят каждый год. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе существует высокий риск возникновения лесного пожара&lt;/b&gt;. Он расположен между жилыми поселениями и лесом. Территория западного Вашингтона подвержена умеренному риску возникновения лесных пожаров. Тем не менее&amp;#44; в восточной части округа Кинг лесные пожары происходят каждый год. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе нет высокого риска возникновения лесного пожара&lt;/b&gt;&amp;#44; но он расположен в 1 км от района&amp;#44; где существует высокий риск возникновения лесного пожара. При подходящих условиях лесной пожар может распространиться и на этот район. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;карта&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе риск возникновения лесного пожара низкий или очень низкий&lt;/b&gt;. Но если вы живете вблизи леса&amp;#44; помните о том&amp;#44; что здесь могут происходить лесные пожары. &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Поскольку это водная зона&amp;#44; риск возникновения лесного пожара здесь отсутствует.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе может случиться сильный лесной пожар&lt;/b&gt;. Его пламя будет распространятся очень быстро и может быстро менять направление. Чтобы его потушить&amp;#44; пожарной бригаде может понадобиться от нескольких дней до нескольких недель. ДЫМ от лесных пожаров может распространяться на большую территорию. Даже если поблизости нет пожаров&amp;#44; само по себе наличие дыма — уже опасный фактор. Проверить качество воздуха в вашем районе можно &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;здесь&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе может случиться лесной пожар&lt;/b&gt;. Его пламя будет распространятся очень быстро и может быстро менять направление. Чтобы его потушить&amp;#44; пожарной бригаде может понадобиться от нескольких дней до нескольких недель. ДЫМ от лесных пожаров может распространяться на большую территорию. Даже если поблизости нет пожаров&amp;#44; само по себе наличие дыма — уже опасный фактор. Проверить качество воздуха в вашем районе можно &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;здесь&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;В этом районе возникновение лесного пожара маловероятно. Но если вы живете возле леса&amp;#44; то вероятность возникновения лесного пожара все же есть&lt;/b&gt;. ДЫМ от лесных пожаров может распространяться на большую территорию. Даже если поблизости нет пожаров&amp;#44; само по себе наличие дыма — уже опасный фактор. Проверить качество воздуха в вашем районе можно  &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;здесь&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Тихоокеанского Северо-Запада значительно возросло&lt;/b&gt;. Судя по всему&amp;#44; эта тенденция продолжиться и в будущем. Лето становится более сухим или же сопровождается большим количеством гроз. А молния&amp;#44; как известно&amp;#44; вызывает пожары. Огромные территории леса могут выгореть&amp;#44; а дым от пожаров — распространиться на близлежащие районы. Щелкните изображение&amp;#44; чтобы узнать больше.&lt;br&gt;&lt;a  ref="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Forests.jpg" alt="Climate Change Forest Infographic"&gt;
+&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Вы видите дым или чувствуете его запах? Предшествовал ли этому затяжной период сухой погоды? Это может быть лесной пожар. Держитесь подальше от активных зон возгорания&amp;#44; а если вы увидели начало пожара&amp;#44; позвоните в службу 9-1-1&amp;#44; чтобы сообщить об этом.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;ОСВОБОДИТЕ ПРОСТРАНСТВО&lt;/b&gt;. Защитите жизни и имущество&amp;#44; создав&lt;b&gt;адаптированное к воздействию огня пространство вокруг вашего дома&lt;/b&gt;&amp;#44; сарая и предприятия. Чтобы узнать&amp;#44; как это сделать&amp;#44; посетите веб-сайт &lt;a href=http://www.firewise.org/wildfire-preparedness.aspx target=_blank&gt;firewise.org&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;НАБЛЮДАЙТЕ ЗА ПОГОДОЙ&lt;/b&gt;. За несколько солнечных дней леса могут высохнуть достаточно&amp;#44; чтобы загореться. Ветреные погодные условия могут привести к тому&amp;#44; что лесные пожары быстро выйдут из-под контроля.&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Firewise_Brochure.jpg" alt="This is an image of ways to prevent wildfire around your home. They include screening decks&amp;#44; pruning trees 6-10 feet from the ground&amp;#44; using fire-resistant wall and roof materials&amp;#44; keeping plants watered&amp;#44; and making sure your driveway can accommodate an emergency vehicle" title="How to Prepare Your Home for Wildfire"&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;СЛЕДИТЕ ЗА НОВОСТЯМИ&lt;/b&gt;. Слушайте местные оповещения о чрезвычайной ситуации по радио и (или) телевизору и будьте готовы к эвакуации в случае необходимости.&lt;/li&gt;&lt;li&gt;&lt;b&gt;УБЕРИТЕ ЛЕГКОВОСПЛАМЕНЯЮЩИЕСЯ МАТЕРИАЛЫ&lt;/b&gt;. Уберите материалы вокруг вашего дома&amp;#44; которые могут загореться (садовые стулья&amp;#44; столы и т. п.).&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДГОТОВЬТЕ СВОЙ ДОМ&lt;/b&gt;. Отодвиньте мягкую мебель подальше от окон. Закройте двери и окна&amp;#44; но не запирайте их.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Fire_during.jpg" alt="This is an icon of an exclaimation point with two triangles behind it" title="During Fire Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Возвращайтесь домой&amp;#44; когда власти сообщат о том&amp;#44; что это безопасно.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Соблюдайте осторожность при входе в выгоревшие зоны&amp;#44;&lt;/b&gt; поскольку опасность все еще может существовать.&lt;/li&gt;
+&lt;li&gt;Проверьте и убедитесь в отсутствии дыма или скрытых тлеющих углей.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Сфотографируйте понесенный ущерб &lt;/b&gt;для целей страхования.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Если вы считаете&amp;#44; что ваше имущество может быть под угрозой&amp;#44; &lt;b&gt;у властей округа Кинг есть информация для землевладельцев&amp;#44; поощрительные программы и обучающие семинары для хозяев&lt;/b&gt;. Вы можете узнать больше &lt;a href=http://www.kingcounty.gov/environment/water-and-land/forestry.aspx target=_blank&gt;здесь&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>На востоке округа Кинг ежегодно случаются небольшие лесные пожары. Как правило&amp;#44; их причиной являются люди. Взгляните&amp;#44; где в прошлом происходили пожары&amp;#44; щелкнув &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_Historic.jpg target=_blank&gt;здесь&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Лахары (вулканические селевые потоки) являются главной опасностью&amp;#44; связанной с горой Рейнир. &lt;b&gt;У людей&amp;#44; которые проживают на юге округа Кинг&amp;#44; есть 1 шанс из 10 стать свидетелем лахара в своей жизни&lt;/b&gt;. Гора Рейнир считается активным вулканом&amp;#44; но до следующего его извержения может пройти много лет.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Если на горе Рейнир образуется лахар&amp;#44; &lt;b&gt;в этой зоне могут наблюдаться наводнения и осадочные породы&amp;#44; такие как грязь&amp;#44; песок&amp;#44; камни и другие обломки&amp;#44; которые будут спускаться вниз по реке из-за лахара&lt;/b&gt;. Это может происходить в течение многих лет и даже десятилетий после лахара. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность того&amp;#44; что в ближайшие 50 лет через этот регион будет протекать лахар с горы Рейнир&amp;#44; составляет 10–40%&lt;/b&gt;. Лахар выглядит как влажный текучий бетон и ведет себя подобным образом. Густая грязь и обломки пород покроют эту зону&amp;#44; если возникнет лахар. Это может серьезно повредить имущество&amp;#44; и для восстановления потребуется много времени. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вероятность того&amp;#44; что в ближайшие 50 лет через эту зону будет протекать лахар с горы Рейнир&amp;#44; составляет 5–10%&lt;/b&gt;. Лахар выглядит как влажный текучий бетон и ведет себя подобным образом. Густая грязь и обломки пород покроют эту зону&amp;#44; если возникнет лахар. Это может серьезно повредить имущество&amp;#44; и для восстановления потребуется много времени. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Вы находитесь ЗА ПРЕДЕЛАМИ ОПАСНОЙ ЗОНЫ&amp;#44; ГДЕ МОЖЕТ ВОЗНИКНУТЬ ЛАХАР&lt;/b&gt;. Если произойдет извержение вулкана Рейнир&amp;#44; этот регион покроет пепел. Он будет очень похож на районы&amp;#44; пострадавшие от извержения вулкана Сент-Хеленс в 1980 году. Толщина слоя пепла будет варьироваться в зависимости от расстояния до вулкана. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(карта)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Как правило&amp;#44; сигналы&amp;#44; свидетельствующие о скором извержении вулкана&amp;#44; можно заметить за несколько дней&amp;#44; а то и месяцев до извержения. &lt;b&gt;Газовая и сейсмическая активность возрастает&amp;#44; а поверхность земли образует возвышенности&amp;#44; поскольку под ней движется магма&lt;/b&gt;. Хотя эти признаки могут быть незаметны для широкой общественности&amp;#44; гора Рейнир постоянно контролируется учеными в рамках &lt;a href=http://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;программы по отслеживанию вулканических рисков Геологической службы США&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;ЗАДАВАЙТЕ ВОПРОСЫ&lt;/b&gt;. Узнайте&amp;#44; какие меры предприняли местные чиновники&amp;#44; чтобы подготовиться к вулканическим событиям. &lt;b&gt;Расспросите у должностных лиц&amp;#44; какой у них план и как они будут общаться с вами во время события&lt;/b&gt;. Вы можете сделать это&amp;#44; обратившись в &lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=_blank&gt;службу по чрезвычайным ситуациям округа Кинг&lt;/a&gt; округа Кинг.&lt;/li&gt;&lt;li&gt;&lt;b&gt;СОСТАВЬТЕ ПЛАН&lt;/b&gt;. Поговорите со своими друзьями и соседями. Если вы находитесь в зоне высокого риска&amp;#44; &lt;b&gt;решите&amp;#44; куда вы направитесь&amp;#44; что вы возьмете с собой и к кому вы обратитесь&lt;/b&gt;.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Во время извержения слушайте новости для получения последних известий и соблюдайте инструкции по действиям в чрезвычайной ситуации.
+&lt;ul&gt;&lt;li&gt;&lt;b&gt;В ЗОНЕ ЛАХАРА: немедленно переместитесь на возвышенность.&lt;/b&gt;&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;НА УЛИЦЕ&lt;/b&gt;: прикрывайте рот&amp;#44; нос и тело&amp;#44; чтобы избежать раздражения. &lt;b&gt;Найдите укрытие&lt;/b&gt;. &lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ВНУТРИ: не открывайте двери и вентиляционные отверстия в доме и оставайтесь в помещении&amp;#44; если не было получено иных указаний&lt;/b&gt;. Положите влажные полотенца у порогов дверей и заклейте лентой окна&amp;#44; которые пропускают воздух. Не заводите двигатели легковых и грузовых автомобилей&amp;#44; чтобы избежать повреждений из-за скопления пепла. Защитите животных и оборудование&amp;#44; перенеся их в дом или в другую крытую зону.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/intensity/Volcano_during.jpg" alt="This is an panel of three images of what to do during a volcanic eruption or lahar. In lahar zone&amp;#44; outside&amp;#44; inside." title="During Volcano Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;После того как непосредственная опасность от извержения миновала&amp;#44; основной задачей будет уборка вулканического пепла.&lt;br&gt;  &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/MtStHel_Yakima_graders.jpg" alt="This image shows two graders shoveling inches of ashfall from Saint Helens' eruption" title="Ashfall Cleanup in Yakima After Mt. Saint Helens"&gt;&lt;li&gt;Выходя на улицу&amp;#44; надевайте защитные очки и маску. &lt;b&gt;Качество воздуха будет плохим&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Не запускайте двигатели транспортных средств&lt;/b&gt;. Если вам необходимо воспользоваться автомобилем&amp;#44; не развивайте высокую скорость (не более 55 км/час) и часто проверяйте масло&amp;#44; масляные и воздушные фильтры. &lt;/li&gt;&lt;li&gt;Вулканический пепел очень тяжелый и может привести к разрушению зданий. Если это безопасно&amp;#44; &lt;b&gt;уберите пепел с крыш и водосточных желобов&lt;/b&gt;.&lt;/li&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Вы можете больше узнать о горе Рейнир и потенциальных опасностях из целого ряда источников: 
+&lt;ul&gt;&lt;li&gt;&lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;мониторинг и другая информация&lt;/a&gt; - сайт Геологической службы США;&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=blank&gt;общая информация по округу Кинг&lt;/a&gt; - сайт округа Кинг;&lt;li&gt;&lt;a href=https://www.nps.gov/mora/planyourvisit/geohazards.htm target=_blank&gt;геологические опасности у горы Рейнир&lt;/a&gt; - сайт Службы национальных парков США;&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.pnsn.org/volcanoes/mount-rainier target=_blank&gt;землетрясения вблизи горы Рейнир&lt;/a&gt; - сайт Тихоокеанской Северо-Западной сейсмической сети.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;На горе Рейнир случалось множество &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_eruption_history.html target=_blank&gt;извержений&lt;/a&gt; и &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_lahars.html target=_blank&gt;лахаров&lt;/a&gt;. Около 500 лет назад селевой поток Electron хлынул с горы и прошел через Пуйаллап до г. Самнер&amp;#44; штат Вашингтон. За тысячи лет до этого множество лахаров спускались вниз по местным рекам&amp;#44; доходя до г. Оберн.  &lt;b&gt;Некоторые города (Северо-Восточная Такома&amp;#44; Ортинг и Пуйаллап) построены на отложениях&amp;#44; которые образовались после лахаров.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;В округе Кинг зима может быть сопряжена с такими явлениями&amp;#44; как минусовые температуры&amp;#44; покрытые льдом дороги и потенциально сильные бури. Снегопады бывают нечасто&amp;#44; и в основном они наблюдаются на больших высотах. &lt;b&gt;Зимние бури могут нести с собой сильные ветры&amp;#44; которые ломают деревья и разрушают линии электропередач.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Сильные снегопады могут привести к серьезной дестабилизации в работе транспорта&amp;#44; служб общественной безопасности и коммунальных служб. &lt;b&gt;Электричество может отсутствовать в течение многих дней.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;В ближайшие 50 лет в Тихоокеанском Северо-Западном регионе будут наблюдаться более сильные бури&lt;/b&gt;. Они могут нести с собой сильные ветры и проливные дожди&amp;#44; ведущие к наводнениям. Зимние мероприятия будут сорваны. В 2015 году был зарегистрирован самый низкий уровень снежного покрова&amp;#44; который составил лишь 4 % от среднего показателя. Теплые зимы могут стать причиной засухи на всей территории штата. Щелкните изображение&amp;#44; чтобы узнать больше. &lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Winter.jpg" alt="Climate Change Winter Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Метеорологи достигли больших успехов в прогнозировании снежных и ледяных бурь. &lt;b&gt;Обращайте внимание на местные прогнозы погоды и зарегистрируйтесь в доступных системах оповещения и предупреждения &lt;/b&gt;(&lt;a href=http://alert.seattle.gov/ target=_blank&gt;Служба оповещения в г. Сиэтл&lt;/a&gt; и &lt;a href=http://www.kingcounty.gov/depts/emergency-management/alert-king-county.aspx target=_blank&gt;Служба оповещения в округе Кинг&lt;/a&gt;)&amp;#44; чтобы получать самую актуальную информацию об ожидающихся неблагоприятных метеоусловиях.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;СДЕЛАЙТЕ ЗАПАСЫ. Запаситесь топливом и необходимыми принадлежностями&amp;#44;&lt;/b&gt; чтобы продержаться несколько дней без электричества&amp;#44; тепла и горячей воды. Подумайте над приобретением генератора и соблюдайте стандарты безопасности.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДГОТОВЬТЕ СВОЙ ДОМ К ЗИМЕ.&lt;/b&gt; Установите окна с двойным переплетом. Выполните теплоизоляцию стен&amp;#44; чердаков и труб. Нанесите уплотняющий состав и герметичную изоляцию на двери и окна. В холодную погоду позволяйте кранам немного протекать&amp;#44; чтобы трубы не замерзали. &lt;b&gt;Узнайте&amp;#44; как перекрываются водяные клапаны (на случай разрыва трубы)&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ПОДГОТОВЬТЕ ВАШИ ТРАНСПОРТНЫЕ СРЕДСТВА К ЗИМЕ.&lt;/b&gt; Топливные баки должны быть по крайней мере наполовину заполнены. Регулярно проверяйте аккумулятор&amp;#44; систему зажигания&amp;#44; радиатор&amp;#44; фары&amp;#44; тормоза и шины. Залейте в резервуары антифриз&amp;#44; масло и стеклоомыватель. &lt;b&gt;Храните необходимые принадлежности для зимней погоды в багажнике.&lt;/b&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;ОСТАВАЙТЕСЬ В КУРСЕ.&lt;/b&gt; Следите за местными новостями по телевизору&amp;#44; через мобильное устройство или радио с питанием от аккумулятора. Соблюдайте инструкции по действиям в чрезвычайной ситуации и учитывайте рекомендации относительно поездок.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ИЗБЕГАЙТЕ ПОЕЗДОК.&lt;/b&gt; Если вам необходимо куда-то поехать&amp;#44; заполните бензобак&amp;#44; оставайтесь на главных дорогах и сообщайте другим о своем маршруте. Не спешите. Если вы застряли&amp;#44; обратитесь за помощью&amp;#44; включите аварийную сигнализацию и оставайтесь у своего автомобиля. Не пытайтесь идти пешком&amp;#44; если поблизости нет укрытия.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ОСОЗНАВАЙТЕ РИСКИ.&lt;/b&gt; 
+&lt;ul&gt;
+&lt;li&gt;&lt;b&gt;Переохлаждение.&lt;/b&gt; Если вы заметили симптомы&amp;#44; немедленно обратитесь за медицинской помощью. Для ознакомления с симптомами и другой информацией щелкните &lt;a href=https://www.cdc.gov/disasters/winter/staysafe/hypothermia.html target=_blank&gt;здесь&lt;/a&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Отравление угарным газом.&lt;/b&gt; Оно случается&amp;#44; когда топливо (например&amp;#44; газ&amp;#44; бензин&amp;#44; керосин&amp;#44; древесина или древесный уголь) сгорает в замкнутом пространстве. Сотни людей погибают таким образом каждый год. Узнайте больше &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/carbon-monoxide.aspx target=_blank&gt;здесь&lt;/a&gt;.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;li&gt;&lt;b&gt;ИЗБЕГАЙТЕ ОПАСНОСТИ.&lt;/b&gt; Держитесь подальше от упавших линий электропередач&amp;#44; затопленных дорог и других сооружений&amp;#44; ослабленных из-за тяжелого снега или льда.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Winter_during.jpg" alt="This is a panel of four images of what to do during bad winter weather. Stay Tuned&amp;#44; Stay Inside&amp;#44; Know Risks&amp;#44; and Avoid Hazards." title="During Winter Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;Обновите запас необходимых принадлежностей&lt;/b&gt;. Подготовьтесь на случай еще одной бури.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Усовершенствуйте свой семейный план&lt;/b&gt;. Что сработало? Что можно было сделать лучше?&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Поговорите со своими соседями&lt;/b&gt;. Поделитесь друг с другом советами и идеями&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Узнайте больше о зимних погодных условиях и о том&amp;#44; как к ним подготовиться.  
+&lt;ul&gt;&lt;li&gt;
+&lt;a href=http://takewinterbystorm.org target=_blank&gt;Покорение зимы &lt;/a&gt;- советы по подготовке и актуальная информация для Западного Вашингтона.&lt;/li&gt;
+&lt;li&gt;
+&lt;a href=http://kingcounty.gov/depts/transportation/metro/alerts-updates/winter.aspx target=_blank&gt;Погодный дайджест округа Кинг &lt;/a&gt; - ссылки на приложения для планирования зимних поездок и штормовые предупреждения.&lt;/li&gt;
+&lt;li&gt;
+&lt;a href=https://www.seattle.gov/transportation/winterweather.htm target=_blank&gt;Департамент транспорта г. Сиэтл&lt;/a&gt; - узнайте&amp;#44; где уже прошли снегоуборочные машины&amp;#44; и другую информацию о дорожных условиях. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Череда снежных&amp;#44; ледяных и ливневых штормов&amp;#44; начавшаяся 26 декабря 1996 года&amp;#44; вызвала 16 смертей в штате и убытки на сумму 57 миллионов долларов США в Сиэтле и округе Кинг&lt;/b&gt;. После двух снежных бурь (во время одной выпало 15–30 см мокрого снега&amp;#44; а во время другой — 25 см) последовал сильный ливень&amp;#44; который разрушил крытые автостоянки&amp;#44; накрыл лодочные причалы и поломал линии электропередач. Впервые за историю метрополитен полностью остановил свою работу. Мороз и таяние снега способствовали наводнениям и оползням в течение следующей недели. Готовы ли вы к тому&amp;#44; что такая буря повторится?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Не позволяйте дождливой осени и зиме ввести вас в заблуждение  - &lt;b&gt;лето в округе Кинг может быть ЖАРКИМ. Иногда температура поднимается до отметки 30 °C и выше на несколько дней подряд&lt;/b&gt;. По всему региону возможны грозы&amp;#44; ураганы&amp;#44; лесные пожары и аномальная жара.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Сильная жара может удерживаться в течение многих дней&amp;#44; в результате чего в сообществах возрастает количество заболеваний&amp;#44; вызванных перегревом&amp;#44; включая ТЕПЛОВОЕ ИСТОЩЕНИЕ и ТЕПЛОВОЙ УДАР. Высокие температуры&amp;#44; сухие погодные условия и повышенная вероятность появления молний могут привести к лесным пожарам.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Июль 2015 года был самым жарким месяцем в истории! &lt;b&gt;Согласно прогнозам&amp;#44; средняя годовая температура возрастет на 3–10 градусов Фаренгейта к 2100 году&lt;/b&gt;. В Вашингтоне будет наблюдаться меньше летних дождей&amp;#44; а когда дожди будут происходить&amp;#44; они будут очень сильными (т. е. проливными). Щелкните изображение&amp;#44; чтобы узнать больше. &lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storm Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Тепловое истощение и тепловой удар — это серьезные заболевания&amp;#44; которые могут возникать&amp;#44; когда человек подвергается воздействию очень высоких температур.&lt;/p&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;ПРИЗНАКИ ТЕПЛОВОГО ИСТОЩЕНИЯ&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;сильное потоотделение;&lt;/li&gt;
+&lt;li&gt;слабость;&lt;/li&gt;
+&lt;li&gt;слабый пульс;&lt;/li&gt;
+&lt;li&gt;Обморок.&lt;/li&gt;
+&lt;li&gt;рвота&lt;/li&gt;
+&lt;li&gt;холодная бледная кожа.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;ПРИЗНАКИ ТЕПЛОВОГО УДАРА&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;высокая температура тела (39 °C и выше);&lt;/li&gt;
+&lt;li&gt;горячая и сухая кожа;&lt;/li&gt;
+&lt;li&gt;быстрый и сильный пульс;&lt;/li&gt;
+&lt;li&gt;возможна потеря сознания.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Пожилые люди&amp;#44; маленькие дети&amp;#44; а также люди с психическими заболеваниями и хроническими болезнями более подвержены риску недомогания&amp;#44; вызванного перегревом.
+&lt;ol&gt;&lt;li&gt;&lt;b&gt;ЗНАЙТЕ ПРИЗНАКИ.&lt;/b&gt; Недомогание&amp;#44; вызванное перегревом&amp;#44; может развиваться быстро. Знайте&amp;#44; кто из ваших соседей может быть подвержен риску. &lt;/li&gt;&lt;li&gt;&lt;b&gt;ОСТАВАЙТЕСЬ В КУРСЕ.&lt;/b&gt; Слушайте местные новости&amp;#44; чтобы узнать общую информацию и местоположение &lt;b&gt;центров охлаждения&lt;/b&gt; (общественные места&amp;#44; которые могут использоваться жителями для охлаждения).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;НЕ ПЕРЕГРЕВАЙТЕСЬ.&lt;/b&gt; Оставайтесь в помещении&amp;#44; а если возможно&amp;#44; в местах с кондиционерами (торговый центр&amp;#44; библиотека&amp;#44; театр и т. п.). Ограничьте активность на открытом воздухе.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ЗАЩИЩАЙТЕ КОЖУ.&lt;/b&gt; Носите легкую&amp;#44; светлую&amp;#44; свободную одежду. Также помогут широкополая шляпа&amp;#44; солнцезащитные очки и солнцезащитный крем.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ПЕЙТЕ ВОДУ.&lt;/b&gt; Пейте много жидкостей (избегайте кофеина&amp;#44; алкоголя и сладких напитков) и носите с собой бутылку воды.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ДУМАЙТЕ О ДРУГИХ.&lt;/b&gt; Не оставляйте детей и домашних животных в жарких автомобилях. Контролируйте состояние родственников&amp;#44; друзей и соседей&amp;#44; находящихся в группе риска.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Summer_during.jpg" alt="This is a panel of three images of what to do during bad summer weather. Stay Cool&amp;#44; Protect Skin&amp;#44; and Drink Water." title="During Summer Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Используйте занавески&amp;#44; чтобы  &lt;b&gt;закрыть окна и удерживать прохладный воздух внутри&lt;/b&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Подумайте над приобретением системы кондиционирования воздуха &lt;/b&gt; и (или) установите герметизирующие прокладки в тех местах&amp;#44; где просачивается горячий воздух. &lt;/li&gt;
+&lt;li&gt;&lt;b&gt;МАЛОБЮДЖЕТНЫЙ ВАРИАНТ.&lt;/b&gt; Используйте теплоотражатели между окнами и занавесками (например&amp;#44; картон&amp;#44; завернутый в алюминиевую фольгу)&amp;#44; чтобы отражать тепло обратно на улицу. Щелкните &lt;a href=http://www.instructables.com/id/Heat-blocking-curtains/ target=_blank&gt;здесь&lt;/a&gt;&amp;#44; чтобы узнать&amp;#44; как сделать это своими руками.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Дополнительную информацию о том&amp;#44; как сохранять хорошее самочувствие и безопасность&amp;#44; можно найти на странице &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/hot-weather.aspx target=_blank&gt;Жара&lt;/a&gt; сайта округа Кинг.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;В 2015 году в округе Кинг было зарегистрировано рекордное количество дней&amp;#44; когда температура превышала 32 °C. &lt;b&gt;Июль 2015 года был самым жарким месяцем&amp;#44; когда-либо зарегистрированным в округе Кинг!&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>text-ru</t>
   </si>
 </sst>
 </file>
@@ -12617,7 +13332,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -12642,6 +13357,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="683">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -13660,13 +14377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J292"/>
+  <dimension ref="A1:K292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13675,9 +14392,10 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="8" max="10" width="53.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13708,8 +14426,11 @@
       <c r="J1" s="1" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="20" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -13737,8 +14458,11 @@
       <c r="J2" s="1" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="21" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -13766,8 +14490,11 @@
       <c r="J3" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="21" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -13795,12 +14522,15 @@
       <c r="J4" s="1" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="21" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -13828,8 +14558,11 @@
       <c r="J6" s="1" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="21" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -13857,8 +14590,11 @@
       <c r="J7" s="1" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="21" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -13886,8 +14622,11 @@
       <c r="J8" s="1" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="21" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -13915,8 +14654,11 @@
       <c r="J9" s="1" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="21" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -13944,12 +14686,15 @@
       <c r="J10" s="1" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="21" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -13977,8 +14722,11 @@
       <c r="J12" s="1" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="21" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -14006,8 +14754,11 @@
       <c r="J13" s="1" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="21" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -14035,12 +14786,15 @@
       <c r="J14" s="1" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="21" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -14068,8 +14822,11 @@
       <c r="J16" s="1" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="21" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -14097,8 +14854,11 @@
       <c r="J17" s="1" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="20" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -14126,8 +14886,11 @@
       <c r="J18" s="1" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="20" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -14155,8 +14918,11 @@
       <c r="J19" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="21" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -14184,8 +14950,11 @@
       <c r="J20" s="1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="21" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -14213,12 +14982,15 @@
       <c r="J21" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="21" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -14246,8 +15018,11 @@
       <c r="J23" s="1" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="20" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -14275,8 +15050,11 @@
       <c r="J24" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="21" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -14304,8 +15082,11 @@
       <c r="J25" s="1" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="21" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -14333,8 +15114,11 @@
       <c r="J26" s="1" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="21" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -14362,8 +15146,11 @@
       <c r="J27" s="1" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="21" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -14391,8 +15178,11 @@
       <c r="J28" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="21" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -14420,8 +15210,11 @@
       <c r="J29" s="1" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="21" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -14449,8 +15242,11 @@
       <c r="J30" s="1" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="21" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -14478,12 +15274,15 @@
       <c r="J31" s="1" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="21" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -14511,8 +15310,11 @@
       <c r="J33" s="1" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="21" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -14540,8 +15342,11 @@
       <c r="J34" s="1" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="21" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -14569,8 +15374,11 @@
       <c r="J35" s="1" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="21" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -14598,8 +15406,11 @@
       <c r="J36" s="1" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="21" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -14627,12 +15438,15 @@
       <c r="J37" s="1" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="21" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -14660,12 +15474,15 @@
       <c r="J39" s="1" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="21" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D40" s="3"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -14690,8 +15507,11 @@
       <c r="J41" s="1" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="21" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -14716,8 +15536,11 @@
       <c r="J42" s="1" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="21" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -14742,12 +15565,15 @@
       <c r="J43" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="20" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D44" s="3"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -14772,8 +15598,11 @@
       <c r="J45" s="1" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="1" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -14798,8 +15627,11 @@
       <c r="J46" s="1" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -14824,8 +15656,11 @@
       <c r="J47" s="1" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -14850,8 +15685,11 @@
       <c r="J48" s="1" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -14876,8 +15714,11 @@
       <c r="J49" s="1" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -14902,8 +15743,11 @@
       <c r="J50" s="1" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -14928,8 +15772,11 @@
       <c r="J51" s="1" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -14954,8 +15801,11 @@
       <c r="J52" s="1" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -14980,8 +15830,11 @@
       <c r="J53" s="1" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K53" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -15006,8 +15859,11 @@
       <c r="J54" s="1" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -15032,8 +15888,11 @@
       <c r="J55" s="1" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -15058,8 +15917,11 @@
       <c r="J56" s="1" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -15084,8 +15946,11 @@
       <c r="J57" s="1" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -15110,8 +15975,11 @@
       <c r="J58" s="1" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -15136,8 +16004,11 @@
       <c r="J59" s="1" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -15162,8 +16033,11 @@
       <c r="J60" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -15188,8 +16062,11 @@
       <c r="J61" s="1" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="1" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -15214,8 +16091,11 @@
       <c r="J62" s="1" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>47</v>
       </c>
@@ -15240,8 +16120,11 @@
       <c r="J63" s="1" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -15266,8 +16149,11 @@
       <c r="J64" s="1" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -15292,8 +16178,11 @@
       <c r="J65" s="1" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -15318,8 +16207,11 @@
       <c r="J66" s="1" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -15344,8 +16236,11 @@
       <c r="J67" s="1" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="1" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -15370,8 +16265,11 @@
       <c r="J68" s="1" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -15396,8 +16294,11 @@
       <c r="J69" s="1" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -15422,8 +16323,11 @@
       <c r="J70" s="1" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -15448,8 +16352,11 @@
       <c r="J71" s="1" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -15474,8 +16381,11 @@
       <c r="J72" s="1" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -15500,8 +16410,11 @@
       <c r="J73" s="1" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>47</v>
       </c>
@@ -15526,8 +16439,11 @@
       <c r="J74" s="1" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -15552,8 +16468,11 @@
       <c r="J75" s="1" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -15578,8 +16497,11 @@
       <c r="J76" s="1" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>47</v>
       </c>
@@ -15604,8 +16526,11 @@
       <c r="J77" s="1" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77" s="1" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>47</v>
       </c>
@@ -15630,8 +16555,11 @@
       <c r="J78" s="1" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -15656,8 +16584,11 @@
       <c r="J79" s="1" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -15682,8 +16613,11 @@
       <c r="J80" s="1" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80" s="1" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -15708,8 +16642,11 @@
       <c r="J81" s="1" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="1" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>47</v>
       </c>
@@ -15734,8 +16671,11 @@
       <c r="J82" s="1" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -15760,8 +16700,11 @@
       <c r="J83" s="1" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -15786,8 +16729,11 @@
       <c r="J84" s="1" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84" s="1" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -15812,8 +16758,11 @@
       <c r="J85" s="1" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85" s="1" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>47</v>
       </c>
@@ -15838,8 +16787,11 @@
       <c r="J86" s="1" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86" s="1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>47</v>
       </c>
@@ -15864,8 +16816,11 @@
       <c r="J87" s="1" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87" s="1" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>47</v>
       </c>
@@ -15890,8 +16845,11 @@
       <c r="J88" s="1" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88" s="1" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -15916,8 +16874,11 @@
       <c r="J89" s="1" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -15942,8 +16903,11 @@
       <c r="J90" s="1" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -15968,8 +16932,11 @@
       <c r="J91" s="1" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91" s="1" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>47</v>
       </c>
@@ -15994,8 +16961,11 @@
       <c r="J92" s="1" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>47</v>
       </c>
@@ -16020,8 +16990,11 @@
       <c r="J93" s="1" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93" s="1" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>47</v>
       </c>
@@ -16046,8 +17019,11 @@
       <c r="J94" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94" s="1" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -16072,8 +17048,11 @@
       <c r="J95" s="1" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95" s="1" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -16098,8 +17077,11 @@
       <c r="J96" s="1" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96" s="1" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -16124,8 +17106,11 @@
       <c r="J97" s="1" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97" s="1" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -16150,8 +17135,11 @@
       <c r="J98" s="1" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -16176,8 +17164,11 @@
       <c r="J99" s="1" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99" s="1" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -16202,8 +17193,11 @@
       <c r="J100" s="1" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100" s="1" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>47</v>
       </c>
@@ -16228,8 +17222,11 @@
       <c r="J101" s="1" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101" s="1" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>47</v>
       </c>
@@ -16254,8 +17251,11 @@
       <c r="J102" s="1" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102" s="1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -16280,8 +17280,11 @@
       <c r="J103" s="1" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>47</v>
       </c>
@@ -16306,8 +17309,11 @@
       <c r="J104" s="1" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -16332,8 +17338,11 @@
       <c r="J105" s="1" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105" s="1" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -16358,8 +17367,11 @@
       <c r="J106" s="1" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -16384,8 +17396,11 @@
       <c r="J107" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>47</v>
       </c>
@@ -16410,8 +17425,11 @@
       <c r="J108" s="1" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>47</v>
       </c>
@@ -16436,12 +17454,15 @@
       <c r="J109" s="1" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D110" s="3"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>53</v>
       </c>
@@ -16466,20 +17487,25 @@
       <c r="J111" s="1" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K111" s="21" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E112" s="13"/>
       <c r="H112" s="14"/>
       <c r="I112" s="16"/>
       <c r="J112" s="14"/>
-    </row>
-    <row r="113" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K112" s="21"/>
+    </row>
+    <row r="113" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E113" s="13"/>
       <c r="H113" s="14"/>
       <c r="I113" s="16"/>
       <c r="J113" s="14"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K113" s="21"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -16507,8 +17533,11 @@
       <c r="J114" s="1" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K114" s="21" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -16536,8 +17565,11 @@
       <c r="J115" s="1" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K115" s="21" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -16565,8 +17597,11 @@
       <c r="J116" s="1" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K116" s="21" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -16594,8 +17629,11 @@
       <c r="J117" s="1" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K117" s="21" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -16623,8 +17661,11 @@
       <c r="J118" s="1" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K118" s="21" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -16652,8 +17693,11 @@
       <c r="J119" s="1" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K119" s="21" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -16681,8 +17725,11 @@
       <c r="J120" s="1" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K120" s="21" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -16710,12 +17757,15 @@
       <c r="J121" s="1" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K121" s="21" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D122" s="4"/>
       <c r="I122" s="8"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -16743,8 +17793,11 @@
       <c r="J123" s="1" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K123" s="21" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -16772,8 +17825,11 @@
       <c r="J124" s="1" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K124" s="21" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -16801,8 +17857,11 @@
       <c r="J125" s="1" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K125" s="21" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -16830,8 +17889,11 @@
       <c r="J126" s="1" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K126" s="21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -16859,8 +17921,11 @@
       <c r="J127" s="1" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K127" s="21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -16888,8 +17953,11 @@
       <c r="J128" s="1" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128" s="21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -16917,8 +17985,11 @@
       <c r="J129" s="1" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129" s="21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -16946,12 +18017,15 @@
       <c r="J130" s="1" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130" s="21" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D131" s="4"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -16979,8 +18053,11 @@
       <c r="J132" s="1" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132" s="21" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -17008,8 +18085,11 @@
       <c r="J133" s="1" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133" s="21" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -17037,8 +18117,11 @@
       <c r="J134" s="1" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134" s="21" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -17066,8 +18149,11 @@
       <c r="J135" s="1" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135" s="21" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -17095,8 +18181,11 @@
       <c r="J136" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136" s="21" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -17124,8 +18213,11 @@
       <c r="J137" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137" s="21" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -17153,8 +18245,11 @@
       <c r="J138" s="1" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138" s="21" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -17182,8 +18277,11 @@
       <c r="J139" s="1" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139" s="21" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -17211,8 +18309,11 @@
       <c r="J140" s="1" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140" s="21" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -17240,8 +18341,11 @@
       <c r="J141" s="1" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K141" s="21" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -17269,8 +18373,11 @@
       <c r="J142" s="1" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K142" s="21" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -17298,8 +18405,11 @@
       <c r="J143" s="1" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K143" s="21" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -17327,8 +18437,11 @@
       <c r="J144" s="1" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K144" s="21" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -17356,8 +18469,11 @@
       <c r="J145" s="1" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K145" s="21" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -17385,12 +18501,15 @@
       <c r="J146" s="1" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K146" s="21" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
       <c r="I147" s="8"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -17418,8 +18537,11 @@
       <c r="J148" s="1" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K148" s="21" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -17447,8 +18569,11 @@
       <c r="J149" s="1" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K149" s="21" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -17476,8 +18601,11 @@
       <c r="J150" s="1" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K150" s="21" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -17505,8 +18633,11 @@
       <c r="J151" s="1" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K151" s="21" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -17534,12 +18665,15 @@
       <c r="J152" s="1" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K152" s="21" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D153" s="4"/>
       <c r="I153" s="8"/>
     </row>
-    <row r="154" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
         <v>7</v>
       </c>
@@ -17564,12 +18698,15 @@
       <c r="J154" s="1" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K154" s="21" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D155" s="4"/>
       <c r="I155" s="8"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -17597,12 +18734,15 @@
       <c r="J156" s="17" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K156" s="20" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D157" s="4"/>
       <c r="I157" s="8"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>47</v>
       </c>
@@ -17627,8 +18767,11 @@
       <c r="J158" s="1" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K158" s="20" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>47</v>
       </c>
@@ -17653,8 +18796,11 @@
       <c r="J159" s="1" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K159" s="20" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>47</v>
       </c>
@@ -17679,12 +18825,15 @@
       <c r="J160" s="1" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K160" s="20" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D161" s="4"/>
       <c r="I161" s="8"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>47</v>
       </c>
@@ -17712,8 +18861,11 @@
       <c r="J162" s="1" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K162" s="1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -17741,8 +18893,11 @@
       <c r="J163" s="1" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K163" s="1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -17770,8 +18925,11 @@
       <c r="J164" s="1" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K164" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>47</v>
       </c>
@@ -17799,8 +18957,11 @@
       <c r="J165" s="1" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K165" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -17828,8 +18989,11 @@
       <c r="J166" s="1" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K166" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>47</v>
       </c>
@@ -17857,8 +19021,11 @@
       <c r="J167" s="1" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K167" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>47</v>
       </c>
@@ -17886,8 +19053,11 @@
       <c r="J168" s="1" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K168" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>47</v>
       </c>
@@ -17915,8 +19085,11 @@
       <c r="J169" s="1" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K169" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -17944,8 +19117,11 @@
       <c r="J170" s="1" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K170" s="1" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>47</v>
       </c>
@@ -17973,8 +19149,11 @@
       <c r="J171" s="1" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K171" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>47</v>
       </c>
@@ -18002,8 +19181,11 @@
       <c r="J172" s="1" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K172" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>47</v>
       </c>
@@ -18031,8 +19213,11 @@
       <c r="J173" s="1" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K173" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -18060,8 +19245,11 @@
       <c r="J174" s="1" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K174" s="1" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -18089,8 +19277,11 @@
       <c r="J175" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K175" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>47</v>
       </c>
@@ -18118,12 +19309,15 @@
       <c r="J176" s="1" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K176" s="1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D177" s="4"/>
       <c r="I177" s="8"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>53</v>
       </c>
@@ -18148,20 +19342,25 @@
       <c r="J178" s="1" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K178" s="21" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E179" s="13"/>
       <c r="H179" s="14"/>
       <c r="I179" s="16"/>
       <c r="J179" s="14"/>
-    </row>
-    <row r="180" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K179" s="21"/>
+    </row>
+    <row r="180" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E180" s="13"/>
       <c r="H180" s="14"/>
       <c r="I180" s="16"/>
       <c r="J180" s="14"/>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K180" s="21"/>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -18189,8 +19388,11 @@
       <c r="J181" s="18" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K181" s="18" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -18218,8 +19420,11 @@
       <c r="J182" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K182" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -18247,8 +19452,11 @@
       <c r="J183" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K183" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -18276,8 +19484,11 @@
       <c r="J184" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K184" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -18305,8 +19516,11 @@
       <c r="J185" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K185" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -18334,8 +19548,11 @@
       <c r="J186" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K186" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -18363,8 +19580,11 @@
       <c r="J187" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K187" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -18392,8 +19612,11 @@
       <c r="J188" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K188" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -18421,8 +19644,11 @@
       <c r="J189" s="18" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K189" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C190" s="8"/>
       <c r="D190" s="15"/>
       <c r="E190"/>
@@ -18431,7 +19657,7 @@
       <c r="I190" s="8"/>
       <c r="J190" s="18"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -18459,8 +19685,11 @@
       <c r="J191" s="1" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K191" s="1" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -18488,8 +19717,11 @@
       <c r="J192" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K192" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -18517,8 +19749,11 @@
       <c r="J193" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K193" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -18546,8 +19781,11 @@
       <c r="J194" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K194" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -18575,8 +19813,11 @@
       <c r="J195" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K195" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -18604,8 +19845,11 @@
       <c r="J196" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K196" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -18633,8 +19877,11 @@
       <c r="J197" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K197" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -18662,8 +19909,11 @@
       <c r="J198" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K198" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -18691,14 +19941,17 @@
       <c r="J199" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K199" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C200" s="8"/>
       <c r="D200" s="15"/>
       <c r="E200"/>
       <c r="I200" s="8"/>
     </row>
-    <row r="201" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A201" s="8" t="s">
         <v>7</v>
       </c>
@@ -18723,14 +19976,17 @@
       <c r="J201" s="1" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K201" s="21" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="D202" s="5"/>
       <c r="I202" s="8"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -18758,12 +20014,15 @@
       <c r="J203" s="1" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K203" s="20" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D204" s="5"/>
       <c r="I204" s="8"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>47</v>
       </c>
@@ -18788,8 +20047,11 @@
       <c r="J205" s="1" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K205" s="20" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>47</v>
       </c>
@@ -18814,8 +20076,11 @@
       <c r="J206" s="1" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K206" s="20" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>47</v>
       </c>
@@ -18840,8 +20105,11 @@
       <c r="J207" s="1" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K207" s="21" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>47</v>
       </c>
@@ -18866,12 +20134,15 @@
       <c r="J208" s="1" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K208" s="21" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D209" s="5"/>
       <c r="I209" s="8"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>53</v>
       </c>
@@ -18896,8 +20167,11 @@
       <c r="J210" s="1" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K210" s="21" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>53</v>
       </c>
@@ -18922,8 +20196,11 @@
       <c r="J211" s="1" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K211" s="21" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>53</v>
       </c>
@@ -18948,8 +20225,11 @@
       <c r="J212" s="1" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K212" s="21" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>53</v>
       </c>
@@ -18974,8 +20254,11 @@
       <c r="J213" s="1" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K213" s="21" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>53</v>
       </c>
@@ -19000,8 +20283,11 @@
       <c r="J214" s="1" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K214" s="20" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>53</v>
       </c>
@@ -19026,8 +20312,11 @@
       <c r="J215" s="1" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K215" s="20" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>53</v>
       </c>
@@ -19052,8 +20341,11 @@
       <c r="J216" s="1" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K216" s="21" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>53</v>
       </c>
@@ -19078,8 +20370,11 @@
       <c r="J217" s="1" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K217" s="21" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>53</v>
       </c>
@@ -19104,8 +20399,11 @@
       <c r="J218" s="1" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K218" s="21" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>53</v>
       </c>
@@ -19130,20 +20428,25 @@
       <c r="J219" s="1" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K219" s="20" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E220" s="13"/>
       <c r="H220" s="14"/>
       <c r="I220" s="16"/>
       <c r="J220" s="14"/>
-    </row>
-    <row r="221" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K220" s="21"/>
+    </row>
+    <row r="221" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E221" s="13"/>
       <c r="H221" s="14"/>
       <c r="I221" s="16"/>
       <c r="J221" s="14"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K221" s="21"/>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -19171,8 +20474,11 @@
       <c r="J222" s="1" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K222" s="20" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -19200,8 +20506,11 @@
       <c r="J223" s="1" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K223" s="21" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -19229,8 +20538,11 @@
       <c r="J224" s="1" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K224" s="21" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -19258,8 +20570,11 @@
       <c r="J225" s="1" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K225" s="20" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -19287,12 +20602,15 @@
       <c r="J226" s="1" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K226" s="20" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D227" s="6"/>
       <c r="I227" s="8"/>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>7</v>
       </c>
@@ -19320,8 +20638,11 @@
       <c r="J228" s="1" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K228" s="20" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>7</v>
       </c>
@@ -19349,8 +20670,11 @@
       <c r="J229" s="1" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K229" s="21" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>7</v>
       </c>
@@ -19378,8 +20702,11 @@
       <c r="J230" s="1" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K230" s="20" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>7</v>
       </c>
@@ -19407,12 +20734,15 @@
       <c r="J231" s="1" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K231" s="20" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D232" s="6"/>
       <c r="I232" s="8"/>
     </row>
-    <row r="233" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A233" s="8" t="s">
         <v>7</v>
       </c>
@@ -19437,12 +20767,15 @@
       <c r="J233" s="1" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K233" s="21" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D234" s="6"/>
       <c r="I234" s="8"/>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>7</v>
       </c>
@@ -19467,12 +20800,15 @@
       <c r="J235" s="19" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K235" s="21" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D236" s="6"/>
       <c r="I236" s="8"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>47</v>
       </c>
@@ -19494,8 +20830,11 @@
       <c r="J237" s="1" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K237" s="21" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>47</v>
       </c>
@@ -19517,8 +20856,11 @@
       <c r="J238" s="1" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K238" s="21" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>47</v>
       </c>
@@ -19540,12 +20882,15 @@
       <c r="J239" s="1" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K239" s="21" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D240" s="6"/>
       <c r="I240" s="8"/>
     </row>
-    <row r="241" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>47</v>
       </c>
@@ -19567,12 +20912,15 @@
       <c r="J241" s="1" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K241" s="21" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D242" s="6"/>
       <c r="I242" s="8"/>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>53</v>
       </c>
@@ -19594,20 +20942,25 @@
       <c r="J243" s="1" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="244" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K243" s="21" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E244" s="13"/>
       <c r="H244" s="14"/>
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
-    </row>
-    <row r="245" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K244" s="14"/>
+    </row>
+    <row r="245" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E245" s="13"/>
       <c r="H245" s="14"/>
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K245" s="14"/>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>7</v>
       </c>
@@ -19635,11 +20988,15 @@
       <c r="J246" s="1" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K246" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D247" s="7"/>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K247" s="1"/>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>7</v>
       </c>
@@ -19667,8 +21024,11 @@
       <c r="J248" s="1" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K248" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>7</v>
       </c>
@@ -19696,8 +21056,11 @@
       <c r="J249" s="1" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K249" s="1" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>7</v>
       </c>
@@ -19725,8 +21088,11 @@
       <c r="J250" s="1" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K250" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>7</v>
       </c>
@@ -19754,11 +21120,15 @@
       <c r="J251" s="1" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K251" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D252" s="7"/>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K252" s="1"/>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>7</v>
       </c>
@@ -19786,11 +21156,15 @@
       <c r="J253" s="1" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K253" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D254" s="7"/>
-    </row>
-    <row r="255" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K254" s="1"/>
+    </row>
+    <row r="255" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>47</v>
       </c>
@@ -19815,8 +21189,11 @@
       <c r="J255" s="1" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="256" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K255" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>47</v>
       </c>
@@ -19841,8 +21218,11 @@
       <c r="J256" s="1" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="257" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K256" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>47</v>
       </c>
@@ -19867,8 +21247,11 @@
       <c r="J257" s="1" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="258" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K257" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>47</v>
       </c>
@@ -19893,11 +21276,15 @@
       <c r="J258" s="1" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K258" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D259" s="7"/>
-    </row>
-    <row r="260" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K259" s="1"/>
+    </row>
+    <row r="260" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>53</v>
       </c>
@@ -19922,20 +21309,25 @@
       <c r="J260" s="1" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K260" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E261" s="13"/>
       <c r="H261" s="14"/>
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
-    </row>
-    <row r="262" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K261" s="14"/>
+    </row>
+    <row r="262" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E262" s="13"/>
       <c r="H262" s="14"/>
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
-    </row>
-    <row r="263" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K262" s="14"/>
+    </row>
+    <row r="263" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>7</v>
       </c>
@@ -19960,11 +21352,14 @@
       <c r="J263" s="1" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K263" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D264" s="9"/>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>7</v>
       </c>
@@ -19989,11 +21384,15 @@
       <c r="J265" s="1" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K265" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D266" s="9"/>
-    </row>
-    <row r="267" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K266" s="1"/>
+    </row>
+    <row r="267" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A267" s="8" t="s">
         <v>7</v>
       </c>
@@ -20018,13 +21417,17 @@
       <c r="J267" s="1" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K267" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="D268" s="9"/>
-    </row>
-    <row r="269" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K268" s="1"/>
+    </row>
+    <row r="269" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>7</v>
       </c>
@@ -20049,11 +21452,15 @@
       <c r="J269" s="1" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K269" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D270" s="9"/>
-    </row>
-    <row r="271" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K270" s="1"/>
+    </row>
+    <row r="271" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>47</v>
       </c>
@@ -20075,8 +21482,11 @@
       <c r="J271" s="1" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="272" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K271" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>47</v>
       </c>
@@ -20098,8 +21508,11 @@
       <c r="J272" s="1" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="273" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K272" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>47</v>
       </c>
@@ -20121,8 +21534,11 @@
       <c r="J273" s="1" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="274" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K273" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>47</v>
       </c>
@@ -20144,11 +21560,15 @@
       <c r="J274" s="1" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K274" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D275" s="9"/>
-    </row>
-    <row r="276" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K275" s="1"/>
+    </row>
+    <row r="276" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>53</v>
       </c>
@@ -20170,20 +21590,25 @@
       <c r="J276" s="1" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="277" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K276" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E277" s="13"/>
       <c r="H277" s="14"/>
       <c r="I277" s="14"/>
       <c r="J277" s="14"/>
-    </row>
-    <row r="278" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K277" s="14"/>
+    </row>
+    <row r="278" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E278" s="13"/>
       <c r="H278" s="14"/>
       <c r="I278" s="14"/>
       <c r="J278" s="14"/>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K278" s="14"/>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>7</v>
       </c>
@@ -20208,11 +21633,15 @@
       <c r="J279" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K279" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D280" s="10"/>
-    </row>
-    <row r="281" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K280" s="1"/>
+    </row>
+    <row r="281" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>7</v>
       </c>
@@ -20237,11 +21666,15 @@
       <c r="J281" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K281" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D282" s="10"/>
-    </row>
-    <row r="283" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K282" s="1"/>
+    </row>
+    <row r="283" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>7</v>
       </c>
@@ -20266,11 +21699,15 @@
       <c r="J283" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K283" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D284" s="10"/>
-    </row>
-    <row r="285" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K284" s="1"/>
+    </row>
+    <row r="285" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>7</v>
       </c>
@@ -20295,11 +21732,15 @@
       <c r="J285" s="1" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K285" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D286" s="10"/>
-    </row>
-    <row r="287" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K286" s="1"/>
+    </row>
+    <row r="287" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>47</v>
       </c>
@@ -20321,8 +21762,11 @@
       <c r="J287" s="1" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="288" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K287" s="1" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>47</v>
       </c>
@@ -20344,8 +21788,11 @@
       <c r="J288" s="1" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="289" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K288" s="1" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>47</v>
       </c>
@@ -20367,8 +21814,11 @@
       <c r="J289" s="1" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="290" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K289" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>47</v>
       </c>
@@ -20390,11 +21840,15 @@
       <c r="J290" s="1" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K290" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D291" s="10"/>
-    </row>
-    <row r="292" spans="1:10" ht="19" x14ac:dyDescent="0.3">
+      <c r="K291" s="1"/>
+    </row>
+    <row r="292" spans="1:11" ht="19" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>53</v>
       </c>
@@ -20415,6 +21869,9 @@
       </c>
       <c r="J292" s="1" t="s">
         <v>791</v>
+      </c>
+      <c r="K292" s="1" t="s">
+        <v>1008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Somali snuggets (NOT FULLY TESTED)
There’s an issue with the Somali support in my localhost install, so I
can confirm that the snugget loader runs on this, but I haven’t been
able to view the results.
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets.xlsx
+++ b/disasterinfosite/data/snuggets.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1225">
   <si>
     <t>section</t>
   </si>
@@ -12502,6 +12502,714 @@
   </si>
   <si>
     <t>text-ru</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD SAREYSO&lt;/b&gt; (84%) ee baaxada 6.5+ dhulgariir qotodheer oo dhufanayo 50 sanno ee xigo. Waxay dareemeysaa si lamid ah M6.8 ee Dhulgariirka Nisqually ee 2001. Gariirka dhaxedhaxaadka waxaa dareemaya ku dhawaad qof walboo halkaan joogo. &lt;b&gt;Albaabada wuu lulmayaa&amp;#44; sawirada darbiyada way shanqarayaan&amp;#44; iyo sheeyada yaryar way dhici karaan. Waxyeelada way yaraaneysaa.&lt;/b&gt;  &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD SAREYSO&lt;/b&gt; (84%) ee baaxada 6.5+ dhulgariir qotodheer oo dhufanayo 50 sanno ee xigo. Waxay dareemeysaa si lamid ah M6.8 ee Dhulgariirka Nisqually ee 2001. &lt;b&gt;Gariir xoogan wuu ku adkeynayaa inuu halkaan ku lugeeyo. Buuggaagta&amp;#44; galaasyada&amp;#44; iyo sheeyada way ka dhacayaan iska faalooyinka. Albaabada armaajada iyo qaanadaha way furmayaan&lt;/b&gt;. Qaar ka mid ah shooladaha iyo si liito ugu dhisan dhismooyinka way waxyeeloobayaan. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD SAREYSO&lt;/b&gt; (84%) ee baaxada 6.5+ dhulgariir qotodheer oo dhufanayo 50 sanno ee xigo. Waxay dareemeysaa si lamid ah M6.8 ee Dhulgariirka Nisqually ee 2001. &lt;b&gt;Gariir aad u xoogan ayaa ku adkeynayo in halkaan la taagnaado. Alaabta guriga way dhaqaaqeysaa iyo sheeyo badan waxay ka soo dhacayaan iska faalooyinka.&lt;/b&gt; Waxyeelada muhiim ah oo si liidato ugu dhisan qaabdhismeedyada oo wax yar dhexdhaxaadinayo qaabdhismeedyo caadi ah. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;FURSAD HOOSE&lt;/b&gt; (5%) ee ka jirto baaxada 7+ dhulgariirka Qaladka Seattle ee 50 sanno ee xiggo&amp;#44; laakin haddii ay sameyso waxyeelo ayay noqoneysaa. &lt;b&gt;Gariirka dhaxedhaxaadka waxaa dareemaya ku dhawaad qof walboo joogo. Albaabada wuu lulmayaa&amp;#44; sawirada darbiyada way shanqarayaan&amp;#44; iyo sheeyada yaryar way dhici karaan. Waxyeelada way yaraaneysaa.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;FURSAD HOOSE&lt;/b&gt; (5%) ee ka jirto baaxada 7+ dhulgariirka Qaladka Seattle ee 50 sanno ee xiggo&amp;#44; laakin haddii ay sameyso waxyeelo ayay noqoneysaa. Gariir xoogan wuu ku adkeynayaa inuu ku lugeeyo. &lt;b&gt;Buuggaagta&amp;#44; galaasyada&amp;#44; iyo sheeyada way ka dhacayaan iska faalooyinka. Qaar ka mid ah shooladaha iyo si liito ugu dhisan dhismooyinka way waxyeeloobayaan.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;FURSAD HOOSE&lt;/b&gt; (5%) ee ka jirto baaxada 7+ dhulgariirka Qaladka Seattle ee 50 sanno ee xiggo&amp;#44; laakin haddii ay sameyso waxyeelo ayay noqoneysaa. &lt;b&gt;Gariir aad u xoogan ayaa adkeyneyso in la taagnaado. Alaabta guriga way dhaqaaqeysaa iyo sheeyo ayaa dhacayo&lt;/b&gt;. Waxyeelada waxay muhiim u noqoneysaa dhismooyinka sida liidato loo dhisay iyo dhexdhaxaadka dhismooyinka caadiga ah. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(qariirada) &lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;FURSAD HOOSE&lt;/b&gt; (5%) ee ka jirto baaxada 7+ dhulgariirka Qaladka Seattle ee 50 sanno ee xiggo&amp;#44; laakin haddii ay sameyso waxyeelo ayay noqoneysaa. &lt;b&gt;Gariir daran ayaa ku adkeynayo in la taagnaado ama la kaxeeyo. Alaabaha guriga culus waa la afgambinayaa. Qeybaha dhismooyinka &lt;a href="http://www.seattle.gov/dpd/codesrules/changestocode/unreinforcedmasonrybuildings/whatwhy/" target=_blank&gt;URM&lt;/a&gt; wuu burburayaa iyo guryaha naqshada alwaaxa waxay isku badelayaan aasaasyada&lt;/b&gt;. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;FURSAD HOOSE&lt;/b&gt; (5%) ee ka jirto baaxada 7+ dhulgariirka Qaladka Seattle ee 50 sanno ee xiggo&amp;#44; laakin haddii ay sameyso waxyeelo ayay noqoneysaa. &lt;b&gt;Gariirka xiigan wuxuu ku sababayaa faafida naxdinta iyo dilaacyada dhulka way aasaasmeysaa. Dhulka buuraha waxaa lagu kicinayaa dalcadaha dagaandaga iyo godka waxay ka dhaceysaa ciidaha qoyan.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD DHEXDHAXAAD&lt;/b&gt; (10-30%) ee baaxada 8+ dhulgariirka Cascadia oo dhufanayo Wuqooyiga galbeed ee 50 sanno ee xiggo. &lt;b&gt;Marka ay dhacdo&amp;#44; waxaad dareemeysaa gariir dhexdhaxaad ah ee ku adkeysto daqiiqado halkaan. Sheeyada aan badbaadada aheyn way ka dhacayaan iska faalooyinka. Albaabada armaajada way lulmayaan oo furmayaan oo xirmayaan&lt;/b&gt;. Awooda iyo biyaha way dan sanaan karaan maalmo illaa isbuucyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD DHEXDHAXAAD&lt;b&gt; (10-30%) ee baaxada 8+ dhulgariirka Cascadia oo dhufanayo Wuqooyiga galbeed ee 50 sanno ee xiggo. &lt;b&gt;Marka ay dhacdo&amp;#44; waxaad dareemeysaa gariir xoogan ah halhaan ee ku adkeysto daqiiqado. Way adkaaneysaa in la socdo. Dhismooyinka Bulkeetiga oo Culu way waxyeeloobayaan iyo dadka way dhaawacmayaan &lt;/b&gt;. Awooda iyo biyaha way damayaan maalmo illaa isbuucyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Waxaa jiro &lt;b&gt;FURSAD DHEXDHAXAAD&lt;/b&gt; (10-30%) ee baaxada 8+ dhulgariirka Cascadia oo dhufanayo Wuqooyiga galbeed ee 50 sanno ee xiggo. &lt;b&gt;Marka ay dhacdo&amp;#44; waxaad dareemeysaa gariir aad u xoogan ee ku adkeysto daqiiqado halkaan. Taagnaashada way adkaaneysaa iyo wax badan ayaa dhaawacmayo. Bulkeetiyada iyo galaasyada burbursan waxay aftiiminayaan wadooyinka&lt;/b&gt;. Awooda iyo biyaha way damayaan maalmo illaa isbuucyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Waxaad joogtaa &lt;b&gt;aaga tusanaamiga halista SEREYSO&lt;/b&gt;. Heerarka biyaha waxay ka sara kacayaan madaxaaga daqiiqado illaa tobannaadyo daqiiqado ee xigo dhulgariirka. Markii gariirka joogsado KA GUUR ISLA MARKIIBA dhul sareeyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Waxaad joogtaa &lt;b&gt;aaga tusanaamiga halista SEREYSO&lt;/b&gt;. Heerarka biyaha waxay ku gaarayaan inta u dhaxeyso jilbahaaga iyo madaxaaga daqiiqa illaa tobanaadyo daqiiqad ee xiggaa dhul gariirka. Markii gariirka joogsado KA GUUR ISLA MARKIIBA dhul sareeyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Waxaad joogtaa &lt;b&gt;aaga tusanaamiga halista SEREYSO&lt;/b&gt;. Heerarka biyaha waxay gaarayaan illaa ilbahaaga ee degdega hadeer ee ku filan inuu kugu dhufto. Waxaad haysataa daqiiqado illaa toban daqiiqado ee looga GUURAYO dhulal sareeyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Waxaad banaanka ka jirtaa aaga tusunaamiga halista ah ee la calaameeyay&lt;/b&gt;&amp;#44; laakin hirarka tusanaamiga way isbedeli kartaa. Miyaad ku nooqshahay ama ka shaqeysaa aaga buur hoose (ee gudaha 30fiit ee heerka biyaha) u dhow badda? Haddii ay sidaas tahay&amp;#44; KA GUUR ISLA MARKIIBA dhul sareeyo kadib dhul weyn. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Waxaad ku jirtaa gudaha rubac mayl ee badda&lt;/b&gt;. Haddii joogtid meel buur hoose (within 30fiit ee heerka badda) waxaad halis ugu jiri kartaa tusanaami ee xigga dhul gariirka u dhow. Raadi dhul sareeyo isla markiiba. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Haddii aad doon saarantahay inta lagu jiro dhul gariirka waxaad la kulmi kartaa hirarka dhaqaaqa tusunaamiga oo xoogan oo kugu soo socdo. T illaa iyada. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(qariirada)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: SAREEYO&lt;/b&gt;&lt;br&gt;Ciida rokmeyso waxay noqoneysaa mid aan aad u xasilooneyn oo waxay u dhaqmeysaa sida ciid degdega ah. Biyaha ciida ka buuxo kor ayaa soo aadi kartaa oo dhinaca dilaacyada wadooyinka. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: DHEXDHAXAAD - SAREEYO&lt;/b&gt;&lt;br&gt;Ciida gariirmeyso waxay noqoneysaa mid aan xasilooneyn. Tani waxay yareyneysaa kartida ciida looga baxayo ee guryahaa haysto&amp;#44; baabuurta&amp;#44; iyo qaabdhismeedyada kale. Biyaha ciida ka buuxo kor ayaa soo aadi kartaa oo dhinaca dilaacyada wadooyinka. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: HOOSEEYO - DHEXDHAXAAD&lt;/b&gt;&lt;br&gt;Jiritaano qaarkood oo imaan karo ee godka halkaan. Gariirinta waxay ku sababi kartaa ciida inay xasiloon wayso. Wadooyinka way dilaaci karaan oo waxyeeloobi karaan.&lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: HOOSEEYO&lt;/b&gt;&lt;br&gt;Illaa gariirka uu xooganyahay uusan u nasiib laheyn waxaad ku arkeysaa godka halkaan. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: AAD U HOOSEEYO - HOOSEEYO&lt;/b&gt;&lt;br&gt;Illaa gariirka aad u xooganyahay&amp;#44; waa nasiib daro inaad ku arkeysid god halkaan. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: AAD U HOOSEEYO&lt;/b&gt;&lt;br&gt;Illaa gariirka aad u xooganyahay&amp;#44; waa nasiib daro inaad ku arkeysid god halkaan. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: MA JIRAAN&lt;/b&gt;&lt;br&gt;Aagaan waa dhagax adag&amp;#44; dhagax adaga ee hoos yaalo ciida iyo biyaha. Ma biyo noqoneyso. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: MA JIRAAN&lt;/b&gt;&lt;br&gt;Aagaan waa caro madow&amp;#44; arinta dabiiciga ah ee ka kooban waxyaabaha ciida madow. Way isku laabmi kartaa laakin ma biyo noqoneyso. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Imaan karo: MA JIRAAN&lt;/b&gt;&lt;br&gt;Aagaan waxaa laga sameeyay baraf iyo ma biyo noqoneyso. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MUGGA AAD U HOOSEEYO: 0 illaa 10 dhismooyinka bulkeetiga (URM) dhismayaasha wareega maylkiiba.&lt;/b&gt;&lt;br&gt;Dhismaha noocaan ah&amp;#44; dhul gariir xoogan ayaa ku sababayo darbiyada bulkeetiga ama saqafyada inay dhacaan. Haraaga wuxuu wasaqeynayaa wadooyinka. Fiiri halka URM uu &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;kuu dhowyahay&lt;/a&gt; iyo haddii horay loogu daray. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MUGGA HOOSEEYO: 10 illaa 25 dhismooyinka bulkeetiga (URM) dhismayaasha wareega maylkiiba.&lt;/b&gt;&lt;br&gt;Dhismaha noocaan ah&amp;#44; dhul gariir xoogan ayaa ku sababayo darbiyada bulkeetiga ama saqafyada inay dhacaan. Haraaga wuxuu wasaqeynayaa wadooyinka. Fiiri halka URM uu &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;kuu dhowyahay&lt;/a&gt; iyo haddii horay loogu daray. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MUGGA DHEXDHAXAADKA: 25 illaa 50 dhismooyinka bulkeetiga (URM) dhismayaasha wareega maylkiiba.&lt;/b&gt;&lt;br&gt;Dhismaha noocaan ah&amp;#44; dhul gariir xoogan ayaa ku sababayo darbiyada bulkeetiga ama saqafyada inay dhacaan. Haraaga wuxuu wasaqeynayaa wadooyinka. Fiiri halka URM uu &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;kuu dhowyahay&lt;/a&gt; iyo haddii horay loogu daray. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MUGGA SAREEYO: 50 illaa 100 dhismooyinka bulkeetiga (URM) dhismayaasha wareega maylkiiba.&lt;/b&gt;&lt;br&gt;Haddii aad joogtid URM inta lagu jiro Istuurka dhulgariirka&amp;#44; Isdabool&amp;#44; iyo Qabso. Dhismooyinkaan&amp;#44; dhul gariir xoogan ayaa ku sababayo darbiyada bulkeetiga iyo saqafyada inay dhacaan. Haraaga wuxuu wasaqeynayaa wadooyinka. Fiiri halka URM uu &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;kuu dhowyahay&lt;/a&gt; iyo haddii horay loogu daray. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MUGGA AAD U SAREEYO: 100 illaa 250 dhismooyinka bulkeetiga (URM) dhismayaasha wareega maylkiiba.&lt;/b&gt;&lt;br&gt;Haddii aad joogtid URM inta lagu jiro Istuurka dhulgariirka&amp;#44; Isdabool&amp;#44; iyo Qabso. Dhismooyinkaan&amp;#44; dhul gariir xoogan ayaa ku sababayo darbiyada bulkeetiga iyo saqafyada inay dhacaan. Haraaga wuxuu wasaqeynayaa wadooyinka. Fiiri halka URM uu &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;kuu dhowyahay&lt;/a&gt; iyo haddii horay loogu daray. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Saynisyahanka ma qiyaasi karo goorta dhulgariir dhacayo marka ka taxadar iyo haddii aad dareentid gariir&amp;#44; istuur dabool&amp;#44; oo qabso. Nidaamka digniinta hore hadeer waxaa loo hormariyay Xeebta Galbeedka. Waxaad ka heli kartaa waxbadan &lt;a href=http://earthquake.usgs.gov/research/earlywarning/ target="_blank"&gt;halkaan&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;DHAQANKA&lt;/b&gt; - Ka taxadar oo ku dhaqan "Is tuur&amp;#44; Isdabool&amp;#44; oo Qabso"&lt;/li&gt;&lt;li&gt;&lt;b&gt;QORSHEY&lt;/b&gt; - Samey qorshaha qoyska (&lt;a href=http://www.fema.gov/media-library-data/0e3ef555f66e22ab832e284f826c2e9e/FEMA_plan_parent_508_071513.pdf target="_blank"&gt;wixii qof weyn ah&lt;/a&gt; &amp;amp; &lt;a href=http://www.fema.gov/media-library-data/a260e5fb242216dc62ae380946806677/FEMA_plan_child_508_071513.pdf target="_blank"&gt;wixii carruur ah&lt;/a&gt;) oo dhis &lt;a href=http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf target="_blank"&gt;sanduuqa saadka&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;U DIYAARGAROW&lt;/b&gt; - hubi sheeyada dhici karo oo ogow goobta korontada ka dantay.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;GUDAHA - HALKAAN JOOG!&lt;/b&gt; Isku dabool hoosta miiska ama miiska ka baxsan sheeyada kugu soo dhici karo oo qabso. HA KU ordin banaanka ka hor inta uusan gariirka joogsan.&lt;/li&gt;&lt;li&gt;&lt;b&gt;BANAANKA - GAL MEEL BANAAN&lt;/b&gt; ee ka baxsan dhismooyinka&amp;#44; fiilooyinka korontada&amp;#44; munaaradaha&amp;#44; ama waxyaabaha kugu soo dhici karo adiga.&lt;/li&gt;&lt;li&gt;&lt;b&gt;GAARI KAXEYNTA - SI TAXADAR AH U JOOGSO&lt;/b&gt; (ma ahan buundo hoosteeda&amp;#44; buundooyinka la hoos maro&amp;#44; fiilooyinka korontada&amp;#44; iwm.) iyo JOOG GUDAHA GAARIGA.&lt;/li&gt;&lt;li&gt;&lt;b&gt;U DHOW XEEBTA&lt;/b&gt; - Raac tilmaamaha kore illaa gariirka ka joogsado. Kadib &lt;b&gt;MADAXA OO DHUL SAREEYO&lt;/b&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/EQ_during.jpg" alt="This is a panel of four cartoon images showing what to do during an earthquake if inside&amp;#44; outside&amp;#44; driving&amp;#44; or near the ocean." title="During Earthquake Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;U DIYAAR GAROW NADXINTA KADIB&lt;/b&gt; (dhulgariirka ee xigga naxdinta ugu weyn waa caadi ee ku sababi kartaa waxyeelo ka badan gariirka hore).&lt;ul&gt;&lt;li&gt;Qadadka taleefonka way buux dhaafayaan; &lt;b&gt;fariin qoraalka waxay noqon kartaa wado wanaagsan ee lagula xiriiro qoyska.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;Ka hubi nafsadaada iyo dadka kale dhaawacyo.&lt;/li&gt;&lt;li&gt;Markii aad badbaado tahay&amp;#44; &lt;b&gt;fiir wargelinada aqbaaraha&lt;/b&gt; oo dhinaca raadiyaha batariga ku shaqeeyo&amp;#44; telefishanada&amp;#44; warbaahinta bulshada&amp;#44; iyo digniinada qoraalka mobeelka oo warbixinta gurmadka.&lt;/li&gt;&lt;li&gt;Shaqaalaha gurmadka way mashquulayaan. &lt;b&gt;Waxay ku xirantahay saaxibadaada iyo dariska&lt;/b&gt; oo taageerada inta lagu jiro saacadaha iyo maalmaha xigo dhulgariirka.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Xakameynta korontada haddii ay muhiim tahay&lt;/b&gt;. Wax badan ka ogow goorta iyo sida &lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target="_blank"&gt;loo xakameeyo gaaska iyo biyaha dhulgariirka kadib&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;Daawo &lt;a href=https://www.fema.gov/media-library/assets/videos/98767 target="_blank"&gt;fiidiyahaan&lt;/a&gt; si aad wax badan uga ogaatid waxa la sameynayo &lt;b&gt;INTA LAGU JIRO&lt;/b&gt; iyo &lt;b&gt;KADIB&lt;/b&gt; dhulgariirka.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Morgan Junction Park Hub &lt;br&gt;Goobta Xarunta: At Morgan Junction Park&amp;#44; &lt;br&gt;6413 California Ave SW&amp;#44; Seattle&amp;#44; WA 98118 &lt;br&gt;Xarunta Hub: Cindi Barker&lt;br&gt;I-meelka: &lt;a href="mailto:cindiLbarker@gmail.com" target="_top"&gt;cindiLbarker@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-933-6968&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/west-seattle/" target=_blank&gt;http://seattleemergencyhubs.org/west-seattle&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;North Highland Park Hub &lt;br&gt;Goobta Xarunta: The Highland Park Improvement Club &lt;br&gt;1116 SW Holden St&lt;br&gt;Xarunta Hub:Volunteer Needed &lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;South Park Neighborhood Center &lt;br&gt;Goobta Xarunta: 8201 10th Ave S&lt;br&gt;Xarunta Hub: Dagmar Cronn&lt;br&gt;I-meelka: &lt;a href="mailto:cronn@oakland.edu" target="_top"&gt;cronn@oakland.edu&lt;/a&gt;&lt;br&gt;Taleefonka: 206-327-1828&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt; &lt;br&gt;description: Meet by the blue box in the park&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Pigeon Point Hub &lt;br&gt;Goobta Xarunta: The intersection of 20th Ave SW &amp; SW Genesee St&amp;#44; Seattle&amp;#44; WA 98106 &lt;br&gt;NW corner of the Park&amp;#44; just north of the school.&lt;br&gt;Xarunta Hub: Wade Harper&lt;br&gt;I-meelka: &lt;a href="mailto:wade.harper@outlook.com" target="_top"&gt;wade.harper@outlook.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-455-5407&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Hiawatha Playfield/Community Center (Admiral Hub) &lt;br&gt;Goobta Xarunta: At California Ave SW &amp; SW Lander St&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Xarunta Hub: Paul Stancik&lt;br&gt;I-meelka: &lt;a href="mailto:pstancik@mindspring.com" target="_top"&gt;pstancik@mindspring.com&lt;/a&gt;&lt;br&gt;Taleefonka:TBD &lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Fauntleroy Church Hub &lt;br&gt;Goobta Xarunta: Fauntleroy Church&amp;#44; 9140 California Ave SW&lt;br&gt;Xarunta Hub: Gordon Wiehler&lt;br&gt;I-meelka:: &lt;a href="mailto:gmwinv@Comcast.net" target="_top"&gt;gmwinv@Comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka:: 206-577-4292&lt;br&gt;Websaydka:&lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Providence/Mount St. Vincent&amp;#44; parking lot (Fairmount Hub) &lt;br&gt;Goobta Xarunta: At SW Hudson St &amp; 35th Ave SW&amp;#44; Seattle&amp;#44; WA 98126 &lt;br&gt; (meet at the SE parking lot under the flag pole )&lt;br&gt;Xarunta Hub: Sharonn Meeks&lt;br&gt;I-meelka: &lt;a href="mailto:smeeks50@comcast.net" target="_top"&gt;smeeks50@comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka: 206-938-1007&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Neighborhood House (High Point Hub) &lt;br&gt;Goobta Xarunta: At 6400 Sylvan Way SW (note that east of 35th Ave SW&amp;#44; SW Morgan Street becomes Sylvan Way SW). Neighborhood House is next to Lanham Place SW. Meet at the amphitheater. &lt;br&gt;Xarunta Hub: Heather Hutchison&lt;br&gt;I-meelka: &lt;a href="mailto:heather.hutchison@manage" target="_top"&gt;heather.hutchison@manage&lt;/a&gt;&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Ercolini Park Hub &lt;br&gt;Goobta Xarunta: At 48th Ave SW &amp; SW Alaska St.&amp;#44; in the park&lt;br&gt;Xarunta Hub: Jon Wright&lt;br&gt;I-meelka:&lt;a href="mailto:ercolini@westseattlebeprepared.org" target="_top"&gt;ercolini@westseattlebeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;EC Hughes Playground (Olympic Heights Hub) &lt;br&gt;Goobta Xarunta: At 29th Ave SW &amp; SW Holden St&amp;#44; Seattle&amp;#44; WA 98126&amp;#44; at the NE corner of Hughes Playground.&lt;br&gt;Xarunta Hub: Volunteer needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Salvation Army&amp;#44; parking lot (South Highland Park Hub) &lt;br&gt;Goobta Xarunta: At 9050 16th Ave SW (near SW Barton St.)&amp;#44; the Salvation Army parking lot is the gathering place for this hub.&lt;br&gt;Xarunta Hub: Volunteer Needed &lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;North Delridge P-Patch Hub &lt;br&gt;Goobta Xarunta: At the P-Patch&amp;#44; located at 5078 25th Ave SW&amp;#44; Seattle&amp;#44; WA&lt;br&gt;Xarunta Hub: Jay McNally&lt;br&gt;I-meelka: &lt;a href="mailto:Newcarissa@gmail.com" target="_top"&gt;Newcarissa@gmail.com &lt;/a&gt;&lt;br&gt;Taleefonka: 206-484-6613&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Hope Lutheran Church (Alaska Junction Hub) &lt;br&gt;Goobta Xarunta: 4456 42nd Ave SW&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Alki Community Center (Alki Hub) &lt;br&gt;Goobta Xarunta: At 59th Ave SW &amp; SW Stevens St&amp;#44; Seattle&amp;#44; WA 98116. This is adjacent to Whale Tail Park&amp;#44; near the west edge of the playfield. North side of Alki Playfield&lt;br&gt;Xarunta Hub: Tony Fragada (98126)&lt;br&gt;I-meelka: &lt;a href="mailto:tfragada@yahoo.com" target="_top"&gt;tfragada@yahoo.com&lt;/a&gt; &lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Maa Nyei Lai Ndeic P-Patch Hub &lt;br&gt;Goobta Xarunta: 4913 Columbia Dr S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Xarunta Hub: Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Hillman City P-Patch Hub &lt;br&gt;Goobta Xarunta: 4613 S Lucile St&amp;#44; Seattle&amp;#44; WA 98118 (Corner of South Lucile &amp; 46th Ave South)&lt;br&gt;Xarunta Hub: Joanne Tilton&lt;br&gt;I-meelka: &lt;a href="mailto:Jtilton22@comcast.net" target="_top"&gt;Jtilton22@comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka: 206-650-2071&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Judkins P-Patch Hub &lt;br&gt;Goobta Xarunta: 24th Avenue S &amp; S Norman Street Seattle&amp;#44; WA 98112 (Meeting Location: P-Patch entrance off Norman &amp; 24th Ave S.)&lt;br&gt;Xarunta Hub: Jen Ellis&lt;br&gt;I-meelka:   &lt;a href="mailto:JenniferEllis.206@gmail.com" target="_top"&gt;JenniferEllis.206@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-276-4982&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Fisher Pavilion Hub &lt;br&gt;Goobta Xarunta: 2nd Ave N &amp; Thomas St&lt;br&gt;Xarunta Hub: MIQA Be Prepared&lt;br&gt;I-meelka:  &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka:  &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Interbay Fishermen's Terminal Hub &lt;br&gt;Goobta Xarunta: Interbay Fishermen's Terminal&lt;br&gt;Xarunta Hub: MIQA Be Prepared&lt;br&gt;I-meelka: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Eastlake Hub &lt;br&gt;Goobta Xarunta: Rogers Playfield&lt;br&gt;Xarunta Hub: Amy O'Donnell&lt;br&gt;I-meelka:  &lt;a href="mailto:eastlake.hub@gmail.com" target="_top"&gt;eastlake.hub@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Madison Park Hub &lt;br&gt;Goobta Xarunta: 42nd Ave E and E Howe St (at the north side of tennis courts)&lt;br&gt;Xarunta Hub: John Madrid&lt;br&gt;I-meelka:  &lt;a href="mailto:johnmadrid@hotmail.com" target="_top"&gt;johnmadrid@hotmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-498-1880&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Sunrise P-Patch Hub &lt;br&gt;Goobta Xarunta: 33rd Ave S &amp; S Oregon St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Aaron Deitz&lt;br&gt;I-meelka: &lt;a href="mailto:aarondietz@gmail.com" target="_top"&gt;aarondietz@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-694-3966&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Snoqualmie P-Patch Hub &lt;br&gt;Goobta Xarunta: 4549 13th Ave S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Xarunta Hub: Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;New Holly Youth &amp; Family P-Patch Hub &lt;br&gt;Goobta Xarunta: 32nd Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;New Holly Power P-Patch Hub &lt;br&gt;Goobta Xarunta: 7123 S Holly Park Dr&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;New Holly Lucky Garden Hub &lt;br&gt;Goobta Xarunta: S Holly St &amp; Shaffer Ave S&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;New Holly 29 P-Patch Hub &lt;br&gt;Goobta Xarunta: 29th Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;John C. Little P-Patch Hub &lt;br&gt;Goobta Xarunta: 6961 37th Ave S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Dakota P-Patch Hub &lt;br&gt;Goobta Xarunta: 2902 S Dakota St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Beacon Food Forest Hub &lt;br&gt; Goobta Xarunta:: 15th Ave S &amp; S Dakota St&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Ethiopian Community in Seattle &lt;br&gt;Goobta Xarunta: 8323 Rainier Ave S (meet at main building)&lt;br&gt;Xarunta Hub: Kassa Kachara&lt;br&gt;I-meelka:  &lt;a href="mailto:kabiso_kass@yahoo.com" target="_top"&gt;kabiso_kass@yahoo.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-325-0304&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Angel Morgan P-Patch (Angel Morgan Hub) &lt;br&gt;Goobta Xarunta: 3956 S Morgan St&amp;#44; Seattle&amp;#44; WA 98118 (The P Patch is located at 42nd Ave S &amp; S Morgan Street)&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Thistle P-Patch Hub &lt;br&gt;Goobta Xarunta: Martin Luther King Jr Way S &amp; S Cloverdale St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;New Holly Rockery &amp; Market Hub &lt;br&gt;Goobta Xarunta: S Holly Park Dr &amp; Rockery Dr S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Xarunta Hub: Contact Debbie Goetz&lt;br&gt;I-meelka: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Taleefonka: 206-684-0517&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Lakewood Seward Park Hub &lt;br&gt;Goobta Xarunta: Lakewood Seward Park Community Club - 4916 S. Angeline Street&lt;br&gt;Xarunta Hub: Aaron Evanson&lt;br&gt;I-meelka:  &lt;a href="mailto:aaronevanson@gmail.com" target="_top"&gt;aaronevanson@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206.660.3822&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Rainier Beach Community Club Hub &lt;br&gt;Goobta Xarunta: Rainier Beach Community Club - VFW Hall &amp;#44; 6038 S. Pilgrim&amp;#44; Seattle  WA  98118&lt;br&gt;Xarunta Hub: Ron Angeles&lt;br&gt;I-meelka:  &lt;a href="mailto:ranestoba@comcast.net" target="_top"&gt;ranestoba@comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka: 206-721-5326 and 206-351-0813&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Queen Anne Bowl &lt;br&gt;Goobta Xarunta: 2806 3rd Ave W&lt;br&gt;Xarunta Hub: Chris Saether&lt;br&gt;I-meelka: &lt;a href="mailto:csaether@msn.com" target="_top"&gt;csaether@msn.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Interbay Athletic Complex &lt;br&gt;Goobta Xarunta: 3027 17th Ave W&lt;br&gt;Xarunta Hub: MIQA Be Prepared&lt;br&gt;I-meelka: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Magnolia Manor Park &lt;br&gt; Goobta Xarunta: 3500 28th Ave W&lt;br&gt;Xarunta Hub: MIQA Be Prepared&lt;br&gt;I-meelka: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Magnolia Metropolitan Market&lt;br&gt;Goobta Xarunta: 3830 34th Ave W&lt;br&gt;Xarunta Hub: MIQA Be Prepared&lt;br&gt;I-meelka: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;West Queen Anne Playfield Hub &lt;br&gt;Goobta Xarunta: 150 W Blaine St&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD &lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;West Magnolia Playfield Hub &lt;br&gt;Goobta Xarunta: 32nd Ave W &amp; W Smith St&amp;#44; South Playfield&amp;#44; Southwest corner&lt;br&gt;Xarunta Hub: Frank Gaul&lt;br&gt;I-meelka:  &lt;a href="mailto:ftgaul@gmail.com" target="_top"&gt;ftgaul@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-499-8690&lt;br&gt;Websaydka: &lt;a href="http://www.miqabeprepared.org/" target=_blank&gt;http://www.miqabeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Ballard Commons Hub &lt;br&gt;Goobta Xarunta: NW 57th &amp; 22nd Ave NW&lt;br&gt;Xarunta Hub: Colin Getty&lt;br&gt;I-meelka:  &lt;a href="mailto:k7biowa@gmail.com" target="_top"&gt;k7biowa@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Lower Woodland Playfields Hub &lt;br&gt;Goobta Xarunta: Green Lake Way N &amp; N 50th St&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Ravenna Hub &lt;br&gt; Goobta Xarunta: 6535 Ravenna Ave NE (Ravenna-Eckstein Community Center parking lot)&lt;br&gt;Xarunta Hub: David Ward&lt;br&gt;I-meelka:  &lt;a href="mailto:booksgalore22@gmail.com" target="_top"&gt;booksgalore22@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-523-1161&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Victory Heights Hub &lt;br&gt;Goobta Xarunta: Victory Heights Park (1737 NE 106th St)&lt;br&gt;Xarunta Hub: Ann Forrest&lt;br&gt;I-meelka:  &lt;a href="mailto:aaforrest@hotmail.com" target="_top"&gt;aaforrest@hotmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: (360)550-2234&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Epic Life Church Hub &lt;br&gt;Goobta Xarunta: Epic Life Church - 10503 Stone Ave N&amp;#44; Seattle&amp;#44; WA 98133&lt;br&gt;Xarunta Hub: Larry Chaney&lt;br&gt;I-meelka:  &lt;a href="mailto:larry@epiclifechurch.org" target="_top"&gt;larry@epiclifechurch.org&lt;/a&gt;&lt;br&gt;Taleefonka: 425-218-8849&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Crown Hill Park Hub &lt;br&gt;Goobta Xarunta: NW 92nd &amp; 14th Ave NW&lt;br&gt;Xarunta Hub: Dennis Galvin&lt;br&gt;I-meelka:  &lt;a href="mailto:short.harp@gmail.com" target="_top"&gt;short.harp@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Shilshole Marina Hub &lt;br&gt;Goobta Xarunta: Shilshole Marina&amp;#44; 7001 Seaview Ave NW&lt;br&gt;Xarunta Hub: Jim Doub&lt;br&gt;I-meelka: &lt;a href="mailto:jim@portagebaymarine.com" target="_top"&gt;jim@portagebaymarine.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Loyal Heights Playfield Hub&lt;br&gt;Goobta Xarunta: NW 77th &amp;amp; 21st Ave NW (2101 NW 77th St&amp;#44; Loyal Heights CC basketball half court)&lt;br&gt;Xarunta Hub: Cheryl Dyer&lt;br&gt;I-meelka: &lt;a href="mailto:cheryldy@msn.com" target="_top"&gt;cheryldy@msn.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-784-3724&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Kirke Park Hub&lt;br&gt;Goobta Xarunta: 7028 9th Ave NW&lt;br&gt;Xarunta Hub: Hugh Kelso&lt;br&gt;I-meelka: &lt;a href="mailto:HKelso@mac.com" target="_top"&gt;HKelso@mac.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Gilman Park Hub &lt;br&gt;Goobta Xarunta: NW 54th &amp;amp; 9th Ave NW&lt;br&gt;Xarunta Hub: Linda Frank&lt;br&gt;I-meelka: &lt;a href="mailto:lindabfrank@gmail.com" target="_top"&gt;lindabfrank@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Ross Playground Hub &lt;br&gt;Goobta Xarunta: 4320 4th Ave NW&lt;br&gt;Xarunta Hub: Leslie Matthis&lt;br&gt;I-meelka: &lt;a href="mailto:leslie.matthis@gmail.comv" target="_top"&gt;leslie.matthis@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206.783.1500&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Phinney Neighborhood Center Hub &lt;br&gt;Goobta Xarunta: Phinney Neighborhood Center: 6532 Phinney Avenue North&amp;#44; Seattle&amp;#44; WA  98103 (Meeting Place: Phinney Center upper parking area)&lt;br&gt;Xarunta Hub: David Baum&lt;br&gt;I-meelka: &lt;a href="mailto:phinneyhub@gmail.com" target="_top"&gt;phinneyhub@gmail.com &lt;/a&gt;&lt;br&gt;Taleefonka: 206-913-1021&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Meridian Playfield/Good Shepherd Center Hub &lt;br&gt;Goobta Xarunta: 4649 Sunnyside Ave. N&lt;br&gt;Xarunta Hub: Brian Shapiro&lt;br&gt;I-meelka: &lt;a href="mailto:bshapiro@objectarts.net" target="_top"&gt;bshapiro@objectarts.net&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;History House of Greater Seattle Hub &lt;br&gt;Goobta Xarunta: 790 N 34th St&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Greenwood Senior Center Hub &lt;br&gt;Goobta Xarunta: Greenwood Senior Center: 525 N 85th  Street&amp;#44; Seattle&amp;#44; WA  98103&lt;br&gt;Xarunta Hub: Kelly Kasper&lt;br&gt;I-meelka: &lt;a href="mailto:kelly@ht2consulting.com" target="_top"&gt;kelly@ht2consulting.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-397-4283&lt;br&gt;Co-Captain: Noel Frame&lt;br&gt;Co-Captain I-meelka: &lt;a href="mailto:noel@noelframe.com" target="_top"&gt;noel@noelframe.com&lt;/a&gt; &lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Green Lake Playfield &amp; Community Center Hub &lt;br&gt;Goobta Xarunta: 7201 Green Lake Dr N&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Bagley Elementary Hub &lt;br&gt;Goobta Xarunta: 7821 Stone Ave N&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Taleefonka: TBD&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Maple Leaf Park Hub &lt;br&gt;Goobta Xarunta: 1020 NE 82nd St&lt;br&gt;Xarunta Hub: Lori Phipps&lt;br&gt;I-meelka: &lt;a href="mailto:lphipps01@gmail.com" target="_top"&gt;lphipps01@gmail.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-947-0309&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Hunter Farm Hub &lt;br&gt;Goobta Xarunta: 7730 35th Ave NE&lt;br&gt;Xarunta Hub: Volunteer Needed&lt;br&gt;I-meelka: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Websaydka:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;University Heights Center &lt;br&gt;Goobta Xarunta: NE 50th Street and University Way NE&lt;br&gt;Xarunta Hub: Ray Munger&lt;br&gt;I-meelka: &lt;a href="mailto:ray@uheightscenter.org" target="_top"&gt;ray@uheightscenter.org&lt;/a&gt;&lt;br&gt;Taleefonka: 206-527-4278&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Lake City Way SR 522/Fred Meyer Hub &lt;br&gt;Goobta Xarunta: 13000 Lake City Way NE (SE corner of lower parking lot)&lt;br&gt;Xarunta Hub: Sandy Motzer (98125)&lt;br&gt;I-meelka: &lt;a href="mailto:sandymotzer@aol.com" target="_top"&gt;sandymotzer@aol.com&lt;/a&gt;&lt;br&gt;Taleefonka: 206-819-8056&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Luther Memorial Lutheran Church Hub &lt;br&gt;Goobta Xarunta: 13047 Greenwood Ave N&lt;br&gt;Xarunta Hub: Dale Johnson&lt;br&gt;I-meelka: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka: 206-362-2980&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Xarumaha Gurmadka Bulshada waa meelaha dariska ay isugu imaan karaan masiibada kadib si ay usu caawiyaan. &lt;p&gt;XARUNTA ADIGA KUU DHOW WAA&amp;#44;&lt;center&gt;&lt;b&gt;Grace Lutheran Church Hub &lt;br&gt; Goobta Xarunta: 11051 Phinney Ave N (Greenwood Avenue N &amp; N 112th Street)&lt;br&gt;Xarunta Hub: Dale Johnson&lt;br&gt;I-meelka: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Taleefonka: 206-362-2980&lt;br&gt;Websaydka: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tan iyo 1870&amp;#44; 15 dhulgariir weyn (oo ka weyn baaxada 5) ayaa ku dhuftay Gobolka Washington. Sheekooyinka asalka sidoo kale way sheegtaa dhulgariir weyn (oo ka weyn baaxada 8) iyo tusanaamiga ee xigay 1700. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/historical_EQs2.jpg" alt="This is an Image showing the sizes of historical earthquakes in Washington. It shows a magnitude(M) 6.5 in 1949 which is 316 times smaller than M9&amp;#44; M6.9 in 2001 which is 160 times smaller than M9&amp;#44; M7.1 in 1965 which is 79 times smaller than M9&amp;#44; and M9 in 1700." title="Relative sizes of notable earthquakes in Washington State"&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Waxaa jiro fursad sareyso ee fatahaada halkaan. Waxay fadhidaa xanuunka fatahaada 100-sanno&lt;/b&gt;. Tani wxaay la micna tahay waxaa jiro 25% oo fursada biyaha fatahaada ee halkaan soo gaarayo 30-ka sanno ee xigga &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Fatahaada waa nasiib daro halkaan&lt;/b&gt;. Heerarka biyaha wax yar ayay kor ukici karaan inta lagu jiro fatahaada ama duufaanta xoogan. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Fatahaada waa nasiib daro halkaan&lt;/b&gt;. Heerarka biya daga wax yar ayay kor ukici karaan inta lagu jiro fatahaada ama duufaanta xoogan. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Fatahaada waa nasiib daro halkaan&lt;/b&gt;. Heerarka biyaha wax yar ayay kor ukici karaan inta lagu jiro fatahaada ama duufaanta xoogan.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Buundooyinka waxay noqon karaan kuwa aan badbaado aheyn marka fatahaada dhaceyso&lt;/b&gt;. Haddii aad ka shakisid in buundo waxyeelowday&amp;#44; ka walaacsanow oo ku soo wargeli Xarunta Digniinta Fatahaada adiga oo soo wacayo 206-296-8200 ama 800-945-9263. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Tamni waxay banaanka ka tahay aagaga fatahaada halista sareyso&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. LAAKIN haddii aad ku nooshahay meel u dhow ama wabi yar ka taxadar inay fatahaad noqon karto sidoo kale. Fiiri &lt;a href=http://www.kingcounty.gov/depts/dnrp/wlr/sections-programs/river-floodplain-section.aspx target=_blank&gt;Websaydka Wabiga iyo Maamulida Fatahaada cad&lt;/a&gt; wixii warbixin dheeraad ah.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Aagaan waxay soo fatahday xiliga la soo dhaafay markii duufaan weyn uu dhuftay Seattle&lt;/b&gt;. Markale ayay dhici kartaa haddii duufaan kale oo xoogan ku sababto in biyaha u buuxsamaan oo u qalalaan si liidato. Hoos u soco oo sida la isu diyaariyo. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Roobka&amp;#44; barafka dhalaalo&amp;#44; ama labadaba waxay ku sababaan in biyaha kor waxyar u kacaan. Biyaha fatahaada waxay buux dhaafiyaan geesaska wabiga&amp;#44; ku daataan dariska&amp;#44; oo saameeyaan wadooyinka. &lt;b&gt;Aagaan waxay ku jirtaa 500-sanno fatahaada ee qariiradeysan oo way fataheysaa&lt;/b&gt;. Waxaa jiro fursada boqolkiiba 6% waxaad arkeysaa fatahaada cabirkaan ah ee 30-ka sanno ee xiggo. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;U dhow biyo dageenada&amp;#44; durdurada&amp;#44; iyo wabiyada way fatahayaan. Tani waxay ka dhigtaa wadooyinka qaarkood inaan lamari karin &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Waa nasiib daro inaad ku arkeysid fatahaad halkaan&lt;/b&gt;. Duufaanta weyn waxay ku sababi kartaa meel u dhow biyo dageenada&amp;#44; durdurada&amp;#44; iyo wabiyada inay sare u kacaan. Dhacitaanka roob culus ayaa abuuri karo barkadaha biyaha taagan ee wadooyinka. Haddii aad la kulantid fatahaada deegaamowday ka soo wac Xarunta Digniinta Gobolka King 206-296-8200 ama 800-945-9263. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Aagaan way unugushahay fatahaada magaalada&lt;/b&gt;. Sida weyn ee duufaanta fatahaada badan ee ku arki kartid dhinacaan. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad sareyso ee Wabiga Cedar ee marayo dhinacaan mustaqbalka&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad sareyso ee Wabiga Green ee marayo dhinacaan mustaqbalka&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad sareyso ee Wabiga Raging ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad sareyso ee Wabiga Snoqualmie ee marayo dhinacaan mustaqbalka&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad sareyso ee Wabiga Tolt ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad dhexaad ah ee Wabiga Cedar ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad dhexaad ah ee Wabiga Green ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad dhaxaad ah ee Wabiga Raging ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad dhexaad ah ee Wabiga Snoqualmie ee marayo dhinacaan mustaqbalka&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad dhaxaad ah ee Wabiga Tolt ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad hooseyso ee Wabiga Green ee marayo dhinacaan mustaqbalka. &lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad hooseyso ee Wabiga Snoqualmie ee marayo dhinacaan mustaqbalka&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. Waxay badelmaan inta badan inta lagu jiro iyo fahatahaada kadib. &lt;b&gt;Aagaan wuxuu leeyahay fursad hooseyso ee Wabiga Tolt ee marayo dhinacaan mustaqbalka. &lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sida waxyaabaha ugu badan&amp;#44; wabiyada waxay maraan wadada diidmada iyo isbadelada waqti kadib. &lt;b&gt;Ma jirto daraasad halkaan lagu sameeyay si loo arko haddii wabiga u dhowyahay inuu dhaqaaqo waqti kadib&amp;#44; laakin ogow inay noqon karto.&lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tani waa gudaha kanaalka wabiga hadeer. Waqti kadib goobta kanaalka wuu isbadeli karaa. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Howlgabka Biyo xireenka waa dhif. Si kastaba&amp;#44; haddii &lt;a href=https://goo.gl/maps/X2HGtZX6Kyz target=_blank&gt;Biyo xireenka George Culmback&lt;/a&gt; ama &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;Biyo xireenka Wabiga Tolt&lt;/a&gt; howlgabo aagaan way fatahi kartaa &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.</t>
+  </si>
+  <si>
+    <t>Howlgabka Biyo xireenka waa dhif. Si kastaba&amp;#44; haddii &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Biyo xireenka Haraha Youngs&lt;/a&gt; howlgabo aagaan waxay halis ugu jirtaa fatahaad &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.</t>
+  </si>
+  <si>
+    <t>Howlgabka Biyo xireenka waa dhif. Si kastaba&amp;#44; haddii &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Biyo xireenka Haraha Youngs&lt;/a&gt; howlgabo aagaan waxay halis ugu jirtaa fatahaad dhexdhaxaad ah &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.</t>
+  </si>
+  <si>
+    <t>Howlgabka Biyo xireenka waa dhif. Si kastaba&amp;#44; haddii &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Biyo xireenka Haraha Youngs&lt;/a&gt; howlgabo aagaan waxay halis ugu jirtaa sareyso ugu jirtaa fatahaad &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.</t>
+  </si>
+  <si>
+    <t>Howlgabka Biyo xireenka waa dhif. Si kastaba&amp;#44; haddii &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;Biyo xireenka Wabiga Tolt&lt;/a&gt; aagaan way fatahi kartaa &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(qariirada)&lt;/a&gt;. Iska diiwaangeli digniinada fatahaada oo &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;i-meel ama fariin ahaan&lt;/a&gt; ama dajiso &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;app-ka digniika fatahaada&lt;/a&gt; ee mobeelada casriga ah.</t>
+  </si>
+  <si>
+    <t>Duufaanada daran waxaa laga filanayo inay kordhiso 50-ka sanno ee xigga. Waxay u keeneysaa roob iyo baraf. Wabiyada waxay yeelanayaan qulqul sareeyo ee u jaheynayo fatahaad badan ee Deyrta/Qaboobaha. Riix sawirka lagu ogaanayo wax badan.&lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Rivers.jpg" alt="Climate Change Rivers Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Miyuu roob adag da’ayay ama maalmo badan? Leeyahay heer kulul kacayo oo sababay baraf dhallaalka lama filaanka ah ee buuraha? Samey heerarka biyaha ee wabiyada deegaanka ee sare u muuqdo? Fursadaha fatahaada way kordhi kartaa. Fiiri wargelinada aqbaarta oo adeegyada cimilada ee digniinada deegaanka.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;QORSHEY&lt;/b&gt; - Samey qorshaha waxa la sameynayo iyo halka la aadayo haddii ay biyaha soo koraan. &lt;b&gt;La how sheeyo muhiim ah oo diyaar ah&lt;/b&gt; (shahaadooyinka dhalashada&amp;#44; waraaqaha muhiimka ah&amp;#44; sawirada&amp;#44; iwm). Hel caymiska fatahaada haddii aad u baahantahay.&lt;/li&gt;&lt;li&gt;&lt;b&gt;U DIYAARGAROW&lt;/b&gt; - Ku keydso sheeyada qiimaha leh iyo kiimikooyinka qoyska meel ka koreyso heerarka fatahaada iyo &lt;b&gt;baro sida loo damiyo korontooyinka&lt;/b&gt; (&lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target=_blank&gt;biyaha&amp;#44; gaaska&amp;#44; iyo korontada&lt;/a&gt;).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;DIYAAR GAROW&lt;/b&gt; - Isu keen sheeyada degdega ah (dharka diiran&amp;#44; toosh&amp;#44; mobeel&amp;#44; raadiyow la qaadi karo&amp;#44; iwm). Haddii waqtiga ogolaado oo wuxuu u muuqdaa muhiim&amp;#44; dami korontooyinka.&lt;/li&gt;&lt;li&gt;&lt;b&gt;DHAGEYSO&lt;/b&gt; - Dhageyso aqbaaraha iyo haddii laguugula taliyo&amp;#44; u guur dhul sareeyo.&lt;/li&gt;&lt;li&gt;&lt;b&gt;KA FOGOW HALISAHA - HA ku lugeynin ama haku kaxeynin dhinaca biyaha fatahaada.&lt;/b&gt; Waxay qaadataa kaliya 6 injis oo dhaqaaqa biyaha ee adiga kugu dhufunayo iyo 2 fiit oo gaariga loogu xaaqayo!&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Flood_during.jpg" alt="This is a panel of four cartoon images showing what to do during an a flood collect essentials&amp;#44; get to high ground&amp;#44; avoid water&amp;#44; and shutt off utilities." title="During Flood Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Haddii gurigaaga fatahay&amp;#44; &lt;b&gt;ka walaacsanow dib u gelida sida ay lahaan karto waxyeelo qaabeysan.&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Lahow korontooyinka eegida xirfadlaha&lt;/b&gt; ka hor inta aadan iska geddin.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Lumitaanada waraaqaha&lt;/b&gt; ee sawirida waxyeelooyinka iyo qarashaadka suubinta duubitaanka.&lt;/li&gt;&lt;li&gt;Ka ogow wax badan &lt;a href=http://www.kingcounty.gov/services/environment/water-and-land/flooding/prepare.aspx target=_blank&gt;halkaan&lt;/a&gt;&lt;/b&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Russell Road Park &lt;br&gt; btwn Russell Rd. iyo S. 240th St.&lt;br&gt; Kent&amp;#44; WA&amp;#44; 98032 &lt;br&gt;  Ciida qaado kaliya (ma lahan jawaanka ciida)&lt;br&gt; Isniinta-Jimcaha 8:00 am - 4:00 pm &lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&amp;#44;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt;Public Works Shops &lt;br&gt;1155 East North Bend Way &lt;br&gt; North Bend&amp;#44; WA 98045&lt;br&gt; Jawaanka ciida iyo ciida qaado&lt;br&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; 33100 NE 45th Street &lt;br&gt; Carnation&amp;#44; WA 98014 &lt;br&gt;Isniinta-Jimcaha 8:00am - 4:30pm &lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Meadowbrook Community Center&lt;br&gt;10517 35th Ave. NE &lt;br&gt; Seattle&amp;#44; WA 98125&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; 1305 C St. SW &lt;br&gt; Auburn&amp;#44; WA 98001&lt;br&gt; Isniinta-Jimcaha 6:30am - 4:00pm&lt;br&gt;Jawaanka ciida iyo ciida qaado --&gt;253-931-3048&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Kent City Public Works&lt;br&gt; 5821 S. 240th St. &lt;br&gt; Kent&amp;#44; WA 98032&lt;br&gt; Isniinta-Jimcaha 8:00am - 4:00pm &lt;br&gt;Jawaanka ciida qaado kaliya (ma lahan ciida)&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Tahoma School District &lt;br&gt; 23015 SE 216th Way&lt;br&gt; Maple Valley&amp;#44; WA 98038&lt;br&gt; 8:00am - 5:00pm&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Pacific City Park &lt;br&gt; 600 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047&lt;br&gt;Sandbag iyo Sand pickup will be announced when White River flooding is imminent&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Pacific/Algona Community Center &lt;br&gt; 100 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047 &lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; City Property @ &lt;br&gt; Railroad Avenue SE iyo SE King Street &lt;br&gt; Snoqualmie&amp;#44; WA 98065&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Preston-Snoqualmie Trail parking lot &lt;br&gt; Lake Alice Road SE iyo SE 56th Place &lt;br&gt; Fall City&amp;#44; WA 98024&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; 14701 Main St. NE &lt;br&gt; Duvall&amp;#44; WA 98019&lt;br&gt;Jawaanka ciida iyo ciida qaado--&gt;425-788-3332&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Haller Lake Neighborhood &lt;br&gt; 12551 Ashworth Ave N.&lt;br&gt; Seattle&amp;#44; WA 98133&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; South Park Neighborhood &lt;br&gt; 731 S. Sullivan &lt;br&gt; Seattle&amp;#44; WA 98108&lt;br&gt;Jawaanka ciida iyo ciida qaado&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>U diyaar garow fatahaada adiga oo qaadayo oo buuxinayo jawaanada ciida. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;p&gt;QEYBIN XARUNTA KUU DHOW ADIGA WAA&amp;#44; &lt;center&gt;&lt;b&gt; Delridge Community Center &lt;br&gt; 4501 Delridge Way SW &lt;br&gt; Seattle&amp;#44; WA 98106&lt;br&gt;Jawaanka ciida iyo ciida qaado &lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Oo leh wabiyaal badan ee fatahaada Gobolka King waa caadi inta lagu jiro muddooyinka dhacitaanada roobka culus ama baraf dhallaalka degdega ah. &lt;b&gt;Fatahaada way ugu caadisantahay ka bilow Nofeembarta illaa Febraayo&lt;/b&gt;&amp;#44; laakin waxay dhici kartaa marwalba oo xaaladaha ay saxanyihiin.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Aagaan waxay leedahay giirada godka oo waxay si yar ugu dhowdsahay inay yeelato dhulalka buurta ah halkaan&lt;/b&gt;. Dhulalka buuraha u muuqdaan inay ka dhacaan markii dhulka uu ka qoyanyahay qeybaha roobka AMA dhulka gariirka sababo. Hoos uga soco dhacdooyinka taariiqiga ah fiiri haddii wax dhulalka buurta ah lagu qoray aagaaga. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Sabab la xiriirto dalcadaha dagaandaga&amp;#44; aagaan waxay leedahay fursad dheeraad ah ee godka dhulalka buurta ah halkaan&lt;/b&gt;. Dhulalka buuraha u muuqdaan inay ka dhacaan markii dhulka uu ka qoyanyahay qeybaha roobka AMA dhulka gariirka sababo. Hoos uga soco dhacdooyinka taariiqiga ah si aad u aragtid dhulka buurta lagu qoray aagaaga. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Lagama yaabo inaad ku aragtid taraarax halkaan&amp;#44; laakin waxaad ku arki kartaa mid u dhow dalcadaha dagaandaga haddii xaaladaha ay saxantahay&lt;/b&gt;. Isha ku hay aagaga aan xasilooneyn. Gaar ahaan wadooyinka ay xireen haraayada ama xaalufay. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Miyay dalcadaha dagaandaga u dhowyihiin meel aan qudaar ka bixin? Miyuu roob da’ayay maalmo? &lt;b&gt;Haddii ay haa tahay&amp;#44; dalcadaha dagaandaga ka dhig si ay aad ugu dhowdahay dhulka buurta ah inay halkaan ka dhacdo&lt;/b&gt;. Isha ku hay aagaga aan xasilooneyn. Gaar ahaan wadooyinka ay xireen haraayada ama xaalufay. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Dhulalka buurta ah waxy inta badan ka dhacdaa illaa taraaraxa xeebta hore ee hirarka ku dhufanayo leemanka xeebta. &lt;b&gt;Biyaha Puget Sound waxay ka kaceen 8 injis tan iyo 1913&lt;/b&gt;! Oo leh heerarka biyaha sareeyo ee nabaadguurka hore ee imaan karo way kordhayaan. Roobka xad dhaafka ee duufaanada daran waxay sidoo kale yareyn karaan dalcadaha ee kicinayo dhulalka buurta badan ee Gobolka King. Riix sawirka lagu ogaanayo wax badan.&lt;br&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storms Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Miyaad maqashaa dhawaqyada alwaaxa dilaacayo&amp;#44; dhagaxaan isgaraacayo&amp;#44; guuxa dhulka? Ma aragtaa jeexyada muuqaalka dhulka iyo dhaqaaqa dalcadaha hoose ee dhulka&amp;#44; dhagaxaanta&amp;#44; iyo qudaarta? Waxay noqon kartaa dhulka buurta ah. U dhaqaaq dhul xasiloon.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;QIIMEY&lt;/b&gt; - Haddii aaga agagaarka gurigaaga laga yaabo inuu u nugulyahay dhulalka buurta &lt;b&gt;&lt;b&gt;raadi tallada taqasusyada dhulka&lt;/b&gt;. Waxay qiimeyn karaan halista dhulka buurta iyo/ama naqshada farsamooyinka saxitaanka ee lagu yareynayo dhulalka buurta.&lt;/li&gt;&lt;li&gt;&lt;b&gt;YAREY HALISTA&lt;/b&gt; -  Abuur daboolka dhulka ee jiirada iyo/ama dhis darbi celinayo ee xasilinayo  &lt;b&gt;dhinacyada buurta.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;DIYAARI&lt;/b&gt; - &lt;b&gt;Samey sanduuqa saadka iyo qorshaha qoyska &lt;/b&gt; oo naqshadeynayo ugu yaraan labo wadooyin badbaado ah&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Ka joogitaanka wadada dhulka buurta ama haraaga waa illaaladaada ugu wanaagsan.&lt;/b&gt; Sahanka Dhulka Mareykanka sidoo kale wuxuu ku taliyay sida xigta&amp;#44; &lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;&lt;b&gt;KA DIGTOONOW - Dhageyso dhawaqyada aan caadiga aheyn&lt;/b&gt;. Xoogan&amp;#44; kala go’a gaaban ee roobka waxay noqon kartaa halis gaar ah&amp;#44; gaar ahaan muddooyin dheer kadib ee dhacitaanka roobka xoogan iyo cimilada qoyan.&lt;/li&gt;&lt;li&gt;&lt;b&gt;TIXGELI KA TAGIDA&lt;/b&gt; - Haddii aad joogtid aagaga ee unugul dhulalka buurta ah iyo qulqulada haraaga&amp;#44; tixgeli ka tagida haddii ay badbaado tahay inaad sidaas sameysid. Haddii aad go'aansatid inaad guriga joogtid&amp;#44; u dhaqaaq sheekada labaad haddii ay suurtogal tahay.&lt;/li&gt;&lt;li&gt;&lt;b&gt;OGOW HEERARKA DURDURKA&lt;/b&gt; - Haddii aad u dhowdahay durdur ama kanaal&amp;#44; &lt;b&gt;ka digtoonow kordhin walboo lama filaan ah ama hoos u dhaca qulqulka biyaha iyo isbadelka biyaha cad oo dhoobo noqonayo&lt;/b&gt;. Kuwaan waxay tilmaami kartaa durdurka kore ee howsha dhulka buurta ah. HAKA DAAHIN! Keydi nafsadaada&amp;#44; ma ahan alaabahaaga.
+&lt;/li&gt;&lt;/ul&gt; Waxaad ka heli kartaa dhulalka buurta ah oo badan USGS  &lt;a href=http://landslides.usgs.gov/learn/prepare.php target=_blank&gt;halkaan&lt;/a&gt;. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Landslide_during.jpg" alt="This is a panel of three cartoon images showing what to do during an a landslide. Stay Alert&amp;#44; Leave the area&amp;#44; and Don't Delay." title="During Landslide Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;U DIYAAR AHOW FATAHAADA (dhulka buurta ah inta badan waxaa xiro wabiyada oo waxay ku sababi karaan wabiyada inay dib u laabtaan oo fatahaan)&lt;/b&gt;.&lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;Ka fogow taraaraxa. Taraaraxyada kale waxay dhici karaan kadib taraaxada guud.&lt;/li&gt;&lt;li&gt;Marka ay badbaado tahay&amp;#44; ka hubi dadka dhaawacmay ama xanibmay.&lt;/li&gt;&lt;li&gt;Ka hubi waxyeelada leemanka korontada oo soo wargeli waxyeelo walba shirkadaada korontada.&lt;/li&gt;&lt;li&gt;Dhageyso warbaahinta deegaanka ama raadiyowga Cimilada NOAA oo warbixinta hadeer ah.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wixii warbixin dheeraad ah ka fiiri bogga Waaxda Illaha Dabiiciga ee &lt;a href=http://www.dnr.wa.gov/programs-and-services/geology/geologic-hazards/landslides#some-historic-landslides-in-washington-state target=_blank&gt;dhulalka buurta&lt;/a&gt; iyo &lt;a href=http://file.dnr.wa.gov/publications/ger_fs_landslide_hazards.pdf target=_blank&gt;halisaha dhulalka buurta ah&lt;/a&gt;. Wixii dhulalka buurta ee xaafadaada&amp;#44; fiiri warbixin laha heli karo &lt;a href=http://www.seattle.gov/dpd/aboutus/whoweare/emergencymanagement target=_blank&gt;&lt;b&gt;Seattle&lt;/b&gt;&lt;/a&gt; iyo &lt;a href=http://www.kingcounty.gov/services/environment/water-and-land/landslides.aspx target=_blank&gt;&lt;b&gt;Gobolka King&lt;/b&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ma jiraan dhulalka buurta oo halkaan lagu aqoonsaday&lt;/b&gt; (&lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;Wargelinta 2016&lt;/a&gt;). Dhulalka buurta caadi ayay ka yihiin dhal la’aanta&amp;#44; dalcadaha dagaandaga halka daadashooyinka isugu imaadaan. Haddii aad ku nooqshahay meel ka hooseyso aaga sida midaan ka taxadar halisahaaga (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg=en target=_blank&gt;qariirada&lt;/a&gt;). Si loogu baaro fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt; Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Saynisyahanada kama aqoonsan wax dhul gariir ah halkaan&lt;/b&gt;. Wixii warbixin dheeraad ah fiiri &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Wargelinta 2016&lt;/a&gt; iyo &lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;qariirada&lt;/a&gt;. Si loogu baaro fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ma jiraan dhulalka buurta ee lagu aqoonsaday halkaan&lt;/b&gt; sida waafaqsan daraasada 1995 ee taraaraxa Caasimafa Seattle. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ma jiraan daraasad lagu dhameystiray halkaan&lt;/b&gt; ee lagu aqoonsanayo haddii dhulalka buurta taariiq ahaan jireen (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;DHULALKA BUURTA WAXAY KA DHACDAY HALKAAN&lt;/b&gt; ee waqti yar ee la soo dhaafay (&lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;Wargelinta 2016&lt;/a&gt;) iyo (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;). Taraaraxyada taariiqiga ah laga yaabo ama laga yaabin inay tilmaanto taraaraxa mustaqbalka dhici karo. Si loo ogaado haddii halisaha weli ka jiraan aaga baahiyada qiimeynta gaarka ah ee uu sameynayo la taliyaha farsamada dhulka. Si loogu baaro fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;DHULALKA BUURTA WAXAY KA DHACDAY HALKAAN&lt;/b&gt; ee waqti yar ee la soo dhaafay (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Wargelinta 2016&lt;/a&gt;) iyo (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;). Taraaraxyada taariiqiga ah laga yaabo ama laga yaabin inay tilmaanto taraaraxa mustaqbalka dhici karo. Si loo ogaado haddii halisaha weli ka jiraan aaga baahiyada qiimeynta gaarka ah ee uu sameynayo la taliyaha farsamada dhulka. Si loogu baaro fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;DHULALKA BUURTA iyo DHACITAANKA DHAGAXA WAXAY KA DHACDAY HALKAAN&lt;/b&gt; ee waqti yar ee la soo dhaafay (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Wargelinta 2016&lt;/a&gt;) iyo (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;). Taraaraxyada taariiqiga ah laga yaabo ama laga yaabin inay tilmaanto taraaraxa mustaqbalka dhici karo. Si loo ogaado haddii halisaha weli ka jiraan aaga baahiyada qiimeynta gaarka ah ee uu sameynayo la taliyaha farsamada dhulka. Baar fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;DHACITAANKA DHAGAXA WAXAY KA DHACDAY HALKAAN&lt;/b&gt; ee waqti yar ee la soo dhaafay (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Wargelinta 2016&lt;/a&gt;) iyo (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;). Taraaraxyada taariiqiga ah laga yaabo ama laga yaabin inay tilmaanto taraaraxa mustaqbalka dhici karo. Si loo ogaado haddii halisaha weli ka jiraan aaga baahiyada qiimeynta gaarka ah ee uu sameynayo la taliyaha farsamada dhulka. Baar fadhiyada xogta si aad u dhow ee &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;Gobolka King iMap&lt;/a&gt; (iska hubi dhulalka buurta in lagu eego sheekada).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;DHULALKA BUURTA WAXAY KA DHACDAY HALKAAN&lt;/b&gt; sida waafaqsan daraasada 1995 ee tararaxyada Caasimada Seattle (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;qariirada&lt;/a&gt;). Taraaraxyada taariiqiga ah laga yaabo ama laga yaabin inay tilmaanto taraaraxa mustaqbalka dhici karo. Si loo ogaado haddii halisaha weli ka jiraan aaga baahiyada qiimeynta gaarka ah ee uu sameynayo la taliyaha farsamada dhulka.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Kani waa bulsho halis aad u sareyso ugu jirto dabka duurka&lt;/b&gt;. Waa xaduuda u dhaxeyso aadanaha iyo duurka. Galbeedka Washington waa heer kulul&amp;#44; laakin dabka duurka waxay ku dhuftaan qeybta bariga ee Gobolka King sannad walba. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Aagaan looma aqoonsan sida inay leedahay halis sareyso ee dabka duurka&lt;/b&gt;&amp;#44; laakin waxay ku taalaa gudaha mayl barkiisa ee bulshada halista sareyso. Xaaladaha wanaagsan dabka duurka wuu faafayaa. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;qariirada&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Aagaan waxay leedahay halis hooseyso aad u hoseyso ee dabka duurka&lt;/b&gt;. Haddii aad ku nooshahay meel u dhow aaga alwaaxda ka taxar dabka duurka wuu dhici karaa. &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Sida tani ay tahay biyo&amp;#44; ma jiraan filashada dabka duurka ee ka jiray halkaan.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Waxaad kala kulmi kartaa dabka duurka oo weyn halkaan&lt;/b&gt;. Waxay noqoneysaa dhaqaaqa dheereeyo&amp;#44; ee la jiro holac weyn oo dhaqso ayuu badeli karaa jahada. Waxay ku qaadan kartaa dab damiyayaasha maalmo ama isbuucyo inay damiyaan. QIIQA ka imaanayo baaxada dabka duurka wuu safri karaa oo waxay xaqiiq u noqon kartaa xittaa haddii waxba aan ku gubaneynin meel kuu dhow. Ka hubi tayada hawadaa deegaankaaga &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;halkaan&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Uma badna&amp;#44; laakin haddii aad ku nooshahay meel u dhow aaga duurka ah waxaad la kulmi kartaa dabka duurka&lt;/b&gt;. QIIQA ka imaanayo baaxada dabka duurka wuu safri karaa oo waxay xaqiiq u noqon kartaa xittaa haddii waxba aan ku gubaneynin meel kuu dhow. Ka hubi tayada hawadaa deegaankaaga &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;halkaan&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tirada &lt;b&gt;dabka duurka ee Badda Wuqooyiga galbeed marhore ayay si weyn u korodhay labaatankii sanno ee la soo dhaafay&lt;/b&gt;. Isbedalkaan wuxuu u dhowyahay inuu ku sii socdo kuleelo qalalan oo duufaan badan (ka fakir daarida dhimbilaha dabkaas). Aagaga weyn ee duurka wuu guban karaa oo qiiq gelin karaa hawada. Riix sawirka lagu ogaanayo wax badan.&lt;br&gt;&lt;a  ref="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Forests.jpg" alt="Climate Change Forest Infographic"&gt;
+&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Ma urineysaa ama ma aragtaa qiiq? Miyay balaaratay abalaaratay cimilada qalalan? Waxay noqon kartaa dabka duurka. Si cad uga tala bixi dabka firfircoon iyo haddii aad aragtid mid soo wac 9-1-1 si aad usoo wargelisid.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;BOOS SAMEEY&lt;/b&gt; - Ka illaali nololaha iyo hantiyada adiga oo aasaasayo &lt;b&gt;boos dabka qabsado ee agagaarka gurigaaga&lt;/b&gt;&amp;#44; harka&amp;#44; iyo ganacsiga. Si aad u ogaatid sida ka fiiri &lt;a href=http://www.firewise.org/wildfire-preparedness.aspx target=_blank&gt;firewise.org&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;DAAWO CIMILADA&lt;/b&gt; - Dhoor maalmood qurax ah waxay ku qalali karaan duurarkeena oo ku filan inay dab qabsadaan. Xaalada dabeysha waxay ku sababi kartaa dabka duurka in la xakameyn waayo durbadiiba.&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Firewise_Brochure.jpg" alt="This is an image of ways to prevent wildfire around your home. They include screening decks&amp;#44; pruning trees 6-10 feet from the ground&amp;#44; using fire-resistant wall and roof materials&amp;#44; keeping plants watered&amp;#44; and making sure your driveway can accommodate an emergency vehicle" title="How to Prepare Your Home for Wildfire"&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;DIGTOONOW&lt;/b&gt; - Ka dhageyso digniinada degdega deegaanka raadiyowga iyo/ama talefishanka oo u diyaargarow inaad ka badbaadid haddii ay muhiim tahay.&lt;/li&gt;&lt;li&gt;&lt;b&gt;KA SAAR WAXYAABAHA GUBAN KARO&lt;/b&gt; - Ka saar alaabaha agaagrka guriga ee ay ku qabsan karaan dabka (kuraasta cowska ah&amp;#44; miisaska&amp;#44; iwm.).&lt;/li&gt;&lt;li&gt;&lt;b&gt;DIYAARGAREE GURIGAAGA&lt;/b&gt; - Dhaqaaji ka dabool alaabah guriga daaqadaha. Xir albaabada iyo daaqadaha&amp;#44; laakin ha xirin iyaga.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Fire_during.jpg" alt="This is an icon of an exclaimation point with two triangles behind it" title="During Fire Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gurigaaga ku laabo markii maamulada ay dhahaan waa badbaado.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Isticmaal taxadarka marka aad galeysid aagaga guban&lt;/b&gt; sida halisaha ay weli jiri karto.&lt;/li&gt;
+&lt;li&gt;Fiiri iyo dib u fiiri qiiqa ama dhimbilaha qarsoon.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Sawir waxyeelada&lt;/b&gt; oo ujeedooyinka caymiska.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Haddii aad u maleysay in hantidaada ay halis ku jrii karto &lt;b&gt;Gobolka King wuxuu hayaa warbixinta milkiilayaasha dhulka&amp;#44; barnaamijyada dhiirogelinta&amp;#44; iyo aqoon isweedaarsiyada tababarka la martigeliyay&lt;/b&gt;. Waxaad ka heli kartaa waxbadan &lt;a href=http://www.kingcounty.gov/environment/water-and-land/forestry.aspx target=_blank&gt;halkaan&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Bariga Gobolka King wuxuu leeyahay dabka yar ee duurka ah sannad walba. Caadi ahaan aadanaha ayaa sababay. Fiiri halka dabka ka dhacay xiliga la soo dhaafay adiga oo riixayo &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_Historic.jpg target=_blank&gt;halkaan&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Foolkaanooyinka (qulqulka dhoobada foolkaanada) waa halista ugu weyn ee la xiriirto Buurta Rainier. &lt;b&gt;Dadka dagan Koonfurta Gobolka King waxay leeyihiin 1 ee 10 fursad ee la kulmida foolkaanada ee nololshooda oo dhan&lt;/b&gt;. Buurta Rainier waxaa loo tixgeliyaa foolkaano firfircoon&amp;#44; laakin waxay noqon kartaa sannooyin badan illaa ay ka qaraxdo markale.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Haddii foolkaanada ay kiciso Buurta Rainier&amp;#44; &lt;b&gt;aagaan wuxuu la kulmi karaa fatahaad iyo haraaga sida dhoobada&amp;#44; ciida&amp;#44; dhagaxaanta&amp;#44; iyo haraaga kale ee hoosta wabiga oo foolkaanada ah&lt;/b&gt;. Tani waxay ka dhici kartaa sannooyin illaa labaataneeyo sanno foolkaanada kadib. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;A 10% - 40% fursad ka jirtay foolkaanada ee Buurta Rainier oo mareyso illaa gobolkaan oo 50-ka sanno ee xiggo&lt;/b&gt;. Dabeecada foolkaanada oo u egtahay dhagax qoyan oo socdo. Dhoobo qaro adag iyo haraa ayaa daboolayo aaga haddii mid dhacdo. Tani waxay si xun u waxyeeleyn kartaa dhismaha oo waxay qaadan kartaa muddo dheer in looga soo kabsado. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;A 5% - 10% fursad ka jirtay foolkaanada ee Buurta Rainier oo mareyso illaa aagaan oo 50-ka sanno ee xiggo&lt;/b&gt;. Dabeecada foolkaanada oo u egtahay dhagax qoyan oo socdo. Dhoobo qaro adag iyo haraa ayaa daboolayo aaga haddii mid dhacdo. Tani waxay si xun u waxyeeleyn kartaa dhismaha oo waxay qaadan kartaa muddo dheer in looga soo kabsado. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Waxaad joogtaa AAGA KA BAXSAN HALISTA FOOLKAANADA&lt;/b&gt;. Haddii Buurta Rainier qaraxdo dambas ayaa daboolayo gobolka. Waxay aad ugu ekaaneysaa sida aagaga saameysay qaraxa Buurta Saint Helen ee 1980. Qara weynida dambasta waxay ku kala duwanaaneysaa baaxada qaraxa. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(qariirada)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foolkaanada caadi ahaan waxay siisaa siinyaalo digniin ah maalmo illaa billo ka hor inta aysan qarxin. &lt;b&gt;Howlaha gaaska iyo dhulgariirka wuu kordhaa iyo saqafka dhulka wuxuu u bararaa sida biyaha dhaxa ku qulqulayo hoosteeda&lt;/b&gt;. Illaa aastaamahaan waxay noqon kartaa dhismo bulshada guud ah&amp;#44; Buurta Rainier waxaa si joogta ah u maamulay saynisyahanada leh &lt;a href=http://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;Barnaamijka Halisaha Foolkaanada USGS&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;WEYDII&lt;/b&gt; - Ogow tallaabooyinka saraakiisha deegaanka qaadeen oo ay ugu diyaar garoobeen dhacdooyinka foolkaanada. &lt;b&gt;Weydii saraakiisha bulshada waxa qorshahooda uu yahay iyo sida ay kugula soo xiriirayaan inta lagu jiro dhacdada&lt;/b&gt;. Waxaad ku sameyn kartaa midaan adiga oo la xiriirayo Xafiiska Gobolka King &lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=_blank&gt;ee Maamulka Degdega&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;QORSHAHA&lt;/b&gt; - La hadal saaxibadaada iyo dariska. Haddii aad joogtid aag halis sareyso&amp;#44; &lt;b&gt;go’aanso halka aad aadi laheyd&amp;#44; waxa aad keeni laheyd&amp;#44; iyo cida aad la xiriiri kartid&lt;/b&gt;.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Inta lagu jiro qaraxa&amp;#44; dhageyso wararka aqbaaraha degdega iyo raac tilmaamaha gurmadka.
+&lt;ul&gt;&lt;li&gt;&lt;b&gt;AAGA FOOLKAANADA - Hel dhul sareeyo isla markiiba.&lt;/b&gt;&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;BANAANKA&lt;/b&gt; - Dabool afkaaga&amp;#44; sankaaga&amp;#44; iyo jirka si aad uga fogaatid xanaaqa. &lt;b&gt;Hel hoy&lt;/b&gt;. &lt;/li&gt;
+&lt;li&gt;&lt;b&gt;GUDAHA - Xir albaabada iyo daloolada guriga oo gudaha ku jir&amp;#44; illaa lagaa tilmaamo haddii kale&lt;/b&gt;. Saar shukumaanada xun mareenada albaabka iyo kuleey daaqadaha. Dami matoorada gaariga iyo taraagyada si aad uga fogaatid waxyeelada cariiriga dambasta. Ka illaali xayawaanada iyo mashiinada adiga oo keenayo gudaha ama aaga daboolan.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/intensity/Volcano_during.jpg" alt="This is an panel of three images of what to do during a volcanic eruption or lahar. In lahar zone&amp;#44; outside&amp;#44; inside." title="During Volcano Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kadib halista degdega ah ee qaraxa way yaraatay&amp;#44; nadiifinta dhacitaanada dambasta waxay noqoneysaa dhacdada ugu weyn.&lt;br&gt;  &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/MtStHel_Yakima_graders.jpg" alt="This image shows two graders shoveling inches of ashfall from Saint Helens' eruption" title="Ashfall Cleanup in Yakima After Mt. Saint Helens"&gt;&lt;li&gt;Xiro ookiyaale iyo maaskaraha wajiga marka aad banaanka joogtid. &lt;b&gt;Tayada hawada way liidaneysaa&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Ka fogow daarnaashaha matoorka gaariga&lt;/b&gt;. Haddii ay tahay inaad ka xeysid&amp;#44; ku haay xawaaraha hoos (oo ka yar 35 MPH) oo fiiri ooliyada&amp;#44; fiiltarada ooliyada&amp;#44; iyo fiiltarada hawada waa joogto. &lt;/li&gt;&lt;li&gt;Dhacitaanada dambasta way culustahay oo waxay ku sababi kartaa dhismooyinka inay dumaan. Haddii ay badbaado tahay inaad sidaas sameysid&amp;#44; &lt;b&gt;ka cadey dambasta safaqyada iyo roob celiyayaasha&lt;/b&gt;.&lt;/li&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Waxaad wax badan ka baran kartaa ee ku saabsan Buurta Rainier iyo halisaha imaan karo illo badan: 
+&lt;ul&gt;&lt;li&gt;&lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;Kormeerida iyo warbixinta kale&lt;/a&gt; - Sahanka Dhulka Mareykanka&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=blank&gt;Warbixinta Guud ee Gobolka King&lt;/a&gt; - Gobolka King&lt;li&gt;&lt;a href=https://www.nps.gov/mora/planyourvisit/geohazards.htm target=_blank&gt;Dhulka halista ah ee Rainier&lt;/a&gt; - Adeega Darjiinka Qaranka&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.pnsn.org/volcanoes/mount-rainier target=_blank&gt;Dhul gariirka u dhow Rainier&lt;/a&gt; - Badda Wuqooyiga galbeed Shabakada Seismic&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Buurta Rainier waxay leedahay taariiq dheer oo &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_eruption_history.html target=_blank&gt;qaraxyo ah&lt;/a&gt; iyo &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_lahars.html target=_blank&gt;foolkaano&lt;/a&gt;. Qiyaastii 500 sanno ka hor Qulqulka dhoobada Electron ayaa usu keenay buurta hoose ee ku safrayo dhinaca Puyallup iyo sida dheer ee Sumner&amp;#44; WA. Kumanaanka sanno ka hor inta aysan foolkaanadaas badan ku safrin dhinaca wabiyada gaarayo sida ugu dheer ee Auburn.  &lt;b&gt;Magaalooyinka qaarkood (NE Tacoma&amp;#44; Orting&amp;#44; iyo Puyallup) waxay dhisantahay haraayada foolkaanada taariqiga ah.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Qaboobaha Gobolka King oo dhan wuxuu keeni karaa heerkululka qabow hooseeyo&amp;#44; wadooyin baraf ah&amp;#44; iyo duufaanaha weyn ee imaan kara. Dhacitaanka barafka wuxuu dhacaa mararka qaarkood&amp;#44; iyo aad u leedahay taagag sare. &lt;b&gt;Duufaanada qaboobaha waxay keeni karaan dabeyl sareyso ee ku sababo inay geedaha dhacaan oo korontada danto.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Dhacdada dhacitaanka baraf la taaban karo wuxuu ku sababi karaa carqalado gaadiidka&amp;#44; adeegyada badbaadada bulshada&amp;#44; iyo korontada. &lt;b&gt;Korontada waxay maqnaan kartaa maalmo badan.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Badda Wuqooyiga galbeed waxay arkeysaa duufaan aad u daran oo 50-ka sanno ee xigo&lt;/b&gt;. Waxay qaadi karaan dabeyl culus&amp;#44; dhacitaanka roobka mahiigaanka ah oo sababayo fatahaada. Howlaha qaboobaha way saameyneysaa. 2015 arag heerarka bacda barafka la qoray ee ugu hooseyso oo leh kaliya 4% oo isku celcelis. Qaboobaha diiran wuxuu dajinayaa heerka abaaraha gobolka oo dhan. Riix sawirka lagu ogaanayo wax badan.  &lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Winter.jpg" alt="Climate Change Winter Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Saadiyayaasha wuxuu sameeyay guul wanaagsan ee saadaalinta barafka iyo duufaanaha barafka. &lt;b&gt;Ka taxadar saadaalinta cimilada deegaanka oo iska diiwaangeli digniinta la heli karo iyo nidaamyada digniinta &lt;/b&gt;(&lt;a href=http://alert.seattle.gov/ target=_blank&gt;Digniin sii Seattle&lt;/a&gt; iyo &lt;a href=http://www.kingcounty.gov/depts/emergency-management/alert-king-county.aspx target=_blank&gt;Digniin sii Gobolka King&lt;/a&gt;) si aad u hubisid inaad heshid warbixinta ugu dambeyso ee ku saabsan cimilada daran ee hartay.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;HEL SAADADKA - Keydso shidaal dheeraad ah iyo saadadka gurmadka&lt;/b&gt; si aad ugu badbaadid dhoor maalmood iyada oo aan kroonto jirin&amp;#44; kuleelka&amp;#44; iyo biyaha kulul. Tixgeli inaad iibsatid ganareetar oo raac heerarka badbaadada.&lt;/li&gt;&lt;li&gt;&lt;b&gt;QABOOJI GURIGAAGA&lt;/b&gt; - Geli daaqadaha duufaanta. Dahaarsaar darbiyada&amp;#44; dusha sare&amp;#44; iyo tuubooyinka. Saar biya celiyaha iyo goomaha cimilada albaabada iyo daaqadaha. U ogolow tubooyinka inay waxyar tifqaan inta lagu jiro cimilada qabowga si ay ugu joogteyso tubooyinka inay barafoobaan. &lt;b&gt;Baro sida loo damiyo faalfayaasha (haddii tuubo ay jabto)&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;QABOOJI GAWAARIDAADA&lt;/b&gt; - Ku hayso shidaalka si buuxdo ugu yaraan buux barkiisa. Hubi batariga&amp;#44; qalabka kicinta&amp;#44; hiitarka&amp;#44; nalalka&amp;#44; bareekyada&amp;#44; iyo taayarada. Ku buuxi biya daga ka hortaga barafka&amp;#44; ooliyada&amp;#44; iyo daaqadaha dhaqo biyaha. &lt;b&gt;Ku hay saadadka gurmadka qaboobaha buudkaaga.&lt;/b&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;LA SOCO&lt;/b&gt; - Ka kormeer aqbaaraha deegaanka talefeshinkaaga&amp;#44; qalabka mobeelka&amp;#44; ama raadiyaha batariga ku shaqeeyo. Raac tilmaamaha degdega oo ka taxadar inaad u safartid tallo bixin.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;KA FOGOW SAFARKA&lt;/b&gt; - Haddii ay tahay inaad gaari kaxeysid&amp;#44; buuxi taangiga shidaalka&amp;#44; haay wadooyinka weyn&amp;#44; oo ogeysii dadka kale faahfaahintaada. Is tartiibi. Haddii aad xayirantid&amp;#44; u yeero caawin&amp;#44; daar nalalka halisaha&amp;#44; oo gaarigaaga joog. Banaanka cagahaaga haku fariisan illaa hoy uu kuu dhowyahay.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;OGOW HALISAHAAGA &lt;/b&gt;- 
+&lt;ul&gt;
+&lt;li&gt;&lt;b&gt;Barafowga&lt;/b&gt; - Haddii aad ogaatid aastaamaha hel caawinta caafimaadka isla markaasba. Wixii aastaamaha iyo warbixin kale riix &lt;a href=https://www.cdc.gov/disasters/winter/staysafe/hypothermia.html target=_blank&gt;halkaan&lt;/a&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Sumowga Gubashada Gaaska&lt;/b&gt; - Waxay dhacdaa markii shidaalka sida gaaska&amp;#44; ooliyada&amp;#44; bansiinka&amp;#44; alwaaxa&amp;#44; ama dhuxusha ay ku gubato boos xiran. Boqolaal dad ayaa sannad walba si shil ah ugu dhinto. Ka ogow wax badan &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/carbon-monoxide.aspx target=_blank&gt;halkaan&lt;/a&gt;.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;li&gt;&lt;b&gt;KA FOGOW HALISAHA&lt;/b&gt; - Si cad uga tala bixi leemanka korontada soo dhacay&amp;#44; fatahaada&amp;#44; wadooyinka&amp;#44; iyo qaabdhismeedyada kale ee dumiyay barafka culus am barafka.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Winter_during.jpg" alt="This is a panel of four images of what to do during bad winter weather. Stay Tuned&amp;#44; Stay Inside&amp;#44; Know Risks&amp;#44; and Avoid Hazards." title="During Winter Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;Dib u iibso saadadka gurmadka&lt;/b&gt;. U diyaargarow haddii duufaan kale ku dhafato.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Hormari qorshaha qoyskaaga&lt;/b&gt; - Maxaa shaqeeyay? Maxaa la wanaajin karaa?&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;La hadal dariskaaga&lt;/b&gt;. La wadaag tallooyinka iyo afkaaraha midba midka kale.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Baro wax badan oo ku saabsan xaalada qaboobaha iyo sida loo diyaar garoobo: 
+&lt;ul&gt;&lt;li&gt;
+&lt;a href=http://takewinterbystorm.org target=_blank&gt;Ku qaado Qaboobaha Duufaan ahaan&lt;/a&gt;-  Tallooyinka diyaargarowga iyo warbixinta la cusbooneysiiyay ee Galbeedka Washington&lt;/li&gt;
+&lt;li&gt;
+&lt;a href=http://kingcounty.gov/depts/transportation/metro/alerts-updates/winter.aspx target=_blank&gt;Gobolka King Qaboobaha Metro&lt;/a&gt; - Qadadka app-ka qorsheynta safarada qaboobaha iyo digniinta cimilada &lt;/li&gt;
+&lt;li&gt;
+&lt;a href=https://www.seattle.gov/transportation/winterweather.htm target=_blank&gt;Waaxda Gaadiidka ee Seattle&lt;/a&gt; - Fiiri halka baraf ka dhacay iyo warbixinta kale ee xaaladaha wadada &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Taxanaha barafka&amp;#44; barafka iyo roobka duufaanta ee bilowga Diseembar 26&amp;#44; 1996&amp;#44; wuxuu sababay 16 dhimasho oo gobolka ah iyo $57 milyan oo waxyeelo ah ee Gobolka Seattle iyo King&lt;/b&gt;. Labo duufaano — hal gubasho 6-12 inji iyo 10 inji ee barafka qoyan — halka ay raacaan roobka culus kaas oo dumay kanbiga&amp;#44; meesha doomanka daboolan&amp;#44; iyo leemanka korontada oo wareegto ah. Adeega la hakiyay ee ku meelgaark aah ee Metro gabi ahanba waqtigii ugu horeysay ee taariiqdeeda. Qabowga iyo dhallaalka barafka waxay ku deeqaan fatahaad iyo dhulalka buurta ah inta lagu jiro isbuuca xiggo. Diyaar ma u tahay haddii duufaan saan oo kale ah ay dhacdo markale?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ha u ogolaan dhacitaanka roobka iyo qaboobaha inay ku harowdasaan&amp;#44; &lt;b&gt;kuleelaha Gobolka King wuxuu noqon karaa KULEEL. Mararka qaarkood heer kululka wuxuu u kacaa illaa heerka 90s oo maalmo badan ah waqtigiiba&lt;/b&gt;. Duufaanta hilaaca&amp;#44; duufaanta dabeysha&amp;#44; dabka duurka&amp;#44; iyo hirarka kuleelka waa suurtogal gobolka oo dhan.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kuleel daran ayaa socon karo maalmo oo ku sababayo bulshooyinka inay arkaan korodhka kuleelka la xiriiro jirada oo ay ku jiraan DAALKA KULEELKA iyo ISTAROOGA KULEELKA. Heerkululka biriqda&amp;#44; xaaladaha qaleelka&amp;#44; iyo korodhka suurtaglnimada biriqda ee dabka duurka.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Luuliyo 2015 waxay aheyd bisha ugu kulul ee soo marta! &lt;b&gt;Isku celceliska heerkululka sannadlaha waxaa lagu saadilay inay kordheyso inta u dhaxeyso heerka 3 iyo 10 ee Heerkululka xiliga 2100&lt;/b&gt;. Dadka dagan Washington waxay arkayaan dhacitaanka roobka kuleelaha&amp;#44; laakin dhacitaanka roobka ee aan ka dhicin wuu cuslaanayaa (ku fakar roob culus). Riix sawirka lagu ogaanayo wax badan. &lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storm Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Daalka kuleelka iyo istarooga kuleelka waa jiro daran ee dhici karta markii qofka gaaro kuleel daran.&lt;/p&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;AASTAAMAHA DAALKA KULEELKA&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;Dhidid badan&lt;/li&gt;
+&lt;li&gt;Tabar daro&lt;/li&gt;
+&lt;li&gt;Garaaca wadnaha oo liito&lt;/li&gt;
+&lt;li&gt;Suuxdin&lt;/li&gt;
+&lt;li&gt;Matag&lt;/li&gt;
+&lt;li&gt;Qabow&amp;#44; maqaarka cadaado&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;AASTAAMAHA ISTAROOGA KULEELKA&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;Heerkululka jirka sareeyo (103F ama ka sareeyo)&lt;/li&gt;
+&lt;li&gt;Maqaar kuleel oo qalalan&lt;/li&gt;
+&lt;li&gt;Garaaca wadnaha degdega oo xoogan&lt;/li&gt;
+&lt;li&gt;Miiyir beel suurtogal ah&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Dadka weyn&amp;#44; carruurta yar&amp;#44; iyo dadka qaba jirada maskaxda iyo cudurada raaga way ku badanyihiin halisaha arimaha kuleelka la xiriiro.
+&lt;ol&gt;&lt;li&gt;&lt;b&gt;OGOW AASTAAMAHA&lt;/b&gt; - Jirada kuleelka la xiriiro dhaqso ayay dhici kartaa. Ogow iyo midkee ka mid ah dariskaaga ayaa halis ku jiri karo. &lt;/li&gt;&lt;li&gt;&lt;b&gt;KA WARHAY&lt;/b&gt; - Dhageyso aqbaaraha deagaanka oo warbixinta guud ah iyo goobaha ee &lt;b&gt;xarumaha qaboojinta&lt;/b&gt; (boosaska bulshada ee ay u isticmali karaan dadka dagan inay isku qaboojiyaan).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;QABOOBANOW&lt;/b&gt; - Gudaha joog iyo&amp;#44; haddii ay suurtogal tahay&amp;#44; meesha qaboojiyaha (moolalka adeega&amp;#44; maktabadaha&amp;#44; masraxyada&amp;#44; iwm). Xadey howsha banaanka.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;ILLAALI MAQAARKAAGA&lt;/b&gt; - Xiro dhar qafiif ah&amp;#44; midib qafiif ah leh&amp;#44; oo dabacsan. Koofiyad ku dbaoosha oo balaaran&amp;#44; ookiyaale&amp;#44; iyo kareemka quraxda way ku caawineysaa.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;CAB BIYO&lt;/b&gt; - Cab biyo badan (ka fogow kafeega&amp;#44; qamriga&amp;#44; iyo cabitaanada sonkorta leh) oo qaado dhalo biyo ah.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;KA FAKAR DADKA KALE&lt;/b&gt; - Ka fogey carruurta iyo xaywaanada guriga baabuurta kulul. Fiiri qoyska halista ku jiro&amp;#44; saaxibada&amp;#44; iyo dariska inta badan.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Summer_during.jpg" alt="This is a panel of three images of what to do during bad summer weather. Stay Cool&amp;#44; Protect Skin&amp;#44; and Drink Water." title="During Summer Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Isticmaal daahyada daaqada &lt;b&gt;si aad ugu dabooshid daaqadaha si aad ugu hawada qabow ugu haysid gudaha&lt;/b&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Tixgeli iibsashada qalabka qaboojiyaha&lt;/b&gt; iyo/ama gelinta goomaha cimilada guriga halka hawada kulul ay ka soo gasho.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;DOOQA MIISAANIYADA HOOSE&lt;/b&gt;: Dhiso muujiyayaasha kuleelka (oo isticmaalka u dhaxeeyo daaqadaha iyo goomaha daaqadaha)&amp;#44; sida jaandiga kartoonada la daboolay&amp;#44; si loogu daboolo kartoomada bireed si ay ugu celiso kuleelka banaanka. Riix &lt;a href=http://www.instructables.com/id/Heat-blocking-curtains/ target=_blank&gt;halkaan&lt;/a&gt; oo DIY tilmaaha.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wixii warbixin dheeraad ah ee sida qabow loo ahaado iyo badbaadada madaxa &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/hot-weather.aspx target=_blank&gt;Cimilada Kuleelka&lt;/a&gt; ee Gobolka King bogga.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;2015&amp;#44; Gobolka King wuxuu diiwaaniyay tirada maalmaha ay dhaaftay 90F. &lt;b&gt;Luuliyo 2015 waxay aheyd bisha ugu kulul ee marnaba lagu qoray Gobolka King!&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>text-so</t>
   </si>
 </sst>
 </file>
@@ -14377,13 +15085,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K292"/>
+  <dimension ref="A1:L292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14392,10 +15100,10 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="8" max="10" width="53.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="21"/>
+    <col min="11" max="12" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14429,8 +15137,11 @@
       <c r="K1" s="20" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="20" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -14461,8 +15172,11 @@
       <c r="K2" s="21" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -14493,8 +15207,11 @@
       <c r="K3" s="21" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="21" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -14525,12 +15242,15 @@
       <c r="K4" s="21" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="21" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -14561,8 +15281,11 @@
       <c r="K6" s="21" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="21" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -14593,8 +15316,11 @@
       <c r="K7" s="21" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="21" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -14625,8 +15351,11 @@
       <c r="K8" s="21" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="21" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -14657,8 +15386,11 @@
       <c r="K9" s="21" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="21" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -14689,12 +15421,15 @@
       <c r="K10" s="21" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="21" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -14725,8 +15460,11 @@
       <c r="K12" s="21" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -14757,8 +15495,11 @@
       <c r="K13" s="21" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="21" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -14789,12 +15530,15 @@
       <c r="K14" s="21" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="21" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -14825,8 +15569,11 @@
       <c r="K16" s="21" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="21" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -14857,8 +15604,11 @@
       <c r="K17" s="20" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="21" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -14889,8 +15639,11 @@
       <c r="K18" s="20" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="21" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -14921,8 +15674,11 @@
       <c r="K19" s="21" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="21" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -14953,8 +15709,11 @@
       <c r="K20" s="21" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="21" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -14985,12 +15744,15 @@
       <c r="K21" s="21" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="21" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -15021,8 +15783,11 @@
       <c r="K23" s="20" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="20" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -15053,8 +15818,11 @@
       <c r="K24" s="21" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="21" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -15085,8 +15853,11 @@
       <c r="K25" s="21" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="21" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -15117,8 +15888,11 @@
       <c r="K26" s="21" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -15149,8 +15923,11 @@
       <c r="K27" s="21" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" s="21" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -15181,8 +15958,11 @@
       <c r="K28" s="21" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" s="21" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -15213,8 +15993,11 @@
       <c r="K29" s="21" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" s="21" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -15245,8 +16028,11 @@
       <c r="K30" s="21" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" s="21" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -15277,12 +16063,15 @@
       <c r="K31" s="21" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" s="21" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -15313,8 +16102,11 @@
       <c r="K33" s="21" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="21" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -15345,8 +16137,11 @@
       <c r="K34" s="21" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="21" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -15377,8 +16172,11 @@
       <c r="K35" s="21" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="21" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -15409,8 +16207,11 @@
       <c r="K36" s="21" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="21" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -15441,12 +16242,15 @@
       <c r="K37" s="21" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" s="21" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -15477,12 +16281,15 @@
       <c r="K39" s="21" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" s="21" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D40" s="3"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -15510,8 +16317,11 @@
       <c r="K41" s="21" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" s="21" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -15539,8 +16349,11 @@
       <c r="K42" s="21" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" s="21" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -15568,12 +16381,15 @@
       <c r="K43" s="20" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" s="20" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D44" s="3"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -15601,8 +16417,11 @@
       <c r="K45" s="1" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -15630,8 +16449,11 @@
       <c r="K46" s="1" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" s="1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -15659,8 +16481,11 @@
       <c r="K47" s="1" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -15688,8 +16513,11 @@
       <c r="K48" s="1" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" s="1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -15717,8 +16545,11 @@
       <c r="K49" s="1" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -15746,8 +16577,11 @@
       <c r="K50" s="1" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" s="1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -15775,8 +16609,11 @@
       <c r="K51" s="1" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" s="1" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -15804,8 +16641,11 @@
       <c r="K52" s="1" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -15833,8 +16673,11 @@
       <c r="K53" s="1" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L53" s="1" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -15862,8 +16705,11 @@
       <c r="K54" s="1" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54" s="1" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -15891,8 +16737,11 @@
       <c r="K55" s="1" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" s="1" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -15920,8 +16769,11 @@
       <c r="K56" s="1" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -15949,8 +16801,11 @@
       <c r="K57" s="1" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" s="1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -15978,8 +16833,11 @@
       <c r="K58" s="1" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -16007,8 +16865,11 @@
       <c r="K59" s="1" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -16036,8 +16897,11 @@
       <c r="K60" s="1" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -16065,8 +16929,11 @@
       <c r="K61" s="1" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -16094,8 +16961,11 @@
       <c r="K62" s="1" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>47</v>
       </c>
@@ -16123,8 +16993,11 @@
       <c r="K63" s="1" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63" s="1" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -16152,8 +17025,11 @@
       <c r="K64" s="1" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -16181,8 +17057,11 @@
       <c r="K65" s="1" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -16210,8 +17089,11 @@
       <c r="K66" s="1" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66" s="1" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -16239,8 +17121,11 @@
       <c r="K67" s="1" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -16268,8 +17153,11 @@
       <c r="K68" s="1" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68" s="1" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -16297,8 +17185,11 @@
       <c r="K69" s="1" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -16326,8 +17217,11 @@
       <c r="K70" s="1" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -16355,8 +17249,11 @@
       <c r="K71" s="1" t="s">
         <v>854</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -16384,8 +17281,11 @@
       <c r="K72" s="1" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -16413,8 +17313,11 @@
       <c r="K73" s="1" t="s">
         <v>856</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L73" s="1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>47</v>
       </c>
@@ -16442,8 +17345,11 @@
       <c r="K74" s="1" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L74" s="1" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -16471,8 +17377,11 @@
       <c r="K75" s="1" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L75" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -16500,8 +17409,11 @@
       <c r="K76" s="1" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L76" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>47</v>
       </c>
@@ -16529,8 +17441,11 @@
       <c r="K77" s="1" t="s">
         <v>860</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L77" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>47</v>
       </c>
@@ -16558,8 +17473,11 @@
       <c r="K78" s="1" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L78" s="1" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -16587,8 +17505,11 @@
       <c r="K79" s="1" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L79" s="1" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -16616,8 +17537,11 @@
       <c r="K80" s="1" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L80" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -16645,8 +17569,11 @@
       <c r="K81" s="1" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L81" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>47</v>
       </c>
@@ -16674,8 +17601,11 @@
       <c r="K82" s="1" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L82" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -16703,8 +17633,11 @@
       <c r="K83" s="1" t="s">
         <v>866</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L83" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -16732,8 +17665,11 @@
       <c r="K84" s="1" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L84" s="1" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -16761,8 +17697,11 @@
       <c r="K85" s="1" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L85" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>47</v>
       </c>
@@ -16790,8 +17729,11 @@
       <c r="K86" s="1" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L86" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>47</v>
       </c>
@@ -16819,8 +17761,11 @@
       <c r="K87" s="1" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L87" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>47</v>
       </c>
@@ -16848,8 +17793,11 @@
       <c r="K88" s="1" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L88" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -16877,8 +17825,11 @@
       <c r="K89" s="1" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L89" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -16906,8 +17857,11 @@
       <c r="K90" s="1" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L90" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -16935,8 +17889,11 @@
       <c r="K91" s="1" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L91" s="1" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>47</v>
       </c>
@@ -16964,8 +17921,11 @@
       <c r="K92" s="1" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L92" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>47</v>
       </c>
@@ -16993,8 +17953,11 @@
       <c r="K93" s="1" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L93" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>47</v>
       </c>
@@ -17022,8 +17985,11 @@
       <c r="K94" s="1" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L94" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -17051,8 +18017,11 @@
       <c r="K95" s="1" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L95" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -17080,8 +18049,11 @@
       <c r="K96" s="1" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L96" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -17109,8 +18081,11 @@
       <c r="K97" s="1" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L97" s="1" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -17138,8 +18113,11 @@
       <c r="K98" s="1" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L98" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -17167,8 +18145,11 @@
       <c r="K99" s="1" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L99" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -17196,8 +18177,11 @@
       <c r="K100" s="1" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L100" s="1" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>47</v>
       </c>
@@ -17225,8 +18209,11 @@
       <c r="K101" s="1" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L101" s="1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>47</v>
       </c>
@@ -17254,8 +18241,11 @@
       <c r="K102" s="1" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L102" s="1" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -17283,8 +18273,11 @@
       <c r="K103" s="1" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L103" s="1" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>47</v>
       </c>
@@ -17312,8 +18305,11 @@
       <c r="K104" s="1" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L104" s="1" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -17341,8 +18337,11 @@
       <c r="K105" s="1" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L105" s="1" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -17370,8 +18369,11 @@
       <c r="K106" s="1" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L106" s="1" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -17399,8 +18401,11 @@
       <c r="K107" s="1" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L107" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>47</v>
       </c>
@@ -17428,8 +18433,11 @@
       <c r="K108" s="1" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L108" s="1" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>47</v>
       </c>
@@ -17457,12 +18465,15 @@
       <c r="K109" s="1" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L109" s="1" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D110" s="3"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>53</v>
       </c>
@@ -17490,22 +18501,27 @@
       <c r="K111" s="21" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L111" s="21" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E112" s="13"/>
       <c r="H112" s="14"/>
       <c r="I112" s="16"/>
       <c r="J112" s="14"/>
       <c r="K112" s="21"/>
-    </row>
-    <row r="113" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L112" s="21"/>
+    </row>
+    <row r="113" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E113" s="13"/>
       <c r="H113" s="14"/>
       <c r="I113" s="16"/>
       <c r="J113" s="14"/>
       <c r="K113" s="21"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L113" s="21"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -17536,8 +18552,11 @@
       <c r="K114" s="21" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L114" s="21" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -17568,8 +18587,11 @@
       <c r="K115" s="21" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L115" s="21" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -17600,8 +18622,11 @@
       <c r="K116" s="21" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L116" s="21" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -17632,8 +18657,11 @@
       <c r="K117" s="21" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L117" s="21" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -17664,8 +18692,11 @@
       <c r="K118" s="21" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L118" s="21" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -17696,8 +18727,11 @@
       <c r="K119" s="21" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L119" s="21" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -17728,8 +18762,11 @@
       <c r="K120" s="21" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L120" s="21" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -17760,12 +18797,15 @@
       <c r="K121" s="21" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L121" s="21" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D122" s="4"/>
       <c r="I122" s="8"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -17796,8 +18836,11 @@
       <c r="K123" s="21" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L123" s="21" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -17828,8 +18871,11 @@
       <c r="K124" s="21" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L124" s="21" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -17860,8 +18906,11 @@
       <c r="K125" s="21" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L125" s="21" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -17892,8 +18941,11 @@
       <c r="K126" s="21" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L126" s="21" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -17924,8 +18976,11 @@
       <c r="K127" s="21" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L127" s="21" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -17956,8 +19011,11 @@
       <c r="K128" s="21" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L128" s="21" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -17988,8 +19046,11 @@
       <c r="K129" s="21" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L129" s="21" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -18020,12 +19081,15 @@
       <c r="K130" s="21" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L130" s="21" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D131" s="4"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -18056,8 +19120,11 @@
       <c r="K132" s="21" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L132" s="21" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -18088,8 +19155,11 @@
       <c r="K133" s="21" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L133" s="21" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -18120,8 +19190,11 @@
       <c r="K134" s="21" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L134" s="21" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -18152,8 +19225,11 @@
       <c r="K135" s="21" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L135" s="21" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -18184,8 +19260,11 @@
       <c r="K136" s="21" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L136" s="21" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -18216,8 +19295,11 @@
       <c r="K137" s="21" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L137" s="21" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -18248,8 +19330,11 @@
       <c r="K138" s="21" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L138" s="21" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -18280,8 +19365,11 @@
       <c r="K139" s="21" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L139" s="21" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -18312,8 +19400,11 @@
       <c r="K140" s="21" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L140" s="21" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -18344,8 +19435,11 @@
       <c r="K141" s="21" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L141" s="21" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -18376,8 +19470,11 @@
       <c r="K142" s="21" t="s">
         <v>915</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L142" s="21" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -18408,8 +19505,11 @@
       <c r="K143" s="21" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L143" s="21" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -18440,8 +19540,11 @@
       <c r="K144" s="21" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L144" s="21" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -18472,8 +19575,11 @@
       <c r="K145" s="21" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L145" s="21" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -18504,12 +19610,15 @@
       <c r="K146" s="21" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L146" s="21" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
       <c r="I147" s="8"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -18540,8 +19649,11 @@
       <c r="K148" s="21" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L148" s="21" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -18572,8 +19684,11 @@
       <c r="K149" s="21" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L149" s="21" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -18604,8 +19719,11 @@
       <c r="K150" s="21" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L150" s="21" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -18636,8 +19754,11 @@
       <c r="K151" s="21" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L151" s="21" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -18668,12 +19789,15 @@
       <c r="K152" s="21" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L152" s="21" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D153" s="4"/>
       <c r="I153" s="8"/>
     </row>
-    <row r="154" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
         <v>7</v>
       </c>
@@ -18701,12 +19825,15 @@
       <c r="K154" s="21" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L154" s="21" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D155" s="4"/>
       <c r="I155" s="8"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -18737,12 +19864,15 @@
       <c r="K156" s="20" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L156" s="20" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D157" s="4"/>
       <c r="I157" s="8"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>47</v>
       </c>
@@ -18770,8 +19900,11 @@
       <c r="K158" s="20" t="s">
         <v>927</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L158" s="21" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>47</v>
       </c>
@@ -18799,8 +19932,11 @@
       <c r="K159" s="20" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L159" s="20" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>47</v>
       </c>
@@ -18828,12 +19964,15 @@
       <c r="K160" s="20" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L160" s="20" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D161" s="4"/>
       <c r="I161" s="8"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>47</v>
       </c>
@@ -18864,8 +20003,11 @@
       <c r="K162" s="1" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L162" s="1" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -18896,8 +20038,11 @@
       <c r="K163" s="1" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L163" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -18928,8 +20073,11 @@
       <c r="K164" s="1" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L164" s="1" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>47</v>
       </c>
@@ -18960,8 +20108,11 @@
       <c r="K165" s="1" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L165" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -18992,8 +20143,11 @@
       <c r="K166" s="1" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L166" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>47</v>
       </c>
@@ -19024,8 +20178,11 @@
       <c r="K167" s="1" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L167" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>47</v>
       </c>
@@ -19056,8 +20213,11 @@
       <c r="K168" s="1" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L168" s="1" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>47</v>
       </c>
@@ -19088,8 +20248,11 @@
       <c r="K169" s="1" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L169" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -19120,8 +20283,11 @@
       <c r="K170" s="1" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L170" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>47</v>
       </c>
@@ -19152,8 +20318,11 @@
       <c r="K171" s="1" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L171" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>47</v>
       </c>
@@ -19184,8 +20353,11 @@
       <c r="K172" s="1" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L172" s="1" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>47</v>
       </c>
@@ -19216,8 +20388,11 @@
       <c r="K173" s="1" t="s">
         <v>941</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L173" s="1" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -19248,8 +20423,11 @@
       <c r="K174" s="1" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L174" s="1" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -19280,8 +20458,11 @@
       <c r="K175" s="1" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L175" s="1" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>47</v>
       </c>
@@ -19312,12 +20493,15 @@
       <c r="K176" s="1" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L176" s="1" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D177" s="4"/>
       <c r="I177" s="8"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>53</v>
       </c>
@@ -19345,22 +20529,27 @@
       <c r="K178" s="21" t="s">
         <v>945</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L178" s="21" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E179" s="13"/>
       <c r="H179" s="14"/>
       <c r="I179" s="16"/>
       <c r="J179" s="14"/>
       <c r="K179" s="21"/>
-    </row>
-    <row r="180" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L179" s="21"/>
+    </row>
+    <row r="180" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E180" s="13"/>
       <c r="H180" s="14"/>
       <c r="I180" s="16"/>
       <c r="J180" s="14"/>
       <c r="K180" s="21"/>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L180" s="21"/>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -19391,8 +20580,11 @@
       <c r="K181" s="18" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L181" s="18" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -19423,8 +20615,11 @@
       <c r="K182" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L182" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -19455,8 +20650,11 @@
       <c r="K183" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L183" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -19487,8 +20685,11 @@
       <c r="K184" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L184" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -19519,8 +20720,11 @@
       <c r="K185" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L185" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -19551,8 +20755,11 @@
       <c r="K186" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L186" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -19583,8 +20790,11 @@
       <c r="K187" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L187" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -19615,8 +20825,11 @@
       <c r="K188" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L188" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -19647,8 +20860,11 @@
       <c r="K189" s="18" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L189" s="18" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C190" s="8"/>
       <c r="D190" s="15"/>
       <c r="E190"/>
@@ -19657,7 +20873,7 @@
       <c r="I190" s="8"/>
       <c r="J190" s="18"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -19688,8 +20904,11 @@
       <c r="K191" s="1" t="s">
         <v>948</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L191" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -19720,8 +20939,11 @@
       <c r="K192" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L192" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -19752,8 +20974,11 @@
       <c r="K193" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L193" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -19784,8 +21009,11 @@
       <c r="K194" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L194" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -19816,8 +21044,11 @@
       <c r="K195" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L195" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -19848,8 +21079,11 @@
       <c r="K196" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L196" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -19880,8 +21114,11 @@
       <c r="K197" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L197" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -19912,8 +21149,11 @@
       <c r="K198" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L198" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -19944,14 +21184,17 @@
       <c r="K199" s="1" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L199" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C200" s="8"/>
       <c r="D200" s="15"/>
       <c r="E200"/>
       <c r="I200" s="8"/>
     </row>
-    <row r="201" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A201" s="8" t="s">
         <v>7</v>
       </c>
@@ -19979,14 +21222,17 @@
       <c r="K201" s="21" t="s">
         <v>950</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L201" s="21" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="D202" s="5"/>
       <c r="I202" s="8"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -20017,12 +21263,15 @@
       <c r="K203" s="20" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L203" s="20" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D204" s="5"/>
       <c r="I204" s="8"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>47</v>
       </c>
@@ -20050,8 +21299,11 @@
       <c r="K205" s="20" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L205" s="20" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>47</v>
       </c>
@@ -20079,8 +21331,11 @@
       <c r="K206" s="20" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L206" s="21" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>47</v>
       </c>
@@ -20108,8 +21363,11 @@
       <c r="K207" s="21" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L207" s="21" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>47</v>
       </c>
@@ -20137,12 +21395,15 @@
       <c r="K208" s="21" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L208" s="21" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D209" s="5"/>
       <c r="I209" s="8"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>53</v>
       </c>
@@ -20170,8 +21431,11 @@
       <c r="K210" s="21" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L210" s="21" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>53</v>
       </c>
@@ -20199,8 +21463,11 @@
       <c r="K211" s="21" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L211" s="21" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>53</v>
       </c>
@@ -20228,8 +21495,11 @@
       <c r="K212" s="21" t="s">
         <v>958</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L212" s="21" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>53</v>
       </c>
@@ -20257,8 +21527,11 @@
       <c r="K213" s="21" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L213" s="21" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>53</v>
       </c>
@@ -20286,8 +21559,11 @@
       <c r="K214" s="20" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L214" s="21" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>53</v>
       </c>
@@ -20315,8 +21591,11 @@
       <c r="K215" s="20" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L215" s="21" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>53</v>
       </c>
@@ -20344,8 +21623,11 @@
       <c r="K216" s="21" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L216" s="21" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>53</v>
       </c>
@@ -20373,8 +21655,11 @@
       <c r="K217" s="21" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L217" s="21" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>53</v>
       </c>
@@ -20402,8 +21687,11 @@
       <c r="K218" s="21" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L218" s="21" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>53</v>
       </c>
@@ -20431,22 +21719,27 @@
       <c r="K219" s="20" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L219" s="21" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E220" s="13"/>
       <c r="H220" s="14"/>
       <c r="I220" s="16"/>
       <c r="J220" s="14"/>
       <c r="K220" s="21"/>
-    </row>
-    <row r="221" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L220" s="21"/>
+    </row>
+    <row r="221" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E221" s="13"/>
       <c r="H221" s="14"/>
       <c r="I221" s="16"/>
       <c r="J221" s="14"/>
       <c r="K221" s="21"/>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L221" s="21"/>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -20477,8 +21770,11 @@
       <c r="K222" s="20" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L222" s="21" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -20509,8 +21805,11 @@
       <c r="K223" s="21" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L223" s="21" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -20541,8 +21840,11 @@
       <c r="K224" s="21" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L224" s="21" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -20573,8 +21875,11 @@
       <c r="K225" s="20" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L225" s="21" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -20605,12 +21910,15 @@
       <c r="K226" s="20" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L226" s="21" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D227" s="6"/>
       <c r="I227" s="8"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>7</v>
       </c>
@@ -20641,8 +21949,11 @@
       <c r="K228" s="20" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L228" s="21" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>7</v>
       </c>
@@ -20673,8 +21984,11 @@
       <c r="K229" s="21" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L229" s="21" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>7</v>
       </c>
@@ -20705,8 +22019,11 @@
       <c r="K230" s="20" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L230" s="21" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>7</v>
       </c>
@@ -20737,12 +22054,15 @@
       <c r="K231" s="20" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L231" s="21" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D232" s="6"/>
       <c r="I232" s="8"/>
     </row>
-    <row r="233" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A233" s="8" t="s">
         <v>7</v>
       </c>
@@ -20770,12 +22090,15 @@
       <c r="K233" s="21" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L233" s="21" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D234" s="6"/>
       <c r="I234" s="8"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>7</v>
       </c>
@@ -20803,12 +22126,15 @@
       <c r="K235" s="21" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L235" s="21" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D236" s="6"/>
       <c r="I236" s="8"/>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>47</v>
       </c>
@@ -20833,8 +22159,11 @@
       <c r="K237" s="21" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L237" s="21" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>47</v>
       </c>
@@ -20859,8 +22188,11 @@
       <c r="K238" s="21" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L238" s="21" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>47</v>
       </c>
@@ -20885,12 +22217,15 @@
       <c r="K239" s="21" t="s">
         <v>977</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L239" s="21" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D240" s="6"/>
       <c r="I240" s="8"/>
     </row>
-    <row r="241" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>47</v>
       </c>
@@ -20915,12 +22250,15 @@
       <c r="K241" s="21" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L241" s="21" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D242" s="6"/>
       <c r="I242" s="8"/>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>53</v>
       </c>
@@ -20945,22 +22283,27 @@
       <c r="K243" s="21" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L243" s="21" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E244" s="13"/>
       <c r="H244" s="14"/>
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
       <c r="K244" s="14"/>
-    </row>
-    <row r="245" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L244" s="14"/>
+    </row>
+    <row r="245" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E245" s="13"/>
       <c r="H245" s="14"/>
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
       <c r="K245" s="14"/>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L245" s="14"/>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>7</v>
       </c>
@@ -20991,12 +22334,16 @@
       <c r="K246" s="1" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L246" s="1" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D247" s="7"/>
       <c r="K247" s="1"/>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L247" s="1"/>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>7</v>
       </c>
@@ -21027,8 +22374,11 @@
       <c r="K248" s="1" t="s">
         <v>981</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L248" s="1" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>7</v>
       </c>
@@ -21059,8 +22409,11 @@
       <c r="K249" s="1" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L249" s="1" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>7</v>
       </c>
@@ -21091,8 +22444,11 @@
       <c r="K250" s="1" t="s">
         <v>983</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L250" s="1" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>7</v>
       </c>
@@ -21123,12 +22479,16 @@
       <c r="K251" s="1" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L251" s="1" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D252" s="7"/>
       <c r="K252" s="1"/>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L252" s="1"/>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>7</v>
       </c>
@@ -21159,12 +22519,16 @@
       <c r="K253" s="1" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L253" s="1" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D254" s="7"/>
       <c r="K254" s="1"/>
-    </row>
-    <row r="255" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L254" s="1"/>
+    </row>
+    <row r="255" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>47</v>
       </c>
@@ -21192,8 +22556,11 @@
       <c r="K255" s="1" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L255" s="1" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>47</v>
       </c>
@@ -21221,8 +22588,11 @@
       <c r="K256" s="1" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L256" s="1" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>47</v>
       </c>
@@ -21250,8 +22620,11 @@
       <c r="K257" s="1" t="s">
         <v>988</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L257" s="1" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>47</v>
       </c>
@@ -21279,12 +22652,16 @@
       <c r="K258" s="1" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L258" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D259" s="7"/>
       <c r="K259" s="1"/>
-    </row>
-    <row r="260" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L259" s="1"/>
+    </row>
+    <row r="260" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>53</v>
       </c>
@@ -21312,22 +22689,27 @@
       <c r="K260" s="1" t="s">
         <v>990</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L260" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E261" s="13"/>
       <c r="H261" s="14"/>
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
       <c r="K261" s="14"/>
-    </row>
-    <row r="262" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L261" s="14"/>
+    </row>
+    <row r="262" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E262" s="13"/>
       <c r="H262" s="14"/>
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
       <c r="K262" s="14"/>
-    </row>
-    <row r="263" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L262" s="14"/>
+    </row>
+    <row r="263" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>7</v>
       </c>
@@ -21355,11 +22737,15 @@
       <c r="K263" s="1" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L263" s="1" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D264" s="9"/>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L264" s="1"/>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>7</v>
       </c>
@@ -21387,12 +22773,16 @@
       <c r="K265" s="1" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L265" s="1" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D266" s="9"/>
       <c r="K266" s="1"/>
-    </row>
-    <row r="267" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L266" s="1"/>
+    </row>
+    <row r="267" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A267" s="8" t="s">
         <v>7</v>
       </c>
@@ -21420,14 +22810,18 @@
       <c r="K267" s="1" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L267" s="1" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="D268" s="9"/>
       <c r="K268" s="1"/>
-    </row>
-    <row r="269" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L268" s="1"/>
+    </row>
+    <row r="269" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>7</v>
       </c>
@@ -21455,12 +22849,16 @@
       <c r="K269" s="1" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L269" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D270" s="9"/>
       <c r="K270" s="1"/>
-    </row>
-    <row r="271" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L270" s="1"/>
+    </row>
+    <row r="271" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>47</v>
       </c>
@@ -21485,8 +22883,11 @@
       <c r="K271" s="1" t="s">
         <v>995</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L271" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>47</v>
       </c>
@@ -21511,8 +22912,11 @@
       <c r="K272" s="1" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L272" s="1" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>47</v>
       </c>
@@ -21537,8 +22941,11 @@
       <c r="K273" s="1" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L273" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>47</v>
       </c>
@@ -21563,12 +22970,16 @@
       <c r="K274" s="1" t="s">
         <v>998</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L274" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D275" s="9"/>
       <c r="K275" s="1"/>
-    </row>
-    <row r="276" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L275" s="1"/>
+    </row>
+    <row r="276" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>53</v>
       </c>
@@ -21593,22 +23004,27 @@
       <c r="K276" s="1" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L276" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E277" s="13"/>
       <c r="H277" s="14"/>
       <c r="I277" s="14"/>
       <c r="J277" s="14"/>
       <c r="K277" s="14"/>
-    </row>
-    <row r="278" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L277" s="14"/>
+    </row>
+    <row r="278" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E278" s="13"/>
       <c r="H278" s="14"/>
       <c r="I278" s="14"/>
       <c r="J278" s="14"/>
       <c r="K278" s="14"/>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L278" s="14"/>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>7</v>
       </c>
@@ -21636,12 +23052,16 @@
       <c r="K279" s="1" t="s">
         <v>1000</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L279" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D280" s="10"/>
       <c r="K280" s="1"/>
-    </row>
-    <row r="281" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L280" s="1"/>
+    </row>
+    <row r="281" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>7</v>
       </c>
@@ -21669,12 +23089,16 @@
       <c r="K281" s="1" t="s">
         <v>1001</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L281" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D282" s="10"/>
       <c r="K282" s="1"/>
-    </row>
-    <row r="283" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L282" s="1"/>
+    </row>
+    <row r="283" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>7</v>
       </c>
@@ -21702,12 +23126,16 @@
       <c r="K283" s="1" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L283" s="1" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D284" s="10"/>
       <c r="K284" s="1"/>
-    </row>
-    <row r="285" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L284" s="1"/>
+    </row>
+    <row r="285" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>7</v>
       </c>
@@ -21735,12 +23163,16 @@
       <c r="K285" s="1" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L285" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D286" s="10"/>
       <c r="K286" s="1"/>
-    </row>
-    <row r="287" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L286" s="1"/>
+    </row>
+    <row r="287" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>47</v>
       </c>
@@ -21765,8 +23197,11 @@
       <c r="K287" s="1" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L287" s="1" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>47</v>
       </c>
@@ -21791,8 +23226,11 @@
       <c r="K288" s="1" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L288" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>47</v>
       </c>
@@ -21817,8 +23255,11 @@
       <c r="K289" s="1" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L289" s="1" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>47</v>
       </c>
@@ -21843,12 +23284,16 @@
       <c r="K290" s="1" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L290" s="1" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D291" s="10"/>
       <c r="K291" s="1"/>
-    </row>
-    <row r="292" spans="1:11" ht="19" x14ac:dyDescent="0.3">
+      <c r="L291" s="1"/>
+    </row>
+    <row r="292" spans="1:12" ht="19" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>53</v>
       </c>
@@ -21872,6 +23317,9 @@
       </c>
       <c r="K292" s="1" t="s">
         <v>1008</v>
+      </c>
+      <c r="L292" s="1" t="s">
+        <v>1223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and tested Vietnamese snuggets
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets.xlsx
+++ b/disasterinfosite/data/snuggets.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="1443">
   <si>
     <t>section</t>
   </si>
@@ -13211,12 +13211,729 @@
   <si>
     <t>text-so</t>
   </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG CAO&lt;/b&gt; (84%) là sẽ có một trận động đất có cường độ 6.5+ xảy ra trong 50 năm tới. Nó sẽ có cảm giác tương tự như trận động đất Nisqually M6.8 xảy ra vào năm 2001. Gần như tất cả mọi người ở đây đều cảm nhận được rung chấn trung bình. &lt;b&gt;Cửa sẽ đu đưa&amp;#44; tranh treo trên tường sẽ rung lắc và các đồ vật nhỏ có thể rơi xuống. Thiệt hại nhẹ.&lt;/b&gt;  &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG CAO&lt;/b&gt; (84%) là sẽ có một trận động đất có cường độ 6.5+ xảy ra trong 50 năm tới. Nó sẽ có cảm giác tương tự như trận động đất Nisqually M6.8 xảy ra vào năm 2001. &lt;b&gt;Rung chấn mạnh sẽ khiến việc đi bộ tại đây trở nên khó khăn. Sách vở&amp;#44; đồ thuỷ tinh và các đồ vật sẽ rơi từ trên giá xuống. Cửa tủ và ngăn kéo sẽ bị mở tung&lt;/b&gt;. Một số ống khói và công trình xây dựng yếu kém sẽ bị hư hại. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG CAO&lt;/b&gt; (84%) là sẽ có một trận động đất có cường độ 6.5+ xảy ra trong 50 năm tới. Nó sẽ có cảm giác tương tự như trận động đất Nisqually M6.8 xảy ra vào năm 2001. &lt;b&gt;Rung chấn cực mạnh sẽ khiến việc đứng vững trở nên khó khăn. Đồ nội thất sẽ di chuyển và nhiều đồ vật sẽ rơi từ trên giá sách xuống.&lt;/b&gt; Các công trình xây dựng yếu kém sẽ bị hư hại nặng nề và các công trình bình thường sẽ bị hư hại ở mức trung bình. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Nisqually.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG THẤP&lt;/b&gt; (5%) là sẽ có một trận động đất với cường độ 7+ xảy ra tại Phay Seattle trong 50 năm tới&amp;#44; nhưng nếu nó xảy ra&amp;#44; sức tàn phá sẽ rất lớn. &lt;b&gt;Gần như tất cả mọi người sẽ cảm nhận được rung chấn vừa phải. Cửa sẽ đu đưa&amp;#44; tranh treo trên tường sẽ rung lắc và các đồ vật nhỏ có thể rơi xuống. Thiệt hại nhẹ.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG THẤP&lt;/b&gt; (5%) là sẽ có một trận động đất với cường độ 7+ xảy ra tại Phay Seattle trong 50 năm tới&amp;#44; nhưng nếu nó xảy ra&amp;#44; sức tàn phá sẽ rất lớn. Rung chấn mạnh sẽ khiến việc đi bộ khó khăn. &lt;b&gt;Sách vở&amp;#44; đồ thuỷ tinh và các đồ vật sẽ rơi từ trên giá xuống. Một số ống khói và công trình xây dựng yếu kém sẽ bị hư hại.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG THẤP&lt;/b&gt; (5%) là sẽ có một trận động đất với cường độ 7+ xảy ra tại Phay Seattle trong 50 năm tới&amp;#44; nhưng nếu nó xảy ra&amp;#44; sức tàn phá sẽ rất lớn. &lt;b&gt;Rung chấn mạnh sẽ khiến việc đứng vững trở nên khó khăn. Đồ nội thất sẽ di chuyển và đồ vật sẽ bị rơi&lt;/b&gt;. Các công trình xây dựng yếu kém sẽ bị hư hại nặng và các công trình bình thường sẽ bị hư hại ở mức trung bình. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(bản đồ) &lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG THẤP&lt;/b&gt; (5%) là sẽ có một trận động đất với cường độ 7+ xảy ra tại Phay Seattle trong 50 năm tới&amp;#44; nhưng nếu nó xảy ra&amp;#44; sức tàn phá sẽ rất lớn. &lt;b&gt;Rung chấn nghiêm trọng sẽ khiến việc đứng vững hay lái xe trở nên khó khăn. Các đồ nội thất nặng sẽ bị xáo trộn. Các phần của những công trình &lt;a href="http://www.seattle.gov/dpd/codesrules/changestocode/unreinforcedmasonrybuildings/whatwhy/" target=_blank&gt;URM&lt;/a&gt; sẽ sập và những ngôi nhà có khung gỗ sẽ dịch chuyển trên móng&lt;/b&gt;. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG THẤP&lt;/b&gt; (5%) là sẽ có một trận động đất với cường độ 7+ xảy ra tại Phay Seattle trong 50 năm tới&amp;#44; nhưng nếu nó xảy ra&amp;#44; sức tàn phá sẽ rất lớn. &lt;b&gt;Rung chấn mãnh liệt sẽ gây hoảng loạn trên diện rộng và các vết nứt có thể hình thành trên mặt đất. Sạt lở đất sẽ xảy ra trên các sườn núi dốc và hiện tượng hoá lỏng đất sẽ xảy ra đối với đất bão hoà.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target=_blank&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct" title="Seattle Viaduct Visualization Screen Grab"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG TRUNG BÌNH&lt;/b&gt; (10-30%) là sẽ có một trận động đất Cascadia với cường độ 8+ xảy ra tại khu vực Tây Bắc trong 50 năm tới. &lt;b&gt;Khi một trận động đất như vậy xảy ra&amp;#44; bạn sẽ cảm thấy rung chấn trung bình kéo dài trong nhiều phút tại đây. Các đồ vật không được cố định sẽ rơi từ trên giá xuống. Cửa tủ có thể va đập đóng&amp;#44; mở liên tục.&lt;/b&gt; Có thể bị mất điện và nước trong vài ngày cho tới vài tuần. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG TRUNG BÌNH&lt;b&gt; (10-30%) là sẽ có một trận động đất Cascadia với cường độ 8+ xảy ra tại khu vực Tây Bắc trong 50 năm tới. &lt;b&gt;Khi một trận động đất như vậy xảy ra&amp;#44; bạn sẽ cảm thấy sự rung lắc mạnh kéo dài trong nhiều phút. Việc đi bộ sẽ trở nên khó khăn. Nhiều công trình xây dựng không có cốt thép sẽ bị hư hại và con người có thể bị thương&lt;/b&gt;. Sẽ mất điện và nước trong vài ngày cho tới vài tuần. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Có &lt;b&gt;KHẢ NĂNG TRUNG BÌNH&lt;/b&gt; (10-30%) là sẽ có một trận động đất Cascadia với cường độ 8+ xảy ra tại khu vực Tây Bắc trong 50 năm tới. &lt;b&gt;Khi một trận động đất như vậy xảy ra&amp;#44; bạn sẽ cảm thấy rung chấn cực mạnh kéo dài trong nhiều phút tại đây. Khó có thể đứng vững được và nhiều người sẽ bị thương. Gạch và mảnh vụn thuỷ tinh sẽ rơi đầy đường.&lt;/b&gt; Sẽ mất điện và nước trong vài ngày cho tới vài tuần. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Cascadia.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Bạn sống tại khu vực &lt;b&gt;có nguy cơ xảy ra sóng thần CAO&lt;/b&gt;. Mực nước sẽ dâng cao trên đầu bạn trong vài phút hoặc vài chục phút sau khi động đất xảy ra. Khi rung chấn ngừng&amp;#44; NGAY LẬP TỨC DI TẢN lên vùng đất cao. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Bạn sống tại khu vực &lt;b&gt;có nguy cơ xảy ra sóng thần CAO&lt;/b&gt;. Mực nước sẽ dâng cao trên đầu gối cho tới đầu bạn trong vài phút hoặc vài chục phút sau khi động đất xảy ra. Khi rung chấn ngừng&amp;#44; NGAY LẬP TỨC DI TẢN lên vùng đất cao. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Bạn sống tại &lt;b&gt;khu vực có nguy cơ xảy ra sóng thần CAO&lt;/b&gt;. Mực nước sẽ dâng lên tới đầu gối bạn với tốc độ dòng nước nhanh đến mức có thể quật ngã bạn. Bạn có vài phút tới vài chục phút để DI TẢN đến vùng đất cao. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Bạn sống ngoài khu vực được đánh dấu trên bản đồ là có nguy cơ cao xảy ra sóng thần&lt;/b&gt;&amp;#44; nhưng những con sóng thần có thể thiên biến vạn hoá. Bạn sống hoặc làm việc tại khu vực có độ cao thấp (trong vòng 30 ft so với mặt nước biển) gần biển phải không? Nếu đúng vậy&amp;#44; NGAY LẬP TỨC DI TẢN tới vùng đất cao sau khi trận động đất lớn xảy ra. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Bạn sống chỉ cách bờ biển một phần tư dặm&lt;/b&gt;. Nếu bạn sống tại khu vực có độ cao thấp (trong vòng 30 ft so với mặt nước biển)&amp;#44; thì bạn có nguy cơ bị sóng thần tấn công sau khi một trận động đất xảy ra gần đó. Ngay lập tức tìm kiếm vùng đất cao. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Nếu bạn đang ở trên thuyền trong một trận động đất&amp;#44; bạn có thể thấy một cơn sóng thần di chuyển với tốc độ nhanh chóng. Đưa ra hành động theo đó. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: CAO&lt;/b&gt;&lt;br&gt;Đất khi rung lắc sẽ trở nên rất không ổn định và hoạt động giống cát lún. Nước chứa đầy cát sẽ dâng lên qua các vết nức trên đường phố. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: TRUNG BÌNH - CAO&lt;/b&gt;&lt;br&gt;Đất khi rung lắc sẽ trở nên không ổn định. Hiện tượng này sẽ làm giảm khả năng của đất trong việc giữ nhà cửa&amp;#44; phương tiện và các cấu trúc khác. Nước chứa đầy cát sẽ dâng lên qua các vết nức trên đường phố. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: THẤP - TRUNG BÌNH&lt;/b&gt;&lt;br&gt;Hiện tượng hoá lỏng đất có khả năng sẽ xảy ra tại đây. Việc rung lắc có thể khiến đất trở nên không ổn định. Các con đường có thể rạn nứt và bị hư hại. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: THẤP&lt;/b&gt;&lt;br&gt;Trừ khi rung chấn có cường độ mạnh&amp;#44; nếu không có rất ít khả năng xảy ra hiện tượng hoá lỏng đất tại đây. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: RẤT THẤP - THẤP&lt;/b&gt;&lt;br&gt;Trừ khi rung chấn có cường độ rất mạnh&amp;#44; nếu không có rất ít khả năng xảy ra hiện tượng hoá lỏng đất tại đây. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: RẤT THẤP&lt;/b&gt;&lt;br&gt;Trừ khi rung chấn có cường độ rất mạnh&amp;#44; nếu không có rất ít khả năng xảy ra hiện tượng hoá lỏng đất tại đây. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: KHÔNG&lt;/b&gt;&lt;br&gt;Khu vực này nằm trên vùng đá gốc&amp;#44; đá cứng nằm dưới lớp đất và trầm tích. Khu vực này sẽ không xảy ra hiện tượng hoá lỏng đất. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: KHÔNG&lt;/b&gt;&lt;br&gt;Khu vực này nằm trên than bùn&amp;#44; một chất giống như đất có màu đen hình thành từ các vật chất hữu cơ. Đất có thể uốn lượn nhưng không bị hoá lỏng. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khả năng: KHÔNG&lt;/b&gt;&lt;br&gt;Khu vực này hình thành từ băng và sẽ không bị hoá lỏng. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_liquefaction.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;MẬT ĐỘ RẤT THẤP: 0 đến 10 công trình xây dựng không có cốt thép (URM) trên một dặm vuông.&lt;/b&gt;&lt;br&gt;Đối với loại công trình này&amp;#44; rung chấn động đất mạnh có thể khiến các bức tường gạch hoặc mái nhà bị sập. Đống đổ nát vương vãi đầy đường. Xem vị trí của các công trình URM &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;gần bạn nhất&lt;/a&gt; và liệu rằng chúng có được lắp đặt thêm gì mới không. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MẬT ĐỘ THẤP: 10 đến 25 công trình xây dựng không có cốt thép (URM) trên một dặm vuông.&lt;/b&gt;&lt;br&gt;Đối với loại công trình này&amp;#44; rung chấn động đất mạnh có thể khiến các bức tường gạch hoặc mái nhà bị sập. Đống đổ nát vương vãi đầy đường. Xem vị trí của các công trình URM &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;gần bạn nhất&lt;/a&gt; và liệu rằng chúng có được lắp đặt thêm gì mới không. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MẬT ĐỘ TRUNG BÌNH: 25 đến 50 công trình xây dựng không có cốt thép (URM) trên một dặm vuông.&lt;/b&gt;&lt;br&gt;Đối với loại công trình này&amp;#44; rung chấn động đất mạnh có thể khiến các bức tường gạch hoặc mái nhà bị sập. Đống đổ nát vương vãi đầy đường. Xem vị trí của các công trình URM &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;gần bạn nhất&lt;/a&gt; và liệu rằng chúng có được lắp đặt thêm gì mới không. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MẬT ĐỘ CAO: 50 đến 100 công trình xây dựng không có cốt thép (URM) trên một dặm vuông.&lt;/b&gt;&lt;br&gt;Nếu bạn ở trong một công trình URM khi một trận động đất diễn ra&amp;#44; hãy làm theo quy tắc Cúi Thấp&amp;#44; Bảo Vệ Đầu và Cơ Thể&amp;#44; và Bám Chặt. Trong các công trình này&amp;#44; rung lắc động đất mạnh có thể khiến tường gạch và mái nhà bị sập. Đống đổ nát vương vãi đầy đường. Xem vị trí của các công trình URM &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;gần bạn nhất&lt;/a&gt; và liệu rằng chúng có được lắp đặt thêm gì mới không. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MẬT ĐỘ RẤT CAO: 100 đến 250 công trình xây dựng không có cốt thép (URM) trên một dặm vuông.&lt;/b&gt;&lt;br&gt;Nếu bạn ở trong một công trình URM khi một trận động đất diễn ra&amp;#44; hãy làm theo quy tắc Cúi Thấp&amp;#44; Bảo Vệ Đầu và Cơ Thể&amp;#44; và Bám Chặt. Trong các công trình này&amp;#44; rung lắc động đất mạnh có thể khiến tường gạch và mái nhà bị sập. Đống đổ nát vương vãi đầy đường. Xem vị trí của các công trình URM &lt;a href=http://seattlecitygis.maps.arcgis.com/apps/MapSeries/index.html?appid=0489a95dad4e42148dbef571076f9b5b target=_blank&gt;gần bạn nhất&lt;/a&gt; và liệu rằng chúng có được lắp đặt thêm gì mới không. &lt;a href=https://hazardready.org/seattle/static/img/data/Earthquake_URM.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Các nhà khoa học không thể tiên lượng được khi nào thì một trận động đất sẽ xảy ra&amp;#44; vì vậy hãy cảnh giác và nếu bạn cảm nhận thấy có rung lắc&amp;#44; hãy làm theo quy tắc cúi thấp&amp;#44; bảo vệ đầu và cơ thể&amp;#44; và bám chặt. Một hệ thống cảnh báo sớm hiện đang được phát triển cho khu vực Bờ Tây (West Coast). Bạn có thể tìm hiểu thêm &lt;a href=http://earthquake.usgs.gov/research/earlywarning/ target="_blank"&gt;tại đây&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;THỰC HÀNH&lt;/b&gt; - Cảnh giác và thực hành "Cúi Thấp&amp;#44; Bảo Vệ Đầu và Cơ Thể&amp;#44; và Bám Chặt"&lt;/li&gt;&lt;li&gt;&lt;b&gt;KẾ HOẠCH&lt;/b&gt; - Lập một kế hoạch (&lt;a href=http://www.fema.gov/media-library-data/0e3ef555f66e22ab832e284f826c2e9e/FEMA_plan_parent_508_071513.pdf target="_blank"&gt;cho người lớn&lt;/a&gt; &amp;amp; &lt;a href=http://www.fema.gov/media-library-data/a260e5fb242216dc62ae380946806677/FEMA_plan_child_508_071513.pdf target="_blank"&gt;cho trẻ em&lt;/a&gt;) và chuẩn bị một &lt;a href=http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf target="_blank"&gt;bộ vật dụng cần thiết&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;CHUẨN BỊ&lt;/b&gt; - Cố định các đồ vật có thể bị rơi và biết vị trí tắt các tiện ích sinh hoạt&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;Ở TRONG NHÀ - Ở NGUYÊN ĐÓ!&lt;/b&gt; Hãy núp dưới một chiếc bàn vững chắc hoặc bàn ở cách xa các đồ vật có thể đổ lên người bạn và bám chặt. ĐỪNG chạy ra ngoài trước khi ngừng rung chấn.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Ở NGOÀI TRỜI - ĐẾN NƠI THOÁNG ĐÃNG&lt;/b&gt; ở cách xa các toà nhà&amp;#44; đường dây điện&amp;#44; ống khói hoặc những thứ có thể đổ lên người bạn.&lt;/li&gt;&lt;li&gt;&lt;b&gt;ĐANG LÁI XE - CẨN THẬN DỪNG XE LẠI&lt;/b&gt; (không dừng dưới cầu&amp;#44; cầu vượt&amp;#44; đường dây điện&amp;#44; v.v.) và Ở NGUYÊN TRONG PHƯƠNG TIỆN.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Ở GẦN BIỂN&lt;/b&gt; - Làm theo các hướng dẫn trên cho tới khi rung chấn ngừng. Sau đó &lt;b&gt;DI CHUYỂN TỚI VÙNG ĐẤT CAO&lt;/b&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/EQ_during.jpg" alt="This is a panel of four cartoon images showing what to do during an earthquake if inside&amp;#44; outside&amp;#44; driving&amp;#44; or near the ocean." title="During Earthquake Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;CHUẨN BỊ CHO DƯ CHẤN&lt;/b&gt; (các trận động đất xảy ra sau trận động đất chính khá phổ biến và có thể gây ra thiệt hại lớn hơn so với trận động đất đầu tiên).&lt;ul&gt;&lt;li&gt;Các đường dây điện thoại sẽ bị quá tải; &lt;b&gt;nhắn tin có thể là một phương pháp hiệu quả để liên lạc với gia đình.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;Kiểm tra bản thân và những người khác xem có ai bị thương không.&lt;/li&gt;&lt;li&gt;Khi đã an toàn&amp;#44; &lt;b&gt;xem các bản tin&lt;/b&gt; qua đài chạy pin&amp;#44; vô tuyến&amp;#44; mạng xã hội&amp;#44; và cảnh báo tin nhắn qua điện thoại để biết các thông tin khẩn cấp.&lt;/li&gt;&lt;li&gt;Lực lượng phản ứng khẩn cấp sẽ bận rộn. &lt;b&gt;Dựa vào bạn bè và hàng xóm &lt;/b&gt; để được hỗ trợ trong vài giờ hoặc vài ngày sau động đất.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Kiểm soát các tiện ích sinh hoạt nếu cần&lt;/b&gt;. Tìm hiểu thêm về thời gian và cách &lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target="_blank"&gt;kiểm soát khí ga và nước sau khi động xảy ra&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Morgan Junction Park Hub &lt;br&gt;Vị Trí của Trung Tâm: At Morgan Junction Park&amp;#44; &lt;br&gt;6413 California Ave SW&amp;#44; Seattle&amp;#44; WA 98118 &lt;br&gt;Người Đứng Đầu Trung Tâm: Cindi Barker&lt;br&gt;Email: &lt;a href="mailto:cindiLbarker@gmail.com" target="_top"&gt;cindiLbarker@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-933-6968&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/west-seattle/" target=_blank&gt;http://seattleemergencyhubs.org/west-seattle&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;North Highland Park Hub &lt;br&gt;Vị Trí của Trung Tâm: The Highland Park Improvement Club &lt;br&gt;1116 SW Holden St&lt;br&gt;Người Đứng Đầu Trung Tâm:Cần Tuyển Tình Nguyện Viên &lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;South Park Neighborhood Center &lt;br&gt;Vị Trí của Trung Tâm: 8201 10th Ave S&lt;br&gt;Người Đứng Đầu Trung Tâm: Dagmar Cronn&lt;br&gt;Email: &lt;a href="mailto:cronn@oakland.edu" target="_top"&gt;cronn@oakland.edu&lt;/a&gt;&lt;br&gt;Điện thoại: 206-327-1828&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt; &lt;br&gt;description: Meet by the blue box in the park&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Pigeon Point Hub &lt;br&gt;Vị Trí của Trung Tâm: The intersection of 20th Ave SW &amp; SW Genesee St&amp;#44; Seattle&amp;#44; WA 98106 &lt;br&gt;NW corner of the Park&amp;#44; just north of the school.&lt;br&gt;Người Đứng Đầu Trung Tâm: Wade Harper&lt;br&gt;Email: &lt;a href="mailto:wade.harper@outlook.com" target="_top"&gt;wade.harper@outlook.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-455-5407&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Hiawatha Playfield/Community Center (Admiral Hub) &lt;br&gt;Vị Trí của Trung Tâm: At California Ave SW &amp; SW Lander St&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Người Đứng Đầu Trung Tâm: Paul Stancik&lt;br&gt;Email: &lt;a href="mailto:pstancik@mindspring.com" target="_top"&gt;pstancik@mindspring.com&lt;/a&gt;&lt;br&gt;Điện thoại:TBD &lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Fauntleroy Church Hub &lt;br&gt;Vị Trí của Trung Tâm: Fauntleroy Church&amp;#44; 9140 California Ave SW&lt;br&gt;Người Đứng Đầu Trung Tâm: Gordon Wiehler&lt;br&gt;Email:: &lt;a href="mailto:gmwinv@Comcast.net" target="_top"&gt;gmwinv@Comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại:: 206-577-4292&lt;br&gt;Trang web:&lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Providence/Mount St. Vincent&amp;#44; parking lot (Fairmount Hub) &lt;br&gt;Vị Trí của Trung Tâm: At SW Hudson St &amp; 35th Ave SW&amp;#44; Seattle&amp;#44; WA 98126 &lt;br&gt; (meet at the SE parking lot under the flag pole )&lt;br&gt;Người Đứng Đầu Trung Tâm: Sharonn Meeks&lt;br&gt;Email: &lt;a href="mailto:smeeks50@comcast.net" target="_top"&gt;smeeks50@comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại: 206-938-1007&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Neighborhood House (High Point Hub) &lt;br&gt;Vị Trí của Trung Tâm: At 6400 Sylvan Way SW (note that east of 35th Ave SW&amp;#44; SW Morgan Street becomes Sylvan Way SW). Neighborhood House is next to Lanham Place SW. Meet at the amphitheater. &lt;br&gt;Người Đứng Đầu Trung Tâm: Heather Hutchison&lt;br&gt;Email: &lt;a href="mailto:heather.hutchison@manage" target="_top"&gt;heather.hutchison@manage&lt;/a&gt;&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Ercolini Park Hub &lt;br&gt;Vị Trí của Trung Tâm: At 48th Ave SW &amp; SW Alaska St.&amp;#44; in the park&lt;br&gt;Người Đứng Đầu Trung Tâm: Jon Wright&lt;br&gt;Email:&lt;a href="mailto:ercolini@westseattlebeprepared.org" target="_top"&gt;ercolini@westseattlebeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;EC Hughes Playground (Olympic Heights Hub) &lt;br&gt;Vị Trí của Trung Tâm: At 29th Ave SW &amp; SW Holden St&amp;#44; Seattle&amp;#44; WA 98126&amp;#44; at the NE corner of Hughes Playground.&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Salvation Army&amp;#44; parking lot (South Highland Park Hub) &lt;br&gt;Vị Trí của Trung Tâm: At 9050 16th Ave SW (near SW Barton St.)&amp;#44; the Salvation Army parking lot is the gathering place for this hub.&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên &lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;North Delridge P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: At the P-Patch&amp;#44; located at 5078 25th Ave SW&amp;#44; Seattle&amp;#44; WA&lt;br&gt;Người Đứng Đầu Trung Tâm: Jay McNally&lt;br&gt;Email: &lt;a href="mailto:Newcarissa@gmail.com" target="_top"&gt;Newcarissa@gmail.com &lt;/a&gt;&lt;br&gt;Điện thoại: 206-484-6613&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Hope Lutheran Church (Alaska Junction Hub) &lt;br&gt;Vị Trí của Trung Tâm: 4456 42nd Ave SW&amp;#44; Seattle&amp;#44; WA 98116&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Alki Community Center (Alki Hub) &lt;br&gt;Vị Trí của Trung Tâm: At 59th Ave SW &amp; SW Stevens St&amp;#44; Seattle&amp;#44; WA 98116. This is adjacent to Whale Tail Park&amp;#44; near the west edge of the playfield. North side of Alki Playfield&lt;br&gt;Người Đứng Đầu Trung Tâm: Tony Fragada (98126)&lt;br&gt;Email: &lt;a href="mailto:tfragada@yahoo.com" target="_top"&gt;tfragada@yahoo.com&lt;/a&gt; &lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://westseattlebeprepared.org/" target=_blank&gt;http://westseattlebeprepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Maa Nyei Lai Ndeic P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 4913 Columbia Dr S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Người Đứng Đầu Trung Tâm: Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Hillman City P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 4613 S Lucile St&amp;#44; Seattle&amp;#44; WA 98118 (Corner of South Lucile &amp; 46th Ave South)&lt;br&gt;Người Đứng Đầu Trung Tâm: Joanne Tilton&lt;br&gt;Email: &lt;a href="mailto:Jtilton22@comcast.net" target="_top"&gt;Jtilton22@comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại: 206-650-2071&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Judkins P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 24th Avenue S &amp; S Norman Street Seattle&amp;#44; WA 98112 (Meeting Location: P-Patch entrance off Norman &amp; 24th Ave S.)&lt;br&gt;Người Đứng Đầu Trung Tâm: Jen Ellis&lt;br&gt;Email:   &lt;a href="mailto:JenniferEllis.206@gmail.com" target="_top"&gt;JenniferEllis.206@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-276-4982&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Fisher Pavilion Hub &lt;br&gt;Vị Trí của Trung Tâm: 2nd Ave N &amp; Thomas St&lt;br&gt;Người Đứng Đầu Trung Tâm: MIQA Be Prepared&lt;br&gt;Email:  &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web:  &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Interbay Fishermen's Terminal Hub &lt;br&gt;Vị Trí của Trung Tâm: Interbay Fishermen's Terminal&lt;br&gt;Người Đứng Đầu Trung Tâm: MIQA Be Prepared&lt;br&gt;Email: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Eastlake Hub &lt;br&gt;Vị Trí của Trung Tâm: Rogers Playfield&lt;br&gt;Người Đứng Đầu Trung Tâm: Amy O'Donnell&lt;br&gt;Email:  &lt;a href="mailto:eastlake.hub@gmail.com" target="_top"&gt;eastlake.hub@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Madison Park Hub &lt;br&gt;Vị Trí của Trung Tâm: 42nd Ave E and E Howe St (at the north side of tennis courts)&lt;br&gt;Người Đứng Đầu Trung Tâm: John Madrid&lt;br&gt;Email:  &lt;a href="mailto:johnmadrid@hotmail.com" target="_top"&gt;johnmadrid@hotmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-498-1880&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Sunrise P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 33rd Ave S &amp; S Oregon St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Aaron Deitz&lt;br&gt;Email: &lt;a href="mailto:aarondietz@gmail.com" target="_top"&gt;aarondietz@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-694-3966&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Snoqualmie P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 4549 13th Ave S&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Người Đứng Đầu Trung Tâm: Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;New Holly Youth &amp; Family P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 32nd Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;New Holly Power P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 7123 S Holly Park Dr&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;New Holly Lucky Garden Hub &lt;br&gt;Vị Trí của Trung Tâm: S Holly St &amp; Shaffer Ave S&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;New Holly 29 P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 29th Ave S &amp; S Brighton St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;John C. Little P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 6961 37th Ave S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Dakota P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: 2902 S Dakota St&amp;#44; Seattle&amp;#44; WA 98108&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Beacon Food Forest Hub &lt;br&gt; Vị Trí của Trung Tâm:: 15th Ave S &amp; S Dakota St&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Ethiopian Community in Seattle &lt;br&gt;Vị Trí của Trung Tâm: 8323 Rainier Ave S (meet at main building)&lt;br&gt;Người Đứng Đầu Trung Tâm: Kassa Kachara&lt;br&gt;Email:  &lt;a href="mailto:kabiso_kass@yahoo.com" target="_top"&gt;kabiso_kass@yahoo.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-325-0304&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Angel Morgan P-Patch (Angel Morgan Hub) &lt;br&gt;Vị Trí của Trung Tâm: 3956 S Morgan St&amp;#44; Seattle&amp;#44; WA 98118 (The P Patch is located at 42nd Ave S &amp; S Morgan Street)&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Thistle P-Patch Hub &lt;br&gt;Vị Trí của Trung Tâm: Martin Luther King Jr Way S &amp; S Cloverdale St&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;New Holly Rockery &amp; Market Hub &lt;br&gt;Vị Trí của Trung Tâm: S Holly Park Dr &amp; Rockery Dr S&amp;#44; Seattle&amp;#44; WA 98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Contact Debbie Goetz&lt;br&gt;Email: &lt;a href="mailto:debbie.goetz@seattle.gov" target="_top"&gt;debbie.goetz@seattle.gov&lt;/a&gt;&lt;br&gt;Điện thoại: 206-684-0517&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Lakewood Seward Park Hub &lt;br&gt;Vị Trí của Trung Tâm: Lakewood Seward Park Community Club - 4916 S. Angeline Street&lt;br&gt;Người Đứng Đầu Trung Tâm: Aaron Evanson&lt;br&gt;Email:  &lt;a href="mailto:aaronevanson@gmail.com" target="_top"&gt;aaronevanson@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206.660.3822&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Rainier Beach Community Club Hub &lt;br&gt;Vị Trí của Trung Tâm: Rainier Beach Community Club - VFW Hall &amp;#44; 6038 S. Pilgrim&amp;#44; Seattle  WA  98118&lt;br&gt;Người Đứng Đầu Trung Tâm: Ron Angeles&lt;br&gt;Email:  &lt;a href="mailto:ranestoba@comcast.net" target="_top"&gt;ranestoba@comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại: 206-721-5326 and 206-351-0813&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Queen Anne Bowl &lt;br&gt;Vị Trí của Trung Tâm: 2806 3rd Ave W&lt;br&gt;Người Đứng Đầu Trung Tâm: Chris Saether&lt;br&gt;Email: &lt;a href="mailto:csaether@msn.com" target="_top"&gt;csaether@msn.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Interbay Athletic Complex &lt;br&gt;Vị Trí của Trung Tâm: 3027 17th Ave W&lt;br&gt;Người Đứng Đầu Trung Tâm: MIQA Be Prepared&lt;br&gt;Email: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Magnolia Manor Park &lt;br&gt; Vị Trí của Trung Tâm: 3500 28th Ave W&lt;br&gt;Người Đứng Đầu Trung Tâm: MIQA Be Prepared&lt;br&gt;Email: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Magnolia Metropolitan Market&lt;br&gt;Vị Trí của Trung Tâm: 3830 34th Ave W&lt;br&gt;Người Đứng Đầu Trung Tâm: MIQA Be Prepared&lt;br&gt;Email: &lt;a href="mailto:info@miqabeprepared.org" target="_top"&gt;info@miqabeprepared.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://www.MIQABePrepared.org"&gt;http://www.MIQABePrepared.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;West Queen Anne Playfield Hub &lt;br&gt;Vị Trí của Trung Tâm: 150 W Blaine St&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD &lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;West Magnolia Playfield Hub &lt;br&gt;Vị Trí của Trung Tâm: 32nd Ave W &amp; W Smith St&amp;#44; South Playfield&amp;#44; Southwest corner&lt;br&gt;Người Đứng Đầu Trung Tâm: Frank Gaul&lt;br&gt;Email:  &lt;a href="mailto:ftgaul@gmail.com" target="_top"&gt;ftgaul@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-499-8690&lt;br&gt;Trang web: &lt;a href="http://www.miqabeprepared.org/" target=_blank&gt;http://www.miqabeprepared.org/&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Ballard Commons Hub &lt;br&gt;Vị Trí của Trung Tâm: NW 57th &amp; 22nd Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Colin Getty&lt;br&gt;Email:  &lt;a href="mailto:k7biowa@gmail.com" target="_top"&gt;k7biowa@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Lower Woodland Playfields Hub &lt;br&gt;Vị Trí của Trung Tâm: Green Lake Way N &amp; N 50th St&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Ravenna Hub &lt;br&gt; Vị Trí của Trung Tâm: 6535 Ravenna Ave NE (Ravenna-Eckstein Community Center parking lot)&lt;br&gt;Người Đứng Đầu Trung Tâm: David Ward&lt;br&gt;Email:  &lt;a href="mailto:booksgalore22@gmail.com" target="_top"&gt;booksgalore22@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-523-1161&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Victory Heights Hub &lt;br&gt;Vị Trí của Trung Tâm: Victory Heights Park (1737 NE 106th St)&lt;br&gt;Người Đứng Đầu Trung Tâm: Ann Forrest&lt;br&gt;Email:  &lt;a href="mailto:aaforrest@hotmail.com" target="_top"&gt;aaforrest@hotmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: (360)550-2234&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Epic Life Church Hub &lt;br&gt;Vị Trí của Trung Tâm: Epic Life Church - 10503 Stone Ave N&amp;#44; Seattle&amp;#44; WA 98133&lt;br&gt;Người Đứng Đầu Trung Tâm: Larry Chaney&lt;br&gt;Email:  &lt;a href="mailto:larry@epiclifechurch.org" target="_top"&gt;larry@epiclifechurch.org&lt;/a&gt;&lt;br&gt;Điện thoại: 425-218-8849&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Crown Hill Park Hub &lt;br&gt;Vị Trí của Trung Tâm: NW 92nd &amp; 14th Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Dennis Galvin&lt;br&gt;Email:  &lt;a href="mailto:short.harp@gmail.com" target="_top"&gt;short.harp@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Shilshole Marina Hub &lt;br&gt;Vị Trí của Trung Tâm: Shilshole Marina&amp;#44; 7001 Seaview Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Jim Doub&lt;br&gt;Email: &lt;a href="mailto:jim@portagebaymarine.com" target="_top"&gt;jim@portagebaymarine.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Loyal Heights Playfield Hub&lt;br&gt;Vị Trí của Trung Tâm: NW 77th &amp;amp; 21st Ave NW (2101 NW 77th St&amp;#44; Loyal Heights CC basketball half court)&lt;br&gt;Người Đứng Đầu Trung Tâm: Cheryl Dyer&lt;br&gt;Email: &lt;a href="mailto:cheryldy@msn.com" target="_top"&gt;cheryldy@msn.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-784-3724&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Kirke Park Hub&lt;br&gt;Vị Trí của Trung Tâm: 7028 9th Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Hugh Kelso&lt;br&gt;Email: &lt;a href="mailto:HKelso@mac.com" target="_top"&gt;HKelso@mac.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org&lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Gilman Park Hub &lt;br&gt;Vị Trí của Trung Tâm: NW 54th &amp;amp; 9th Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Linda Frank&lt;br&gt;Email: &lt;a href="mailto:lindabfrank@gmail.com" target="_top"&gt;lindabfrank@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Ross Playground Hub &lt;br&gt;Vị Trí của Trung Tâm: 4320 4th Ave NW&lt;br&gt;Người Đứng Đầu Trung Tâm: Leslie Matthis&lt;br&gt;Email: &lt;a href="mailto:leslie.matthis@gmail.comv" target="_top"&gt;leslie.matthis@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206.783.1500&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Phinney Neighborhood Center Hub &lt;br&gt;Vị Trí của Trung Tâm: Phinney Neighborhood Center: 6532 Phinney Avenue North&amp;#44; Seattle&amp;#44; WA  98103 (Meeting Place: Phinney Center upper parking area)&lt;br&gt;Người Đứng Đầu Trung Tâm: David Baum&lt;br&gt;Email: &lt;a href="mailto:phinneyhub@gmail.com" target="_top"&gt;phinneyhub@gmail.com &lt;/a&gt;&lt;br&gt;Điện thoại: 206-913-1021&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Meridian Playfield/Good Shepherd Center Hub &lt;br&gt;Vị Trí của Trung Tâm: 4649 Sunnyside Ave. N&lt;br&gt;Người Đứng Đầu Trung Tâm: Brian Shapiro&lt;br&gt;Email: &lt;a href="mailto:bshapiro@objectarts.net" target="_top"&gt;bshapiro@objectarts.net&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;History House of Greater Seattle Hub &lt;br&gt;Vị Trí của Trung Tâm: 790 N 34th St&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Greenwood Senior Center Hub &lt;br&gt;Vị Trí của Trung Tâm: Greenwood Senior Center: 525 N 85th  Street&amp;#44; Seattle&amp;#44; WA  98103&lt;br&gt;Người Đứng Đầu Trung Tâm: Kelly Kasper&lt;br&gt;Email: &lt;a href="mailto:kelly@ht2consulting.com" target="_top"&gt;kelly@ht2consulting.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-397-4283&lt;br&gt;Co-Captain: Noel Frame&lt;br&gt;Co-Captain Email: &lt;a href="mailto:noel@noelframe.com" target="_top"&gt;noel@noelframe.com&lt;/a&gt; &lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Green Lake Playfield &amp; Community Center Hub &lt;br&gt;Vị Trí của Trung Tâm: 7201 Green Lake Dr N&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Bagley Elementary Hub &lt;br&gt;Vị Trí của Trung Tâm: 7821 Stone Ave N&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Điện thoại: TBD&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Maple Leaf Park Hub &lt;br&gt;Vị Trí của Trung Tâm: 1020 NE 82nd St&lt;br&gt;Người Đứng Đầu Trung Tâm: Lori Phipps&lt;br&gt;Email: &lt;a href="mailto:lphipps01@gmail.com" target="_top"&gt;lphipps01@gmail.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-947-0309&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Hunter Farm Hub &lt;br&gt;Vị Trí của Trung Tâm: 7730 35th Ave NE&lt;br&gt;Người Đứng Đầu Trung Tâm: Cần Tuyển Tình Nguyện Viên&lt;br&gt;Email: &lt;a href="mailto:info@seattleemergencyhubs.org" target="_top"&gt;info@seattleemergencyhubs.org&lt;/a&gt;&lt;br&gt;Trang web:&lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;University Heights Center &lt;br&gt;Vị Trí của Trung Tâm: NE 50th Street and University Way NE&lt;br&gt;Người Đứng Đầu Trung Tâm: Ray Munger&lt;br&gt;Email: &lt;a href="mailto:ray@uheightscenter.org" target="_top"&gt;ray@uheightscenter.org&lt;/a&gt;&lt;br&gt;Điện thoại: 206-527-4278&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Lake City Way SR 522/Fred Meyer Hub &lt;br&gt;Vị Trí của Trung Tâm: 13000 Lake City Way NE (SE corner of lower parking lot)&lt;br&gt;Người Đứng Đầu Trung Tâm: Sandy Motzer (98125)&lt;br&gt;Email: &lt;a href="mailto:sandymotzer@aol.com" target="_top"&gt;sandymotzer@aol.com&lt;/a&gt;&lt;br&gt;Điện thoại: 206-819-8056&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Luther Memorial Lutheran Church Hub &lt;br&gt;Vị Trí của Trung Tâm: 13047 Greenwood Ave N&lt;br&gt;Người Đứng Đầu Trung Tâm: Dale Johnson&lt;br&gt;Email: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại: 206-362-2980&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Các Trung Tâm Khẩn Cấp Cộng Đồng là nơi mà mọi người có thể tập trung sau một thảm hoạ để giúp đỡ lẫn nhau. &lt;p&gt;TRUNG TÂM GẦN BẠN NHẤT LÀ:&lt;center&gt;&lt;b&gt;Grace Lutheran Church Hub &lt;br&gt; Vị Trí của Trung Tâm: 11051 Phinney Ave N (Greenwood Avenue N &amp; N 112th Street)&lt;br&gt;Người Đứng Đầu Trung Tâm: Dale Johnson&lt;br&gt;Email: &lt;a href="mailto:dalerayjohnson@comcast.net" target="_top"&gt;dalerayjohnson@comcast.net&lt;/a&gt;&lt;br&gt;Điện thoại: 206-362-2980&lt;br&gt;Trang web: &lt;a href="http://seattleemergencyhubs.org/" target=_blank&gt;http://seattleemergencyhubs.org &lt;/a&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Kể từ năm 1870&amp;#44; 15 trận động đất mạnh (có cường độ trên 5 độ Richter) đã xảy ra tại Tiểu Bang Washington. Các câu chuyện của người bản địa cũng nhắc tới một trận động đất cực mạnh (có cường độ trên 8 độ Richter) và sóng thần xảy ra sau đó vào năm 1700</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Có khả năng cao xảy ra lũ lụt tại đây. Nó nằm tại vùng ngập của trận lũ với nguy cơ xảy ra là 1%&lt;/b&gt;. Điều này có nghĩa là có 25% khả năng nước lũ sẽ dâng tới đây trong vòng 30 năm tới &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt; email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Có khả năng cao xảy ra lũ lụt tại đây&lt;/b&gt;. Nó nằm tại vùng ngập của trận lũ với nguy cơ xảy ra là 1%. Điều này có nghĩa là có 25% khả năng nước lũ sẽ dâng tới đây trong vòng 30 năm tới &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ít có khả năng lũ lụt sẽ xảy ra tại đây&lt;/b&gt;. Mực nước có thể dâng cao một chút trong các trận lũ hoặc bão lớn. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ít có khả năng lũ lụt sẽ xảy ra tại đây&lt;/b&gt;. Mực nước trong hồ chứa có thể dâng cao một chút trong các trận lũ hoặc bão lớn. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Ít có khả năng lũ lụt sẽ xảy ra tại đây&lt;/b&gt;. Mực nước có thể dâng cao một chút trong các trận lũ hoặc bão lớn.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Các cây cầu có thể trở nên không an toàn khi lũ lụt xảy ra&lt;/b&gt;. Nếu bạn nghi ngờ một cây cầu đã bị hư hại&amp;#44; hãy cẩn thận và báo cáo với Trung Tâm Cảnh Báo Lũ Lụt (Flood Warning Center) bằng cách gọi tới số điện thoại 206-296-8200 hoặc 800-945-9263. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này không nằm trong các khu vực có nguy cơ cao xảy ra lũ lụt&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. NHƯNG nếu bạn sống gần một nhánh sông hoặc một con sông nhỏ&amp;#44; hãy cảnh giác vì khu vực đó có thể cũng bị lũ lụt. Xem &lt;a href=http://www.kingcounty.gov/depts/dnrp/wlr/sections-programs/river-floodplain-section.aspx target=_blank&gt;Xem trang web Quản Lý Sông Hồ và Vùng Ngập&lt;/a&gt; để biết thêm thông tin.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này đã từng bị lũ lụt khi các trận mưa lớn xảy ra tại Seattle&lt;/b&gt;. Việc này có thể sẽ lại xảy ra nếu một cơn bão mạnh khiến nước tích tụ lại và thoát nước kém. Cuộn xuống để xem cách chuẩn bị. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_100yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mưa&amp;#44; tuyết tan&amp;#44; hoặc cả hai hiện tượng đó khiến nước dâng cao nhanh chóng. Nước lũ cao hơn bờ sông&amp;#44; tràn vào các khu vực lân cận và gây ảnh hưởng tới đường xá. &lt;b&gt;Khu vực này nằm trong bản đồ vùng ngập của trận lũ có nguy cơ xảy ra là 0.2% và sẽ xảy ra lũ lụt&lt;/b&gt;. Có 6% khả năng bạn sẽ thấy một trận lũ có quy mô như vậy xảy ra trong 30 năm tới. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Các nhánh sông&amp;#44; suối&amp;#44; và sông gần đó đang tràn nước. Điều này khiến mọi người không thể đi qua đường xá được &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Không có khả năng xảy ra lũ lụt tại đây&lt;/b&gt;. Các trận bão lớn có thể khiến nước trong các nhánh sông&amp;#44; suối và sông gần đó dâng lên. Mưa to có thể tạo ra các vũng nước tù trên đường phố. Nếu bạn phát hiện xảy ra lũ lụt cục bộ&amp;#44; hãy gọi tới Trung Tâm Cảnh Báo Lũ Lụt Quận King qua số điện thoại 206-296-8200 hoặc 800-945-9263. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này dễ xảy ra ngập lụt đô thị&lt;/b&gt;. Bão càng lớn&amp;#44; bạn càng thấy ngập lụt xảy ra nhiều ở gần đây. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_500yr.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ . &lt;b&gt;Có khả năng cao là Sông Cedar sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng cao là Sông Green sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng cao là Sông Raging sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng cao là Sông Snoqualmie sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng cao là Sông Tolt sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng trung bình là Sông Cedar sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng trung bình là Sông Green sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng trung bình là Sông Raging sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng trung bình là Sông Snoqualmie sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng trung bình là Sông Tolt sẽ chảy qua khu vực này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng thấp là Sông Green sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng thấp là Sông Snoqualmie sẽ chảy qua vùng này trong tương lai&lt;/b&gt;.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. Chúng thay đổi nhiều nhất trong và sau các trận lũ. &lt;b&gt;Có khả năng thấp là Sông Tolt sẽ chảy qua vùng này trong tương lai. &lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Giống như vạn vật&amp;#44; các con sông chảy theo đường ít vật cản nhất và thay đổi hoạt động theo thời gian. &lt;b&gt;Chưa từng có nghiên cứu nào được thực hiện tại đây để kiểm tra xem dòng sông này có tràn ra ngoài theo thời gian hay không&amp;#44; nhưng hãy cảnh giác rằng việc này có thể xảy ra.&lt;/b&gt;&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vùng này nằm trong kênh nước hiện tại của con sông. Vị trí của con kênh con có thể thay đổi theo thời gian. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_CMZ.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Trường hợp vỡ đập rất hiếm khi xảy ra. Tuy nhiên&amp;#44; nếu &lt;a href=https://goo.gl/maps/X2HGtZX6Kyz target=_blank&gt;Đập George Culmback&lt;/a&gt; hoặc &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;Đập Sông Tolt&lt;/a&gt; bị vỡ thì khu vực này có thể xảy ra lũ lụt &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.</t>
+  </si>
+  <si>
+    <t>Trường hợp vỡ đập rất hiếm khi xảy ra. Tuy nhiên&amp;#44; nếu &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Đập Hồ Youngs&lt;/a&gt; bị vỡ&amp;#44; khu vực này có nguy cơ bị lũ lụt &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.</t>
+  </si>
+  <si>
+    <t>Trường hợp vỡ đập rất hiếm khi xảy ra. Tuy nhiên&amp;#44; nếu &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Đập Hồ Youngs&lt;/a&gt; bị vỡ&amp;#44; khu vực này có nguy cơ trung bình bị lũ lụt &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trường hợp vỡ đập rất hiếm khi xảy ra. Tuy nhiên&amp;#44; nếu &lt;a href=https://goo.gl/maps/RMaHnAY8RCp target=_blank&gt;Đập Hồ Youngs&lt;/a&gt; bị vỡ&amp;#44; khu vực này có nguy cơ cao bị lũ lụt &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn. Trường hợp vỡ đập rất hiếm khi xảy ra. </t>
+  </si>
+  <si>
+    <t>Trường hợp vỡ đập rất hiếm khi xảy ra. Tuy nhiên&amp;#44; nếu &lt;a href=https://goo.gl/maps/DpotpRjYDvG2 target=_blank&gt;Đập Sông Tolt&lt;/a&gt; bị vỡ&amp;#44; khu vực này có thể bị lũ lụt &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;. Đăng ký để nhận cảnh báo về lũ lụt qua &lt;a href=https://green2.kingcounty.gov/floodalertsystem/ target=_blank&gt;email hoặc tin nhắn&lt;/a&gt; hoặc tải về &lt;a href=http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx target=_blank&gt;ứng dụng cảnh báo lũ lụt&lt;/a&gt; trên điện thoại thông minh của bạn.</t>
+  </si>
+  <si>
+    <t>Các cơn bão khốc liệt được dự đoán sẽ gia tăng trong 50 năm tới. Chúng sẽ gây mưa và tuyết. Các con sông sẽ có dòng chảy cao hơn dẫn tới lũ lụt nhiều hơn vào mùa Thu/Đông. Bấm vào hình ảnh để tìm hiểu thêm. &lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Rivers.jpg" alt="Climate Change Rivers Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Trời đã liên tục mưa to hoặc mưa nhiều ngày rồi? Nhiệt độ tăng lên đã gây ra hiện tượng tuyết tan nhanh trên các ngọn núi? Mực nước trong các con sông tại địa phương nhìn có vẻ cao? Khả năng xảy ra lũ lụt có thể tăng lên. Theo dõi các bản tin từ dịch vụ thời tiết để biết các cảnh báo dành cho địa phương.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;LẬP KẾ HOẠCH&lt;/b&gt; - Lập kế hoạch làm gì và đi đâu khi nước trong các sông hồ dâng lên. &lt;b&gt;Chuẩn bị sẵn sàng các vật dụng cần thiết&lt;/b&gt; (giấy khai sinh&amp;#44; các tài liệu quan trọng&amp;#44; ảnh&amp;#44; v.v.). Mua bảo hiểm lũ lụt nếu bạn cần bảo hiểm.&lt;/li&gt;&lt;li&gt;&lt;b&gt;CHUẨN BỊ&lt;/b&gt; - Cất trữ các vật có giá trị và các hoá chất trong gia đình ở phía trên cao so với mực nước lũ và &lt;b&gt;tìm hiểu cách tắt các tiện ích sinh hoạt&lt;/b&gt; (&lt;a href=http://www.seattle.gov/emergency-management/preparedness/prepare-your-home target=_blank&gt;nước&amp;#44; khí ga&amp;#44; và điện&lt;/a&gt;).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;SẴN SÀNG&lt;/b&gt; - Tập hợp các vật dụng khẩn cấp (quần áo ấm&amp;#44; đèn pin&amp;#44; điện thoại di động&amp;#44; đài cầm tay&amp;#44; v.v.). Nếu thời gian cho phép và thấy cần thiết&amp;#44; hãy tắt các tiện ích sinh hoạt.&lt;/li&gt;&lt;li&gt;&lt;b&gt;THEO DÕI&lt;/b&gt; - Lắng nghe tin tức và sơ tán đến khu vực cao hơn khi được khuyến cáo.&lt;/li&gt;&lt;li&gt;&lt;b&gt;TRÁNH XA NGUY HIỂM – KHÔNG lội hoặc lái xe qua nước lũ.&lt;/b&gt; Chỉ cần dòng nước sâu 6 inch là đủ để quật ngã bạn và 2 feet để cuốn trôi cả một chiếc xe!&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Flood_during.jpg" alt="This is a panel of four cartoon images showing what to do during an a flood collect essentials&amp;#44; get to high ground&amp;#44; avoid water&amp;#44; and shutt off utilities." title="During Flood Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nếu nhà bạn bị ngập&amp;#44; &lt;b&gt;hãy cẩn thận khi vào bên trong bởi kết cấu của nó đã có thể bị hư hại.&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Công viên đường Russell &lt;br&gt; giữa Russell Rd. và S. 240th St.&lt;br&gt; Kent&amp;#44; WA&amp;#44; 98032 &lt;br&gt;  Chỉ lấy cát (không có túi cát)&lt;br&gt; T2-T6 8:00 sáng - 4:00 chiều&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát.&lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&amp;#44;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt;Public Works Shops &lt;br&gt;1155 East North Bend Way &lt;br&gt; North Bend&amp;#44; WA 98045&lt;br&gt;Cát và túi cát&lt;br&gt;&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; 33100 NE 45th St &lt;br&gt; Carnation&amp;#44; WA 98014 &lt;br&gt;T2-T6 8:00 sáng - 4:30 chiều&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Meadowbrook Community Center&lt;br&gt;10517 35th Ave. NE &lt;br&gt; Seattle&amp;#44; WA 98125&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; 1305 C St. SW &lt;br&gt; Auburn&amp;#44; WA 98001&lt;br&gt; T2-T6 6:30 sáng - 4:00 chiều &lt;br&gt;Cát và túi cát--&gt;253-931-3048&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Kent City Public Works&lt;br&gt; 5821 S. 240th St. &lt;br&gt; Kent&amp;#44; WA 98032&lt;br&gt; T2-T6 8:00 sáng - 4:00 chiều &lt;br&gt;Chỉ lấy túi cát (không có cát)&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Tahoma School District &lt;br&gt; 23015 SE 216th Way&lt;br&gt; Maple Valley&amp;#44; WA 98038&lt;br&gt; 8:00 sáng - 5:00 chiều &lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Pacific City Park &lt;br&gt; 600 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Pacific/Algona Community Center &lt;br&gt; 100 3rd Ave. SE &lt;br&gt; Pacific&amp;#44; WA 98047 &lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; City Property @ &lt;br&gt; Railroad Avenue SE và SE King Street &lt;br&gt; Snoqualmie&amp;#44; WA 98065&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Preston-Snoqualmie Trail parking lot &lt;br&gt; Lake Alice Road SE và SE 56th Place &lt;br&gt; Fall City&amp;#44; WA 98024&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; 14701 Main St. NE &lt;br&gt; Duvall&amp;#44; WA 98019&lt;br&gt;Cát và túi cát--&gt;425-788-3332&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Haller Lake Neighborhood &lt;br&gt; 12551 Ashworth Ave N.&lt;br&gt; Seattle&amp;#44; WA 98133&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; South Park Neighborhood &lt;br&gt; 731 S. Sullivan &lt;br&gt; Seattle&amp;#44; WA 98108&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chuẩn bị ứng phó với lũ lụt bằng cách thu thập và làm đầy bao cát. &lt;a href=https://hazardready.org/seattle/static/img/data/Flood_Sandbag_Distr_Centers.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;p&gt;TRUNG TÂM PHÂN PHỐI GẦN BẠN NHẤT LÀ: &lt;center&gt;&lt;b&gt; Delridge Community Center &lt;br&gt; 4501 Delridge Way SW &lt;br&gt; Seattle&amp;#44; WA 98106&lt;br&gt;Cát và túi cát&lt;/b&gt;&lt;/center&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Do có nhiều sông hồ nên Quận King thường xuyên xảy ra lũ lụt khi trời mưa nhiều hoặc tuyết tan nhanh. &lt;b&gt;Lũ lụt xuất hiện nhiều nhất từ tháng Mười Một đến tháng Hai&lt;/b&gt;&amp;#44; nhưng cũng có thể diễn ra bất cứ khi nào hội tụ đủ điều kiện.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này có độ dốc nông nên sẽ ít có khả năng xảy ra sạt lở đất tại đây&lt;/b&gt;. Sạt lở đất thường xảy ra khi nền đất ẩm ướt do mưa nhiều HOẶC rung chấn do động đất gây ra. Kéo xuống phần các sự kiện lịch sử để xem những vụ sạt lở đất nào đã được ghi nhận xảy ra tại khu vực của bạn. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Vì có độ dốc hơn nên khu vực này có nhiều nguy cơ xảy ra sạt lở đất nhẹ&lt;/b&gt;. Sạt lở đất thường xảy ra khi nền đất ẩm ướt do mưa nhiều HOẶC rung chấn do động đất gây ra. Kéo xuống phần các sự kiện lịch sử để xem các hoạt động sạt lở nào đã được ghi nhận xảy ra tại khu vực của bạn. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Không nhiều khả năng xảy ra sạt lở tại đây&amp;#44; nhưng có thể xảy ra tại một sườn dốc gần đó nếu hội tụ đủ điều kiện&lt;/b&gt;. Cảnh giác với những khu vực không ổn định. Đặc biệt là những con đường đã bị đống đổ nát rơi xuống chặn lại hoặc bị mưa gây sụt lún. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Những sườn dốc gần đó có cây hay không? Có phải trời đã mưa suốt nhiều ngày? &lt;b&gt;Nếu câu trả lời là có&amp;#44; những sườn dốc này có nhiều khả năng sẽ xảy ra sạt lở đất&lt;/b&gt;.Cảnh giác với những khu vực không ổn định. Đặc biệt là những con đường đã bị đống đổ nát rơi xuống chặn lại hoặc bị mưa gây sụt lún. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_SteepSlope.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Sạt lở đất thường xảy ra dọc theo những vách đá cạnh bờ biển nơi hứng chịu những đợt sóng đánh vào bờ. &lt;b&gt;Mực nước tại eo biển Puget đã dâng lên thêm 8 inch kể từ năm 1913&lt;/b&gt;! Với mực nước biển cao hơn&amp;#44; nguy cơ xói mòn vách đá cũng tăng lên. Lượng mưa lớn từ những cơn bão cũng làm suy yếu những sườn dốc&amp;#44; gây thêm nhiều vụ sạt lở tại Quận King. Bấm vào hình ảnh để tìm hiểu thêm.&lt;br&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storms Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Bạn có nghe thấy tiếng cây đổ&amp;#44; đá va vào nhau&amp;#44; hay âm thanh từ đất? Bạn có nhìn thấy những vết nứt xung quanh và đất đá&amp;#44; cây cối di chuyển xuống dốc? Đó có thể là một vụ sạt lở đất. Hãy di chuyển đến khu vực vững chãi.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;ĐÁNH GIÁ &lt;/b&gt; - Nếu khu vực xung quanh nhà bạn có nguy cơ sạt lở cao&amp;#44; &lt;b&gt;hãy tìm kiếm lời khuyên từ các chuyên gia địa chất&lt;/b&gt;. Họ có thể đánh giá tai biến sạt lở và/hoặc thiết kế các kỹ thuật khắc phục nhằm giảm thiểu nguy cơ sạt lở.&lt;/li&gt;&lt;li&gt;&lt;b&gt;GIẢM THIỂU NGUY CƠ &lt;/b&gt; -  Trồng cây bao phủ các sườn dốc và/hoặc xây tường chắn để &lt;b&gt;gia cố sườn đồi.&lt;/b&gt;&lt;/li&gt;&lt;li&gt;&lt;b&gt;CHUẨN BỊ - Chuẩn bị một bộ vật dụng cần thiết và lên kế hoạch cho gia đình &lt;/b&gt;với ít nhất hai tuyến đường sơ tán.&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Tránh xa đường sạt lở đất hoặc hướng di chuyển của dòng lũ bùn đá là cách bảo vệ bạn tốt nhất.&lt;/b&gt; Cục Khảo Sát Địa Chất Hoa Kỳ cũng khuyến nghị những biện pháp sau&amp;#44; &lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;&lt;b&gt;CẢNH GIÁC - Lắng nghe những âm thanh bất thường&lt;/b&gt;. Những trận mưa lớn&amp;#44; đột ngột có thể đặc biệt nguy hiểm&amp;#44; nhất là sau khoảng thời gian mưa kéo dài và thời tiết ẩm ướt.&lt;/li&gt;&lt;li&gt;&lt;b&gt;CÂN NHẮC SƠ TÁN&lt;/b&gt; - Nếu bạn ở trong những khu vực dễ bị sạt lở và các dòng lũ bùn đá&amp;#44; hãy cân nhắc đến việc rời khỏi nơi đó nếu an toàn. Nếu bạn quyết định ở trong nhà&amp;#44; hãy chuyển lên tầng cao hơn nếu có thể.&lt;/li&gt;&lt;li&gt;&lt;b&gt;CHÚ Ý MỰC NƯỚC &lt;/b&gt; - Nếu bạn gần sông suối hoặc kênh mương&amp;#44; &lt;b&gt;hãy cảnh giác với sự thay đổi lên xuống bất thường của dòng nước và màu sắc từ trong sang bùn đục&lt;/b&gt;. Đây có thể là dấu hiệu của hoạt động sạt lở ở thượng nguồn. ĐỪNG CHẦN CHỪ! Hãy cứu lấy bản thân chứ không phải đồ đạc của bạn.
+&lt;/li&gt;&lt;/ul&gt; Bạn có thể tìm hiểu thêm lời khuyên về lở đất từ USGS  &lt;a href=http://landslides.usgs.gov/learn/prepare.php target=_blank&gt;tại đây&lt;/a&gt;. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Landslide_during.jpg" alt="This is a panel of three cartoon images showing what to do during an a landslide. Stay Alert&amp;#44; Leave the area&amp;#44; and Don't Delay." title="During Landslide Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;CHUẨN BỊ ỨNG PHÓ VỚI LŨ LỤT (sạt lở đất thường chặn các con sông và khiến mực nước dâng lên và gây lũ lụt)&lt;/b&gt;.&lt;ul style="padding-left:1.2em"&gt;&lt;li&gt;Tránh xa khu vực sạt lở. Các vụ sạt lở khác có thể diễn ra sau vụ sạt lở chính.&lt;/li&gt;&lt;li&gt;Một khi đã an toàn&amp;#44; hãy kiểm tra những người bị thương và mắc kẹt.&lt;/li&gt;&lt;li&gt;Kiểm tra các đường dây cung cấp tiện ích sinh hoạt bị hư hại và báo cáo thiệt hại cho công ty cấp điện&amp;#44; nước hoặc ga của bạn.&lt;/li&gt;&lt;li&gt;Theo dõi truyền thông địa phương hoặc Đài Phát Thanh Thời Tiết NOAA để cập nhật thông tin hiện tại.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Để biết thêm thông tin&amp;#44; hãy truy cập trang web của Bộ Tài Nguyên Môi Trường về &lt;a href=http://www.dnr.wa.gov/programs-and-services/geology/geologic-hazards/landslides#some-historic-landslides-in-washington-state target=_blank&gt;sạt lở đất&lt;/a&gt; và &lt;a href=http://file.dnr.wa.gov/publications/ger_fs_landslide_hazards.pdf target=_blank&gt;hiểm hoạ sạt lở đất&lt;/a&gt;. Để biết thông tin về các vụ sạt lở tại khu vực của bạn&amp;#44; tham khảo những thông tin có sẵn từ &lt;a href=http://www.kingcounty.gov/services/environment/water-and-land/landslides.aspx target=_blank&gt;Quận King&lt;/a&gt; và &lt;a href=http://www.seattle.gov/dpd/aboutus/whoweare/emergencymanagement target=_blank&gt;Seattle&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Chưa xác định có vụ sạt lở nào xảy ra tại đây&lt;/b&gt; (&lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;Báo cáo 2016&lt;/a&gt;). Sạt lở đất diễn ra phổ biến nhất tại những sườn dốc cằn cỗi nơi tập hợp hệ thống thoát nước. Nếu bạn sống dưới một khu vực như vậy thì nên cẩn trọng với những nguy cơ (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg=en target=_blank&gt;bản đồ&lt;/a&gt;). Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Các nhà khoa học chưa ghi nhận được bất kỳ vụ sạt lở nào tại đây&lt;/b&gt;. Để biết thêm thông tin xem &lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Báo cáo 2016&lt;/a&gt; và &lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;bản đồ&lt;/a&gt;. Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Không có vụ sạt lở nào được ghi nhận tại đây&lt;/b&gt; theo một nghiên cứu được tiến hành năm 1995 tại Thành Phố Seattle. (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Chưa có nghiên cứu được hoàn thành tại đây&lt;/b&gt; để xác định xem liệu có vụ sạt lở lịch sử nào từng diễn ra (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MỘT VỤ SẠT LỞ ĐẤT ĐÃ XẢY RA TẠI ĐÂY&lt;/b&gt; trong quá khứ (&lt;a href=http://www.kingcounty.gov/~/media/services/gis/documents/DPER-LS-hazard-map-report.ashx?la=en target=_blank&gt;Báo cáo 2016&lt;/a&gt;) và (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;). Lịch sử sạt lở có thể hoặc không chỉ ra nguy cơ sạt lở trong tương lai. Để xác định mối nguy hiểm có còn tồn tại hay không&amp;#44; cần kiểm tra cụ thể tại hiện trường từ chuyên gia tư vấn địa kỹ thuật. Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MỘT VỤ SẠT LỞ ĐẤT ĐÃ XẢY RA TẠI ĐÂY&lt;/b&gt; trong quá khứ (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Báo cáo 2016&lt;/a&gt;) và (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;). Lịch sử sạt lở có thể hoặc không chỉ ra nguy cơ sạt lở trong tương lai. Để xác định mối nguy hiểm có còn tồn tại hay không&amp;#44; cần kiểm tra cụ thể tại hiện trường từ chuyên gia tư vấn địa kỹ thuật. Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MỘT VỤ SẠT LỞ ĐẤT và LỞ ĐÁ ĐÃ XẢY RA TẠI ĐÂY&lt;/b&gt; trong quá khứ  (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Báo cáo 2016&lt;/a&gt;) và (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;). Lịch sử sạt lở có thể hoặc không chỉ ra nguy cơ sạt lở trong tương lai. Để xác định mối nguy hiểm có còn tồn tại hay không&amp;#44; cần kiểm tra cụ thể tại hiện trường từ chuyên gia tư vấn địa kỹ thuật. Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MỘT VỤ LỞ ĐÁ ĐÃ XẢY RA TẠI ĐÂY&lt;/b&gt; trong quá khứ (&lt;a href=http://your.kingcounty.gov/dnrp/library/2016/kcr2783.pdf =en target=_blank&gt;Báo cáo 2016&lt;/a&gt;) và (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;). Lịch sử sạt lở có thể hoặc không chỉ ra nguy cơ sạt lở trong tương lai. Để xác định mối nguy hiểm có còn tồn tại hay không&amp;#44; cần kiểm tra cụ thể tại hiện trường từ chuyên gia tư vấn địa kỹ thuật. Để kiểm tra những lớp dữ liệu sâu sát hơn&amp;#44; hãy truy cập &lt;a href=https://gismaps.kingcounty.gov/iMap/ target=_blank&gt;iMap Quận King&lt;/a&gt; (đảm bảo sạt lở đất đã được đánh dấu trong phần chú thích).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;MỘT VỤ SẠT LỞ ĐẤT ĐÃ XẢY RA TẠI ĐÂY&lt;/b&gt; theo một nghiên cứu năm 1995 tại Thành Phố Seattle (&lt;a href=https://hazardready.org/seattle/static/img/data/Landslide_existing.jpg =en target=_blank&gt;bản đồ&lt;/a&gt;). Lịch sử sạt lở có thể hoặc không chỉ ra nguy cơ sạt lở trong tương lai. Để xác định mối nguy hiểm có còn tồn tại hay không&amp;#44; cần kiểm tra cụ thể tại hiện trường từ chuyên gia tư vấn địa kỹ thuật.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Đây là khu vực có nguy cơ cháy rừng rất cao&lt;/b&gt;. Nó ở nằm ở ranh giới giữa con người và khu rừng. Miền Tây Washington là vùng có khí hậu ôn hòa&amp;#44; nhưng các vụ cháy rừng cũng tấn công vùng phía Đông của Quận King mỗi năm. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Đây là khu vực có nguy cơ cháy rừng cao&lt;/b&gt;. Nó ở nằm ở ranh giới giữa con người và khu rừng. Miền Tây Washington là vùng có khí hậu ôn hòa&amp;#44; nhưng các vụ cháy rừng cũng tấn công vùng phía Đông của Quận King mỗi năm. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này không được xác định có nguy cơ cháy rừng cao&lt;/b&gt;&amp;#44; nhưng nó cách khu vực nguy cơ cao chỉ khoảng nửa dặm. Nếu gặp điều kiện thuận lợi&amp;#44; ngọn lửa sẽ lan rộng. (&lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;bản đồ&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Khu vực này có nguy cơ cháy rừng thấp hoặc rất thấp&lt;/b&gt;. Nếu bạn sống gần khu vực rừng cây&amp;#44; hãy đề phòng cháy rừng có thể xảy ra. &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Vì đây là nước nên không có nguy cơ cháy rừng xảy ra tại đây.&lt;/b&gt; &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_WUI.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Bạn có thể gặp phải một trận cháy rừng lớn tại đây&lt;/b&gt;. Nó sẽ di chuyển nhanh&amp;#44; với ngọn lửa lớn và có thể đổi hướng nhanh chóng. Phải mất vài ngày hoặc hàng tuần để các nhân viên cứu hoả có thể khống chế được trận hỏa hoạn. KHÓI từ các vụ cháy có thể di chuyển đến khoảng cách xa và có thể là nguy cơ ngay cả khi không có gì cháy xung quanh. Kiểm tra chất lượng không khí khu vực của bạn &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;tại đây&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Bạn có thể gặp phải một trận cháy rừng tại đây&lt;/b&gt;. Nó sẽ di chuyển nhanh&amp;#44; với ngọn lửa lớn và có thể đổi hướng nhanh chóng. Phải mất vài ngày hoặc hàng tuần để các nhân viên cứu hoả có thể khống chế được trận hỏa hoạn. KHÓI từ các vụ cháy có thể di chuyển đến khoảng cách xa và có thể là nguy cơ ngay cả khi không có gì cháy xung quanh. Kiểm tra chất lượng không khí khu vực của bạn &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;tại đây&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Dù không có khả năng&amp;#44; nhưng nếu bạn sống gần khu vực rừng&amp;#44; bạn có thể gặp cháy rừng&lt;/b&gt;. KHÓI từ các vụ cháy có thể di chuyển đến khoảng cách xa và có thể là nguy cơ ngay cả khi không có gì cháy xung quanh. Kiểm tra chất lượng không khí khu vực của bạn &lt;a href=http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx target=_blank&gt;tại đây&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Số lượng &lt;b&gt;các vụ cháy rừng tại vùng Tây Bắc Thái Bình Dương đã tăng lên rõ rệt trong vài thập kỷ qua&lt;/b&gt;. Xu hướng này nhiều khả năng sẽ tiếp diễn với những mùa hè khô hơn và nhiều bão hơn (sét đánh có thể làm bùng lên ngọn lửa). Nhiều khu vực rừng rộng lớn có thể cháy và thải một lượng khói lớn vào khí quyển. Bấm vào hình ảnh để tìm hiểu thêm.&lt;br&gt;&lt;a  ref="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Forests.jpg" alt="Climate Change Forest Infographic"&gt;
+&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Bạn có ngửi hoặc nhìn thấy khói? Đó là một dải thời tiết khô? Đó có thể là cháy rừng. Tránh xa những đám cháy đang cháy và nếu thấy ngọn lửa bùng lên&amp;#44; hãy gọi 9-1-1 để báo cháy</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;TẠO KHÔNG GIAN&lt;/b&gt; - Bảo vệ mạng sống và tài sản bằng cách tạo một &lt;b&gt;không gian thích ứng với lửa xung quanh nhà&amp;#44;&lt;/b&gt; kho và nơi làm việc của bạn. Để biết cách thực hiện&amp;#44; hãy truy cập &lt;a href=http://www.firewise.org/wildfire-preparedness.aspx target=_blank&gt;firewise.org&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;THEO DÕI THỜI TIẾT&lt;/b&gt; - Chỉ cần vài ngày nắng là đủ để khiến rừng cây khô héo và dễ dàng bắt lửa. Điều kiện có gió có thể khiến ngọn lửa nhanh chóng vượt khỏi tầm kiểm soát.&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Firewise_Brochure.jpg" alt="This is an image of ways to prevent wildfire around your home. They include screening decks&amp;#44; pruning trees 6-10 feet from the ground&amp;#44; using fire-resistant wall and roof materials&amp;#44; keeping plants watered&amp;#44; and making sure your driveway can accommodate an emergency vehicle" title="How to Prepare Your Home for Wildfire"&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;THEO DÕI&lt;/b&gt; - Chú ý theo dõi cảnh báo khẩn cấp của địa phương trên đài phát thanh và/hoặc vô tuyến và sẵn sàng để sơ tán nếu cần thiết.&lt;/li&gt;&lt;li&gt;&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Chỉ quay trở về nhà khi chính quyền thông báo đã an toàn.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Thận trọng khi tiến vào các khu vực bị cháy&lt;/b&gt; bởi nguy hiểm vẫn có thể rình rập.&lt;/li&gt;
+&lt;li&gt;Kiểm tra cẩn thận nhiều lần dấu hiệu của khói hoặc tàn lửa còn sót lại.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Chụp ảnh thiệt hại&lt;/b&gt; để phục vụ mục đích bảo hiểm.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nếu bạn nghĩ ngôi nhà của bạn có nguy cơ cao&amp;#44; &lt;b&gt;Quận King có thông tin&amp;#44; chương trình khuyến khích và hội thảo đào tạo dành cho các chủ đất&lt;/b&gt;. Bạn có thể tìm hiểu thêm &lt;a href=http://www.kingcounty.gov/environment/water-and-land/forestry.aspx target=_blank&gt;tại đây&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Phía Đông Quận King có các vụ cháy rừng nhỏ mỗi năm. Thường thì con người là nguyên nhân chủ yếu. Hãy xem nơi các vụ cháy xảy ra trong quá khứ bằng cách bấm &lt;a href=https://hazardready.org/seattle/static/img/data/Wildfire_Historic.jpg target=_blank&gt;tại đây&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lahar (dòng bùn núi lửa) là hiểm hoạ chính từ Núi Rainier. &lt;b&gt;Các cư dân tại phía Nam Quận King có 1/10 cơ hội gặp phải lahar trong đời&lt;/b&gt;. Núi Rainier được coi là một ngọn núi lửa đang hoạt động&amp;#44; nhưng phải nhiều năm nữa nó mới phun trào lại.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nếu lahar xảy ra trên Núi Rainier&amp;#44; &lt;b&gt;khu vực này sẽ bị lũ lụt&amp;#44; và những trầm tích như bùn&amp;#44; cát&amp;#44; đá và các đống đổ nát khác đều sẽ bị dòng lahar cuốn xuống sông&lt;/b&gt;. Hiện tượng này có thể xảy ra hàng năm cho đến hàng thập kỷ sau khi lahar xảy ra. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Có 10% - 40% khả năng lahar sẽ xuất hiện từ Núi Rainier và chảy qua khu vực này trong vòng 50 năm tới&lt;/b&gt;. Lahar hoạt động và trông giống như dòng xi măng ướt. Lớp bùn dày và lũ bùn đá sẽ bao phủ cả khu vực nếu lahar xảy ra. Điều này có thể gây thiệt hại tài sản nghiêm trọng và mất một thời gian dài để tái thiết. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Có 5% - 10% khả năng lahar sẽ xuất hiện từ Núi Rainier và chảy qua khu vực này trong vòng 50 năm tới&lt;/b&gt;. Lahar hoạt động và trông giống như dòng xi măng ướt. Lớp bùn dày và lũ bùn đá sẽ bao phủ cả khu vực nếu lahar xảy ra. Điều này có thể gây thiệt hại tài sản nghiêm trọng và mất một thời gian dài để tái thiết. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Bạn ở BÊN NGOÀI KHU VỰC CÓ HIỂM HOẠ LAHAR&lt;/b&gt;. Nếu Núi Rainier phun trào&amp;#44; tro bụi sẽ che phủ cả khu vực. Nó sẽ trông giống như những khu vực bị ảnh hưởng bởi đợt phun trào của Núi Saint Helen vào năm 1980. Độ dày của tro bụi sẽ thay đổi tùy vào khoảng cách từ vụ phun trào. &lt;a href=https://hazardready.org/seattle/static/img/data/Volcano_Lahar.jpg target=_blank&gt;(bản đồ)&lt;/a&gt;&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>Thông thường núi lửa sẽ có những tín hiệu cảnh báo vài ngày hay hàng tháng trước khi phun trào. &lt;b&gt;Hoạt động khí và động đất gia tăng và bề mặt đất nhô lên khi mắc ma di chuyển bên dưới&lt;/b&gt;. Mặc dù các dấu hiệu này có thể khó nhận biết đối với công chúng&amp;#44; nhưng núi Rainer vẫn được theo dõi liên tục bởi các nhà khoa học thuộc &lt;a href=http://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;Chương Trình Hiểm Hoạ Núi Lửa USGS&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;HỎI&lt;/b&gt; - Tìm hiểu bước mà các nhân viên chính phủ địa phương thực hiện để chuẩn bị cho sự cố núi lửa. &lt;b&gt;Hỏi các nhân viên chính phủ địa phương xem kế hoạch của họ là gì và họ sẽ liên lạc với bạn như thế nào trong khi xảy ra sự cố&lt;/b&gt;. Bạn có thể liên hệ  &lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=_blank&gt;Văn Phòng Quản Lý Trường Hợp Khẩn Cấp&lt;/a&gt; của Quận King.&lt;/li&gt;&lt;li&gt;&lt;b&gt;LẬP KẾ HOẠCH&lt;/b&gt; - Nói với bạn bè và hàng xóm của bạn. Nếu bạn trong vùng có nguy cơ cao&amp;#44; &lt;b&gt;hãy quyết định nơi bạn sẽ đi&amp;#44; bạn sẽ mang theo những gì&amp;#44; và bạn sẽ liên lạc với ai&lt;/b&gt;.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Trong khi núi lửa phun trào&amp;#44; hãy theo dõi thông tin để cập nhật tình hình và làm theo những hướng dẫn khẩn cấp.
+&lt;ul&gt;&lt;li&gt;&lt;b&gt;TRONG VÙNG LAHAR - Di chuyển đến vùng đất cao ngay lập tức.&lt;/b&gt;&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Ở BÊN NGOÀI&lt;/b&gt; - Che miệng&amp;#44; mũi và cơ thể của bạn để tránh bị bỏng rát. &lt;b&gt;Tìm nơi trú ẩn&lt;/b&gt;. &lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Ở TRONG NHÀ - Đóng chặt cửa và các lỗ thông hơi trong nhà và ở trong nhà&amp;#44; trừ phi có chỉ dẫn khác&lt;/b&gt;. Dùng khăn ướt chèn chân cửa ra vào và dán chặt các khe cửa sổ hở. Tắt động cơ xe hơi và xe tải để tránh thiệt hại do tắc nghẽn tro bụi. Bảo vệ các loài động vật và máy móc bằng cách mang chúng vào trong nhà hoặc khu vực được che chắn.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/intensity/Volcano_during.jpg" alt="This is an panel of three images of what to do during a volcanic eruption or lahar. In lahar zone&amp;#44; outside&amp;#44; inside." title="During Volcano Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sau khi mối nguy hiểm từ vụ phun trào đã lắng xuống&amp;#44; việc chính cần làm là dọn dẹp tro bụi.&lt;br&gt;  &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/MtStHel_Yakima_graders.jpg" alt="This image shows two graders shoveling inches of ashfall from Saint Helens' eruption" title="Ashfall Cleanup in Yakima After Mt. Saint Helens"&gt;&lt;li&gt;Đeo kính và mặt nạ khi ra ngoài. &lt;b&gt;Chất lượng không khí sẽ thấp&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Tránh chạy động cơ xe&lt;/b&gt;. Nếu bạn phải lái xe&amp;#44; hãy giữ tốc độ chậm (dưới 35 dặm/giờ) và thường xuyên kiểm tra dầu&amp;#44; bộ lọc dầu và bộ lọc không khí. &lt;/li&gt;&lt;li&gt;Tro bụi rất nặng và có thể khiến các tòa nhà đổ sập. Nếu đủ an toàn&amp;#44; &lt;b&gt;hãy dọn tro bụi từ mái nhà và máng nước mưa&lt;/b&gt;.&lt;/li&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Bạn có thể tìm hiểu thêm về Núi Rainier và nguy cơ tai biến từ các nguồn: 
+&lt;ul&gt;&lt;li&gt;&lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/ target=_blank&gt;Theo dõi và các thông tin khác&lt;/a&gt; - Cục Khảo Sát Địa Chất Hoa Kỳ&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx target=blank&gt;Thông Tin Tổng Quan về Quận King&lt;/a&gt; - Quận King&lt;li&gt;&lt;a href=https://www.nps.gov/mora/planyourvisit/geohazards.htm target=_blank&gt;Hiểm Hoạ Địa Chất tại Rainier&lt;/a&gt; - Cục Công viên Quốc Gia Hoa Kỳ&lt;/li&gt;&lt;li&gt;&lt;a href=http://www.pnsn.org/volcanoes/mount-rainier target=_blank&gt;Các trận động đất gần Rainier&lt;/a&gt; - Mạng Lưới Địa Chấn Tây Bắc Thái Bình Dương&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Núi Rainier có một lịch sử dài về &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_eruption_history.html target=_blank&gt;hoạt động phun trào&lt;/a&gt; và &lt;a href=https://volcanoes.usgs.gov/volcanoes/mount_rainier/geo_hist_lahars.html target=_blank&gt;lahar&lt;/a&gt;. Khoảng 500 năm trước&amp;#44; Dòng bùn núi lửa Electron tràn xuống qua Puyallup và đi xa tới Sumner&amp;#44; WA. Hàng nghìn năm trước đó&amp;#44; nhiều lahar đã di chuyển dọc theo các dòng sông địa phương và vươn tới tận Auburn. &lt;b&gt;Một số thị trấn (NE Tacoma&amp;#44; Orting&amp;#44; và Puyallup) được xây dựng trên các lớp trầm tích của lahar.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Trên khắp Quận King&amp;#44; mùa đông có thể mang đến nền nhiệt độ âm&amp;#44; đóng băng đường xá và nguy cơ xuất hiện các trận bão lớn. Tuyết rơi thường xuyên với tần suất cao hơn tại những khu vực ở độ cao hơn. &lt;b&gt;Những cơn bão mùa đông có thể mang theo những trận gió mạnh đủ sức quật ngã cây cối và gây nên tình trạng mất điện.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hiện tượng tuyết rơi nhiều có thể làm gián đoạn giao thông vận tải&amp;#44; các dịch vụ an toàn công cộng&amp;#44; và tiện ích sinh hoạt. &lt;b&gt;Điện có thể bị cắt trong nhiều ngày.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Khu vực Tây Bắc Thái Bình Dương sẽ phải đối mặt với nhiều cơn bão khắc nghiệt hơn trong vòng 50 năm tới&lt;/b&gt;. Chúng có thể mang theo gió mạnh&amp;#44; mưa lớn&amp;#44; gây nên lũ lụt. Các hoạt động mùa đông có thể sẽ bị ảnh hưởng. Năm 2015 chứng kiến lượng tuyết rơi thấp nhất trong lịch sử chỉ với 4% mức trung bình. Mùa đông ấm áp sẽ dẫn đến tình trạng hạn hán trên toàn bang. Bấm vào hình ảnh để tìm hiểu thêm.  &lt;br&gt;
+&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Winter.jpg" alt="Climate Change Winter Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Các nhà khí tượng học đã có bước tiến lớn trong việc dự báo các cơn bão tuyết. &lt;b&gt;Hãy chú ý theo dõi dự báo thời tiết địa phương và đăng ký nhận tin từ các hệ thống báo động và cảnh báo &lt;/b&gt;(&lt;a href=http://alert.seattle.gov/ target=_blank&gt;Cảnh báo Seattle&lt;/a&gt; và &lt;a href=http://www.kingcounty.gov/depts/emergency-management/alert-king-county.aspx target=_blank&gt;Cảnh báo Quận King&lt;/a&gt;) để đảm bảo bạn được cập nhật thông tin về tình trạng thời tiết khắc nghiệt sắp diễn ra.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;CHUẨN BỊ NHU YẾU PHẨM – Tích trữ nhiên liệu dự phòng và các vật dụng khẩn cấp &lt;/b&gt; để có thể sống sót trong nhiều ngày mà không có điện&amp;#44; máy sưởi và nước nóng. Cân nhắc mua một chiếc máy phát điện và tuân thủ các tiêu chuẩn về an toàn.&lt;/li&gt;&lt;li&gt;&lt;b&gt;NÂNG CẤP CĂN NHÀ CỦA BẠN&lt;/b&gt; - Lắp đặt cửa chống bão. Cách nhiệt cho tường&amp;#44; gác mái và đường ống. Dán và bịt kín các khe cửa ra vào và cửa sổ. Để vòi nước chảy nhỏ giọt trong những ngày thời tiết lạnh nhằm tránh đường ống bị đóng băng. &lt;b&gt;Tìm hiểu cách tắt van nước (trong trường hợp đường ống bị vỡ)&lt;/b&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;NÂNG CẤP PHƯƠNG TIỆN CỦA BẠN&lt;/b&gt; - Giữ nhiên liệu tối thiểu ở mức nửa bình. Kiểm tra pin&amp;#44; hệ thống đánh lửa&amp;#44; bộ tản nhiệt&amp;#44; đèn&amp;#44; phanh và bánh xe. Đổ đầy bình chứa bằng chất chống đông&amp;#44; dầu và dung dịch làm sạch cửa kính. &lt;b&gt;Giữ vật dụng khẩn cấp cho mùa đông trong xe tải của bạn.&lt;/b&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;NẮM THÔNG TIN&lt;/b&gt; - Theo dõi tin tức địa phương qua vô tuyến&amp;#44; thiết bị di động&amp;#44; hoặc đài chạy bằng pin. Tuân thủ hướng dẫn khẩn cấp và chú ý đến các khuyến nghị di chuyển.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;TRÁNH DI CHUYỂN&lt;/b&gt; - Nếu bắt buộc phải lái xe&amp;#44; hãy đổ đầy bình xăng&amp;#44; bám theo đường chính&amp;#44; và thông báo cho mọi người về hành trình của bạn. Di chuyển chậm. Nếu bị mắc kẹt&amp;#44; hãy gọi giúp đỡ&amp;#44; bật đèn cứu nạn và ở yên trong xe. Đừng bước chân ra ngoài trừ phi gần đó có nơi trú ẩn.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;NHẬN BIẾT NGUY CƠ&lt;/b&gt;- 
+&lt;ul&gt;
+&lt;li&gt;&lt;b&gt;Mất nhiệt&lt;/b&gt; - Nếu bạn nhận thấy những dấu hiệu&amp;#44; hãy nhờ sự giúp đỡ y tế ngay lập tức. Để biết về triệu chứng và các thông tin khác&amp;#44; hãy bấm vào &lt;a href=https://www.cdc.gov/disasters/winter/staysafe/hypothermia.html target=_blank&gt;đây&lt;/a&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Ngộ độc khí CO&lt;/b&gt; - Tình trạng này xảy ra khi bạn đốt các nhiên liệu như khí ga&amp;#44; dầu&amp;#44; dầu hỏa&amp;#44; gỗ&amp;#44; hoặc than đá trong một không gian kín. Hàng trăm người đã vô tình thiệt mạng mỗi năm. Tìm hiểu thêm &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/carbon-monoxide.aspx target=_blank&gt;tại đây&lt;/a&gt;.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;li&gt;&lt;b&gt;TRÁNH XA HIỂM HOẠ&lt;/b&gt; - Tránh xa các đường dây điện bị đứt&amp;#44; ngập lụt&amp;#44; đường xá&amp;#44; và các công trình khác bị suy yếu do tuyết và đá dày.&lt;/li&gt;&lt;/ul&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Winter_during.jpg" alt="This is a panel of four images of what to do during bad winter weather. Stay Tuned&amp;#44; Stay Inside&amp;#44; Know Risks&amp;#44; and Avoid Hazards." title="During Winter Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;Bổ sung các vật dụng khẩn cấp&lt;/b&gt;. Sẵn sàng trong trường hợp một cơn bão khác ập đến.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Cải thiện kế hoạch gia đình&lt;/b&gt; - Điều gì có tác dụng? Điều gì cần cải thiện?&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Nói chuyện với hàng xóm&lt;/b&gt;. Cùng nhau chia sẻ mẹo hay và ý tưởng.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Tìm hiểu thêm về tình trạng mùa đông và cách chuẩn bị: 
+&lt;ul&gt;&lt;li&gt;
+&lt;a href=http://takewinterbystorm.org target=_blank&gt;Đối Phó Với Bão Mùa Đông&lt;/a&gt; - Mẹo chuẩn bị và thông tin cập nhật cho Miền Tây Washington&lt;/li&gt;
+&lt;li&gt;
+&lt;a href=http://kingcounty.gov/depts/transportation/metro/alerts-updates/winter.aspx target=_blank&gt;Tuyến Xe Điện Quận King Vào Mùa Đông&lt;/a&gt; - Các liên kết dẫn tới ứng dụng lập kế hoạch du lịch trong mùa đông và cảnh báo thời tiết &lt;/li&gt;
+&lt;li&gt;
+&lt;a href=https://www.seattle.gov/transportation/winterweather.htm target=_blank&gt;Sở Giao Thông Vận Tải Seattle&lt;/a&gt; - Kiểm tra những nơi đã được dọn tuyết và thông tin khác về điều kiện đường xá &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;Một chuỗi mưa bão&amp;#44; đá và tuyết bắt đầu từ ngày 26 tháng Mười Hai&amp;#44; 1996 đã khiến 16 người thiệt mạng trên toàn bang và gây ra thiệt hại lên tới 57 triệu USD tại Quận King và Seattle&lt;/b&gt;. Hai cơn bão — một cơn trút xuống lớp tuyết ẩm dày 6-12 inch và cơn còn lại là 10 inch — kéo theo đó là mưa lớn khiến nhiều nhà để xe đổ sập&amp;#44; che phủ thuyền neo đậu và cắt đứt đường dây điện. Lần đầu tiên trong lịch sử&amp;#44; Metro Transit đã phải ngưng hoàn toàn dịch vụ. Băng đá và tuyết tan góp phần gây nên tình trạng lũ lụt và sạt lở đất trong tuần kế tiếp. Bạn đã sẵn sàng nếu một cơn bão như vậy xảy ra thêm lần nữa?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Đừng để những cơn mưa và mùa đông đánh lừa bạn&amp;#44; &lt;b&gt;mùa hè tại Quận King có thể rất NÓNG. Đôi khi nhiệt độ có thể lên tới đến hơn 90 độ F trong nhiều ngày liên tiếp&lt;/b&gt;. Sấm chớp&amp;#44; bão gió&amp;#44; cháy rừng và những đợt nóng là điều có thể xảy ra trên toàn khu vực.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nắng nóng khắc nghiệt có thể kéo dài nhiều ngày&amp;#44; khiến số lượng các bệnh về nhiệt gia tăng bao gồm KIỆT SỨC DO NÓNG và SỐC NHIỆT. Nhiệt độ cao&amp;#44; khô và nguy cơ sét đánh cao có thể dẫn đến tình trạng cháy rừng.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Tháng Bảy năm 2015 là tháng nóng nhất trong lịch sử! &lt;b&gt;Nhiệt độ trung bình năm được dự đoán sẽ tăng từ 3-10 độ F đến năm 2100&lt;/b&gt;. Người dân Washington sẽ chứng kiến số lượng các cơn mưa mùa hè ít hơn&amp;#44; nhưng lượng mưa sẽ nặng hơn (mưa trút xuống). Bấm vào hình ảnh để tìm hiểu thêm. &lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target=_blank&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="Climate Change Storm Infographic"&gt;
+&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kiệt sức do nóng và sốc nhiệt là các bệnh lý nghiêm trọng có thể xảy ra khi một người tiếp xúc với hơi nóng cực độ.&lt;/p&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;DẤU HIỆU KIỆT SỨC DO NÓNG&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;Đổ mồ hôi nhiều&lt;/li&gt;
+&lt;li&gt;Mệt mỏi&lt;/li&gt;
+&lt;li&gt;Mạch đập yếu&lt;/li&gt;
+&lt;li&gt;Bị ngất xỉu&lt;/li&gt;
+&lt;li&gt;Nôn Mửa&lt;/li&gt;
+&lt;li&gt;Da tái xanh&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;
+&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;
+&lt;b&gt;DẤU HIỆU SỐC NHIỆT&lt;/b&gt;:
+&lt;ul&gt;
+&lt;li&gt;Nhiệt độ cơ thể cao (từ 103 độ F trở lên)&lt;/li&gt;
+&lt;li&gt;Da nóng và khô&lt;/li&gt;
+&lt;li&gt;Mạch đập nhanh và mạnh&lt;/li&gt;
+&lt;li&gt;Có thể ngất xỉu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Người già&amp;#44; trẻ em và những người mắc bệnh về tâm thần và các bệnh mãn tính có nguy cơ gặp vấn đề về nhiệt cao hơn.
+&lt;ol&gt;&lt;li&gt;&lt;b&gt;NHẬN BIẾT DẤU HIỆU&lt;/b&gt; - Các bệnh về nhiệt có thể xảy ra nhanh chóng. Biết và nắm được những người nào xung quanh bạn có thể gặp nguy hiểm. &lt;/li&gt;&lt;li&gt;&lt;b&gt;NẮM THÔNG TIN &lt;/b&gt; - Lắng nghe tin tức địa phương để nắm được thông tin chung và vị trí của &lt;b&gt;trung tâm làm mát&lt;/b&gt; (khu vực công cộng có thể được sử dụng để người dân tránh nóng).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;Ở NƠI MÁT MẺ&lt;/b&gt; - Ở trong nhà và nếu có thể&amp;#44; ở những nơi có điều hòa nhiệt độ (trung tâm mua sắm&amp;#44; thư viện&amp;#44; rạp chiếu phim&amp;#44; v.v.). Hạn chế hoạt động ngoài trời.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;BẢO VỆ DA&lt;/b&gt; - Mặc quần áo nhẹ&amp;#44; mào sắc tươi sáng&amp;#44; thoáng mát. Một chiếc mũ rộng vàng&amp;#44; kính râm và kem chống nắng sẽ rất có ích.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;UỐNG NƯỚC&lt;/b&gt; - Uống nhiều chất lỏng (tránh xa cafein&amp;#44; rượu bia và đồ uống có đường) và mang theo một chai nước.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;QUAN TÂM ĐẾN MỌI NGƯỜI&lt;/b&gt; - Đưa trẻ nhỏ và thú nuôi ra khỏi xe nóng. Thường xuyên kiểm tra các gia đình&amp;#44; bạn bè và hàng xóm có nguy cơ cao.&lt;/li&gt;&lt;/ul&gt;
+&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Summer_during.jpg" alt="This is a panel of three images of what to do during bad summer weather. Stay Cool&amp;#44; Protect Skin&amp;#44; and Drink Water." title="During Summer Weather Image"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Sử dụng rèm để &lt;b&gt;che chắn cửa sổ và giữa không khí mát bên trong&lt;/b&gt;.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Cân nhắc mua hệ thống điều hòa nhiệt độ&lt;/b&gt; và/hoặc bít các khe cửa nơi khí nóng có thể tràn vào.&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;GIẢI PHÁP TIẾT KIỆM&lt;/b&gt;: Lắp đặt tấm phản nhiệt (đặt giữa cửa sổ và rèm)&amp;#44; như tấm bìa phủ giấy bạc để phản chiếu lại nhiệt ra bên ngoài. Bấm &lt;a href=http://www.instructables.com/id/Heat-blocking-curtains/ target=_blank&gt;vào đây&lt;/a&gt; để xem hướng dẫn tự làm tại nhà.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Để biết thêm thông tin về cách làm mát và an toàn&amp;#44; hãy truy cập trang &lt;a href=http://www.kingcounty.gov/depts/health/emergency-preparedness/preparing-yourself/hot-weather.aspx target=_blank&gt;Thời Tiết Nắng Nóng&lt;/a&gt; của Quận King.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vào năm 2015&amp;#44; Quận King đã có số ngày vượt quá ngưỡng nhiệt 90 F nhiều kỷ lục. &lt;b&gt;Tháng Bảy&amp;#44; 2015 là tháng nóng nhất được ghi nhận trong lịch sử Quận King!&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>text-vi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -13276,6 +13993,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -14040,7 +14771,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -14067,6 +14798,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="683">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -15085,13 +15818,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L292"/>
+  <dimension ref="A1:M292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15101,9 +15834,10 @@
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="8" max="10" width="53.1640625" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.83203125" style="21"/>
+    <col min="13" max="13" width="53.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15140,8 +15874,11 @@
       <c r="L1" s="20" t="s">
         <v>1224</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -15175,8 +15912,11 @@
       <c r="L2" s="21" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -15210,8 +15950,11 @@
       <c r="L3" s="21" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="1" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -15245,12 +15988,15 @@
       <c r="L4" s="21" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="1" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -15284,8 +16030,11 @@
       <c r="L6" s="21" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="1" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -15319,8 +16068,11 @@
       <c r="L7" s="21" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="1" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -15354,8 +16106,11 @@
       <c r="L8" s="21" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="1" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -15389,8 +16144,11 @@
       <c r="L9" s="21" t="s">
         <v>1016</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="1" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -15424,12 +16182,15 @@
       <c r="L10" s="21" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="1" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -15463,8 +16224,11 @@
       <c r="L12" s="21" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="1" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -15498,8 +16262,11 @@
       <c r="L13" s="21" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="1" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -15533,12 +16300,15 @@
       <c r="L14" s="21" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="1" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -15572,8 +16342,11 @@
       <c r="L16" s="21" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="1" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -15607,8 +16380,11 @@
       <c r="L17" s="21" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -15642,8 +16418,11 @@
       <c r="L18" s="21" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="1" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -15677,8 +16456,11 @@
       <c r="L19" s="21" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="1" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -15712,8 +16494,11 @@
       <c r="L20" s="21" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="1" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -15747,12 +16532,15 @@
       <c r="L21" s="21" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -15786,8 +16574,11 @@
       <c r="L23" s="20" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="1" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -15821,8 +16612,11 @@
       <c r="L24" s="21" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" s="1" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -15856,8 +16650,11 @@
       <c r="L25" s="21" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" s="1" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -15891,8 +16688,11 @@
       <c r="L26" s="21" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="1" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -15926,8 +16726,11 @@
       <c r="L27" s="21" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="1" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -15961,8 +16764,11 @@
       <c r="L28" s="21" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" s="1" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -15996,8 +16802,11 @@
       <c r="L29" s="21" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -16031,8 +16840,11 @@
       <c r="L30" s="21" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="1" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -16066,12 +16878,15 @@
       <c r="L31" s="21" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" s="1" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -16105,8 +16920,11 @@
       <c r="L33" s="21" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -16140,8 +16958,11 @@
       <c r="L34" s="21" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="1" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -16175,8 +16996,11 @@
       <c r="L35" s="21" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" s="1" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -16210,8 +17034,11 @@
       <c r="L36" s="21" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -16245,12 +17072,15 @@
       <c r="L37" s="21" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -16284,12 +17114,15 @@
       <c r="L39" s="21" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" s="1" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D40" s="3"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -16320,8 +17153,11 @@
       <c r="L41" s="21" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" s="1" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -16352,8 +17188,11 @@
       <c r="L42" s="21" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" s="1" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -16384,12 +17223,15 @@
       <c r="L43" s="20" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D44" s="3"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -16420,8 +17262,11 @@
       <c r="L45" s="1" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" s="1" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -16452,8 +17297,11 @@
       <c r="L46" s="1" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="1" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -16484,8 +17332,11 @@
       <c r="L47" s="1" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="1" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -16516,8 +17367,11 @@
       <c r="L48" s="1" t="s">
         <v>1048</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -16548,8 +17402,11 @@
       <c r="L49" s="1" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -16580,8 +17437,11 @@
       <c r="L50" s="1" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -16612,8 +17472,11 @@
       <c r="L51" s="1" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -16644,8 +17507,11 @@
       <c r="L52" s="1" t="s">
         <v>1052</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" s="1" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -16676,8 +17542,11 @@
       <c r="L53" s="1" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M53" s="1" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -16708,8 +17577,11 @@
       <c r="L54" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" s="1" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -16740,8 +17612,11 @@
       <c r="L55" s="1" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" s="1" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -16772,8 +17647,11 @@
       <c r="L56" s="1" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -16804,8 +17682,11 @@
       <c r="L57" s="1" t="s">
         <v>1057</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" s="1" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -16836,8 +17717,11 @@
       <c r="L58" s="1" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" s="1" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -16868,8 +17752,11 @@
       <c r="L59" s="1" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" s="1" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -16900,8 +17787,11 @@
       <c r="L60" s="1" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -16932,8 +17822,11 @@
       <c r="L61" s="1" t="s">
         <v>1061</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61" s="1" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -16964,8 +17857,11 @@
       <c r="L62" s="1" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62" s="1" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>47</v>
       </c>
@@ -16996,8 +17892,11 @@
       <c r="L63" s="1" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" s="1" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -17028,8 +17927,11 @@
       <c r="L64" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" s="1" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -17060,8 +17962,11 @@
       <c r="L65" s="1" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" s="1" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -17092,8 +17997,11 @@
       <c r="L66" s="1" t="s">
         <v>1066</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -17124,8 +18032,11 @@
       <c r="L67" s="1" t="s">
         <v>1067</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -17156,8 +18067,11 @@
       <c r="L68" s="1" t="s">
         <v>1068</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" s="1" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -17188,8 +18102,11 @@
       <c r="L69" s="1" t="s">
         <v>1069</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" s="1" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -17220,8 +18137,11 @@
       <c r="L70" s="1" t="s">
         <v>1070</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" s="1" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -17252,8 +18172,11 @@
       <c r="L71" s="1" t="s">
         <v>1071</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" s="1" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -17284,8 +18207,11 @@
       <c r="L72" s="1" t="s">
         <v>1072</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M72" s="1" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -17316,8 +18242,11 @@
       <c r="L73" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" s="1" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>47</v>
       </c>
@@ -17348,8 +18277,11 @@
       <c r="L74" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" s="1" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -17380,8 +18312,11 @@
       <c r="L75" s="1" t="s">
         <v>1075</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -17412,8 +18347,11 @@
       <c r="L76" s="1" t="s">
         <v>1076</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" s="1" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>47</v>
       </c>
@@ -17444,8 +18382,11 @@
       <c r="L77" s="1" t="s">
         <v>1077</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M77" s="1" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>47</v>
       </c>
@@ -17476,8 +18417,11 @@
       <c r="L78" s="1" t="s">
         <v>1078</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M78" s="1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -17508,8 +18452,11 @@
       <c r="L79" s="1" t="s">
         <v>1079</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M79" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -17540,8 +18487,11 @@
       <c r="L80" s="1" t="s">
         <v>1080</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M80" s="1" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -17572,8 +18522,11 @@
       <c r="L81" s="1" t="s">
         <v>1081</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M81" s="1" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>47</v>
       </c>
@@ -17604,8 +18557,11 @@
       <c r="L82" s="1" t="s">
         <v>1082</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M82" s="1" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -17636,8 +18592,11 @@
       <c r="L83" s="1" t="s">
         <v>1083</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M83" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -17668,8 +18627,11 @@
       <c r="L84" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M84" s="1" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -17700,8 +18662,11 @@
       <c r="L85" s="1" t="s">
         <v>1085</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M85" s="1" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>47</v>
       </c>
@@ -17732,8 +18697,11 @@
       <c r="L86" s="1" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M86" s="1" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>47</v>
       </c>
@@ -17764,8 +18732,11 @@
       <c r="L87" s="1" t="s">
         <v>1087</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M87" s="1" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>47</v>
       </c>
@@ -17796,8 +18767,11 @@
       <c r="L88" s="1" t="s">
         <v>1088</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M88" s="1" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -17828,8 +18802,11 @@
       <c r="L89" s="1" t="s">
         <v>1089</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M89" s="1" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -17860,8 +18837,11 @@
       <c r="L90" s="1" t="s">
         <v>1090</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M90" s="1" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -17892,8 +18872,11 @@
       <c r="L91" s="1" t="s">
         <v>1091</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M91" s="1" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>47</v>
       </c>
@@ -17924,8 +18907,11 @@
       <c r="L92" s="1" t="s">
         <v>1092</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M92" s="1" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>47</v>
       </c>
@@ -17956,8 +18942,11 @@
       <c r="L93" s="1" t="s">
         <v>1093</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M93" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>47</v>
       </c>
@@ -17988,8 +18977,11 @@
       <c r="L94" s="1" t="s">
         <v>1094</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M94" s="1" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -18020,8 +19012,11 @@
       <c r="L95" s="1" t="s">
         <v>1095</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M95" s="1" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -18052,8 +19047,11 @@
       <c r="L96" s="1" t="s">
         <v>1096</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M96" s="1" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -18084,8 +19082,11 @@
       <c r="L97" s="1" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M97" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -18116,8 +19117,11 @@
       <c r="L98" s="1" t="s">
         <v>1098</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M98" s="1" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -18148,8 +19152,11 @@
       <c r="L99" s="1" t="s">
         <v>1099</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M99" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -18180,8 +19187,11 @@
       <c r="L100" s="1" t="s">
         <v>1100</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M100" s="1" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>47</v>
       </c>
@@ -18212,8 +19222,11 @@
       <c r="L101" s="1" t="s">
         <v>1101</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M101" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>47</v>
       </c>
@@ -18244,8 +19257,11 @@
       <c r="L102" s="1" t="s">
         <v>1102</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M102" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -18276,8 +19292,11 @@
       <c r="L103" s="1" t="s">
         <v>1103</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M103" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>47</v>
       </c>
@@ -18308,8 +19327,11 @@
       <c r="L104" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M104" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -18340,8 +19362,11 @@
       <c r="L105" s="1" t="s">
         <v>1105</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M105" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -18372,8 +19397,11 @@
       <c r="L106" s="1" t="s">
         <v>1106</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M106" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -18404,8 +19432,11 @@
       <c r="L107" s="1" t="s">
         <v>1107</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M107" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>47</v>
       </c>
@@ -18436,8 +19467,11 @@
       <c r="L108" s="1" t="s">
         <v>1108</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M108" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>47</v>
       </c>
@@ -18468,12 +19502,15 @@
       <c r="L109" s="1" t="s">
         <v>1109</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M109" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D110" s="3"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>53</v>
       </c>
@@ -18504,24 +19541,29 @@
       <c r="L111" s="21" t="s">
         <v>1110</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M111" s="22" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E112" s="13"/>
       <c r="H112" s="14"/>
       <c r="I112" s="16"/>
       <c r="J112" s="14"/>
       <c r="K112" s="21"/>
       <c r="L112" s="21"/>
-    </row>
-    <row r="113" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M112" s="14"/>
+    </row>
+    <row r="113" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E113" s="13"/>
       <c r="H113" s="14"/>
       <c r="I113" s="16"/>
       <c r="J113" s="14"/>
       <c r="K113" s="21"/>
       <c r="L113" s="21"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M113" s="14"/>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -18555,8 +19597,11 @@
       <c r="L114" s="21" t="s">
         <v>1111</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M114" s="1" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -18590,8 +19635,11 @@
       <c r="L115" s="21" t="s">
         <v>1111</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M115" s="1" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -18625,8 +19673,11 @@
       <c r="L116" s="21" t="s">
         <v>1112</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M116" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -18660,8 +19711,11 @@
       <c r="L117" s="21" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M117" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -18695,8 +19749,11 @@
       <c r="L118" s="21" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M118" s="1" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -18730,8 +19787,11 @@
       <c r="L119" s="21" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M119" s="1" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -18765,8 +19825,11 @@
       <c r="L120" s="21" t="s">
         <v>1116</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M120" s="1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -18800,12 +19863,15 @@
       <c r="L121" s="21" t="s">
         <v>1117</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M121" s="1" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D122" s="4"/>
       <c r="I122" s="8"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -18839,8 +19905,11 @@
       <c r="L123" s="21" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M123" s="1" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -18874,8 +19943,11 @@
       <c r="L124" s="21" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M124" s="1" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -18909,8 +19981,11 @@
       <c r="L125" s="21" t="s">
         <v>1119</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M125" s="1" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -18944,8 +20019,11 @@
       <c r="L126" s="21" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M126" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -18979,8 +20057,11 @@
       <c r="L127" s="21" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M127" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -19014,8 +20095,11 @@
       <c r="L128" s="21" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M128" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -19049,8 +20133,11 @@
       <c r="L129" s="21" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M129" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -19084,12 +20171,15 @@
       <c r="L130" s="21" t="s">
         <v>1121</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M130" s="1" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D131" s="4"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -19123,8 +20213,11 @@
       <c r="L132" s="21" t="s">
         <v>1122</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M132" s="1" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -19158,8 +20251,11 @@
       <c r="L133" s="21" t="s">
         <v>1123</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M133" s="1" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -19193,8 +20289,11 @@
       <c r="L134" s="21" t="s">
         <v>1124</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M134" s="1" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -19228,8 +20327,11 @@
       <c r="L135" s="21" t="s">
         <v>1125</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M135" s="1" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -19263,8 +20365,11 @@
       <c r="L136" s="21" t="s">
         <v>1126</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M136" s="1" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -19298,8 +20403,11 @@
       <c r="L137" s="21" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M137" s="1" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -19333,8 +20441,11 @@
       <c r="L138" s="21" t="s">
         <v>1128</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M138" s="1" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -19368,8 +20479,11 @@
       <c r="L139" s="21" t="s">
         <v>1129</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M139" s="1" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -19403,8 +20517,11 @@
       <c r="L140" s="21" t="s">
         <v>1130</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M140" s="1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -19438,8 +20555,11 @@
       <c r="L141" s="21" t="s">
         <v>1131</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M141" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -19473,8 +20593,11 @@
       <c r="L142" s="21" t="s">
         <v>1132</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M142" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -19508,8 +20631,11 @@
       <c r="L143" s="21" t="s">
         <v>1133</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M143" s="1" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -19543,8 +20669,11 @@
       <c r="L144" s="21" t="s">
         <v>1134</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M144" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -19578,8 +20707,11 @@
       <c r="L145" s="21" t="s">
         <v>1135</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M145" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -19613,12 +20745,15 @@
       <c r="L146" s="21" t="s">
         <v>1136</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M146" s="1" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
       <c r="I147" s="8"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -19652,8 +20787,11 @@
       <c r="L148" s="21" t="s">
         <v>1137</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M148" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -19687,8 +20825,11 @@
       <c r="L149" s="21" t="s">
         <v>1138</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M149" s="1" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -19722,8 +20863,11 @@
       <c r="L150" s="21" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M150" s="1" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -19757,8 +20901,11 @@
       <c r="L151" s="21" t="s">
         <v>1140</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M151" s="1" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -19792,12 +20939,15 @@
       <c r="L152" s="21" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M152" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D153" s="4"/>
       <c r="I153" s="8"/>
     </row>
-    <row r="154" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
         <v>7</v>
       </c>
@@ -19828,12 +20978,15 @@
       <c r="L154" s="21" t="s">
         <v>1142</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M154" s="1" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D155" s="4"/>
       <c r="I155" s="8"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -19867,12 +21020,15 @@
       <c r="L156" s="20" t="s">
         <v>1143</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M156" s="22" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D157" s="4"/>
       <c r="I157" s="8"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>47</v>
       </c>
@@ -19903,8 +21059,11 @@
       <c r="L158" s="21" t="s">
         <v>1144</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M158" s="1" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>47</v>
       </c>
@@ -19935,8 +21094,11 @@
       <c r="L159" s="20" t="s">
         <v>1145</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M159" s="1" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>47</v>
       </c>
@@ -19967,12 +21129,15 @@
       <c r="L160" s="20" t="s">
         <v>1146</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M160" s="1" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D161" s="4"/>
       <c r="I161" s="8"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>47</v>
       </c>
@@ -20006,8 +21171,11 @@
       <c r="L162" s="1" t="s">
         <v>1147</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M162" s="1" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -20041,8 +21209,11 @@
       <c r="L163" s="1" t="s">
         <v>1148</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M163" s="1" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -20076,8 +21247,11 @@
       <c r="L164" s="1" t="s">
         <v>1149</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M164" s="1" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>47</v>
       </c>
@@ -20111,8 +21285,11 @@
       <c r="L165" s="1" t="s">
         <v>1150</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M165" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -20146,8 +21323,11 @@
       <c r="L166" s="1" t="s">
         <v>1151</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M166" s="1" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>47</v>
       </c>
@@ -20181,8 +21361,11 @@
       <c r="L167" s="1" t="s">
         <v>1152</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M167" s="1" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>47</v>
       </c>
@@ -20216,8 +21399,11 @@
       <c r="L168" s="1" t="s">
         <v>1153</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M168" s="1" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>47</v>
       </c>
@@ -20251,8 +21437,11 @@
       <c r="L169" s="1" t="s">
         <v>1154</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M169" s="1" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -20286,8 +21475,11 @@
       <c r="L170" s="1" t="s">
         <v>1155</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M170" s="1" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>47</v>
       </c>
@@ -20321,8 +21513,11 @@
       <c r="L171" s="1" t="s">
         <v>1156</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M171" s="1" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>47</v>
       </c>
@@ -20356,8 +21551,11 @@
       <c r="L172" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M172" s="1" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>47</v>
       </c>
@@ -20391,8 +21589,11 @@
       <c r="L173" s="1" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M173" s="1" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -20426,8 +21627,11 @@
       <c r="L174" s="1" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M174" s="1" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -20461,8 +21665,11 @@
       <c r="L175" s="1" t="s">
         <v>1160</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M175" s="1" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>47</v>
       </c>
@@ -20496,12 +21703,15 @@
       <c r="L176" s="1" t="s">
         <v>1161</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M176" s="1" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D177" s="4"/>
       <c r="I177" s="8"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>53</v>
       </c>
@@ -20532,24 +21742,29 @@
       <c r="L178" s="21" t="s">
         <v>1162</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M178" s="1" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E179" s="13"/>
       <c r="H179" s="14"/>
       <c r="I179" s="16"/>
       <c r="J179" s="14"/>
       <c r="K179" s="21"/>
       <c r="L179" s="21"/>
-    </row>
-    <row r="180" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M179" s="14"/>
+    </row>
+    <row r="180" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E180" s="13"/>
       <c r="H180" s="14"/>
       <c r="I180" s="16"/>
       <c r="J180" s="14"/>
       <c r="K180" s="21"/>
       <c r="L180" s="21"/>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M180" s="14"/>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -20583,8 +21798,11 @@
       <c r="L181" s="18" t="s">
         <v>1163</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M181" s="18" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -20618,8 +21836,11 @@
       <c r="L182" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M182" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -20653,8 +21874,11 @@
       <c r="L183" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M183" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -20688,8 +21912,11 @@
       <c r="L184" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M184" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -20723,8 +21950,11 @@
       <c r="L185" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M185" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -20758,8 +21988,11 @@
       <c r="L186" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M186" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -20793,8 +22026,11 @@
       <c r="L187" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M187" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -20828,8 +22064,11 @@
       <c r="L188" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M188" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -20863,8 +22102,11 @@
       <c r="L189" s="18" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M189" s="18" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C190" s="8"/>
       <c r="D190" s="15"/>
       <c r="E190"/>
@@ -20872,8 +22114,9 @@
       <c r="H190" s="8"/>
       <c r="I190" s="8"/>
       <c r="J190" s="18"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M190" s="18"/>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -20907,8 +22150,11 @@
       <c r="L191" s="1" t="s">
         <v>1165</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M191" s="1" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -20942,8 +22188,11 @@
       <c r="L192" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M192" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -20977,8 +22226,11 @@
       <c r="L193" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M193" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -21012,8 +22264,11 @@
       <c r="L194" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M194" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -21047,8 +22302,11 @@
       <c r="L195" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M195" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -21082,8 +22340,11 @@
       <c r="L196" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M196" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -21117,8 +22378,11 @@
       <c r="L197" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M197" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -21152,8 +22416,11 @@
       <c r="L198" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M198" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -21187,14 +22454,17 @@
       <c r="L199" s="1" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M199" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C200" s="8"/>
       <c r="D200" s="15"/>
       <c r="E200"/>
       <c r="I200" s="8"/>
     </row>
-    <row r="201" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A201" s="8" t="s">
         <v>7</v>
       </c>
@@ -21225,14 +22495,17 @@
       <c r="L201" s="21" t="s">
         <v>1167</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M201" s="1" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="D202" s="5"/>
       <c r="I202" s="8"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -21266,12 +22539,15 @@
       <c r="L203" s="20" t="s">
         <v>1168</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M203" s="22" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D204" s="5"/>
       <c r="I204" s="8"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>47</v>
       </c>
@@ -21302,8 +22578,11 @@
       <c r="L205" s="20" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M205" s="1" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>47</v>
       </c>
@@ -21334,8 +22613,11 @@
       <c r="L206" s="21" t="s">
         <v>1170</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M206" s="1" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>47</v>
       </c>
@@ -21366,8 +22648,11 @@
       <c r="L207" s="21" t="s">
         <v>1171</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M207" s="1" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>47</v>
       </c>
@@ -21398,12 +22683,15 @@
       <c r="L208" s="21" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M208" s="1" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D209" s="5"/>
       <c r="I209" s="8"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>53</v>
       </c>
@@ -21434,8 +22722,11 @@
       <c r="L210" s="21" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M210" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>53</v>
       </c>
@@ -21466,8 +22757,11 @@
       <c r="L211" s="21" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M211" s="1" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>53</v>
       </c>
@@ -21498,8 +22792,11 @@
       <c r="L212" s="21" t="s">
         <v>1175</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M212" s="1" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>53</v>
       </c>
@@ -21530,8 +22827,11 @@
       <c r="L213" s="21" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M213" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>53</v>
       </c>
@@ -21562,8 +22862,11 @@
       <c r="L214" s="21" t="s">
         <v>1177</v>
       </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M214" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>53</v>
       </c>
@@ -21594,8 +22897,11 @@
       <c r="L215" s="21" t="s">
         <v>1177</v>
       </c>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M215" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>53</v>
       </c>
@@ -21626,8 +22932,11 @@
       <c r="L216" s="21" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M216" s="1" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>53</v>
       </c>
@@ -21658,8 +22967,11 @@
       <c r="L217" s="21" t="s">
         <v>1179</v>
       </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M217" s="1" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>53</v>
       </c>
@@ -21690,8 +23002,11 @@
       <c r="L218" s="21" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M218" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>53</v>
       </c>
@@ -21722,24 +23037,29 @@
       <c r="L219" s="21" t="s">
         <v>1181</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M219" s="1" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E220" s="13"/>
       <c r="H220" s="14"/>
       <c r="I220" s="16"/>
       <c r="J220" s="14"/>
       <c r="K220" s="21"/>
       <c r="L220" s="21"/>
-    </row>
-    <row r="221" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M220" s="14"/>
+    </row>
+    <row r="221" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E221" s="13"/>
       <c r="H221" s="14"/>
       <c r="I221" s="16"/>
       <c r="J221" s="14"/>
       <c r="K221" s="21"/>
       <c r="L221" s="21"/>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M221" s="14"/>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -21773,8 +23093,11 @@
       <c r="L222" s="21" t="s">
         <v>1182</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M222" s="1" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -21808,8 +23131,11 @@
       <c r="L223" s="21" t="s">
         <v>1182</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M223" s="1" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -21843,8 +23169,11 @@
       <c r="L224" s="21" t="s">
         <v>1183</v>
       </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M224" s="1" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -21878,8 +23207,11 @@
       <c r="L225" s="21" t="s">
         <v>1184</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M225" s="1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -21913,12 +23245,15 @@
       <c r="L226" s="21" t="s">
         <v>1185</v>
       </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M226" s="1" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D227" s="6"/>
       <c r="I227" s="8"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>7</v>
       </c>
@@ -21952,8 +23287,11 @@
       <c r="L228" s="21" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M228" s="1" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>7</v>
       </c>
@@ -21987,8 +23325,11 @@
       <c r="L229" s="21" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M229" s="1" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>7</v>
       </c>
@@ -22022,8 +23363,11 @@
       <c r="L230" s="21" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M230" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>7</v>
       </c>
@@ -22057,12 +23401,15 @@
       <c r="L231" s="21" t="s">
         <v>1187</v>
       </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M231" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D232" s="6"/>
       <c r="I232" s="8"/>
     </row>
-    <row r="233" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A233" s="8" t="s">
         <v>7</v>
       </c>
@@ -22093,12 +23440,15 @@
       <c r="L233" s="21" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M233" s="1" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D234" s="6"/>
       <c r="I234" s="8"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>7</v>
       </c>
@@ -22129,12 +23479,15 @@
       <c r="L235" s="21" t="s">
         <v>1189</v>
       </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M235" s="23" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D236" s="6"/>
       <c r="I236" s="8"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>47</v>
       </c>
@@ -22162,8 +23515,11 @@
       <c r="L237" s="21" t="s">
         <v>1190</v>
       </c>
-    </row>
-    <row r="238" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M237" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>47</v>
       </c>
@@ -22191,8 +23547,11 @@
       <c r="L238" s="21" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="239" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M238" s="1" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>47</v>
       </c>
@@ -22220,12 +23579,15 @@
       <c r="L239" s="21" t="s">
         <v>1192</v>
       </c>
-    </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M239" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D240" s="6"/>
       <c r="I240" s="8"/>
     </row>
-    <row r="241" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>47</v>
       </c>
@@ -22253,12 +23615,15 @@
       <c r="L241" s="21" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M241" s="1" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D242" s="6"/>
       <c r="I242" s="8"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>53</v>
       </c>
@@ -22286,24 +23651,29 @@
       <c r="L243" s="21" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="244" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M243" s="1" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E244" s="13"/>
       <c r="H244" s="14"/>
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
       <c r="K244" s="14"/>
       <c r="L244" s="14"/>
-    </row>
-    <row r="245" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M244" s="14"/>
+    </row>
+    <row r="245" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E245" s="13"/>
       <c r="H245" s="14"/>
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
       <c r="K245" s="14"/>
       <c r="L245" s="14"/>
-    </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M245" s="14"/>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>7</v>
       </c>
@@ -22337,13 +23707,16 @@
       <c r="L246" s="1" t="s">
         <v>1195</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M246" s="1" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D247" s="7"/>
       <c r="K247" s="1"/>
       <c r="L247" s="1"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>7</v>
       </c>
@@ -22377,8 +23750,11 @@
       <c r="L248" s="1" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M248" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>7</v>
       </c>
@@ -22412,8 +23788,11 @@
       <c r="L249" s="1" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M249" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>7</v>
       </c>
@@ -22447,8 +23826,11 @@
       <c r="L250" s="1" t="s">
         <v>1198</v>
       </c>
-    </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M250" s="1" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>7</v>
       </c>
@@ -22482,13 +23864,16 @@
       <c r="L251" s="1" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M251" s="1" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D252" s="7"/>
       <c r="K252" s="1"/>
       <c r="L252" s="1"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>7</v>
       </c>
@@ -22522,13 +23907,16 @@
       <c r="L253" s="1" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M253" s="1" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D254" s="7"/>
       <c r="K254" s="1"/>
       <c r="L254" s="1"/>
     </row>
-    <row r="255" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>47</v>
       </c>
@@ -22559,8 +23947,11 @@
       <c r="L255" s="1" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="256" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M255" s="1" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>47</v>
       </c>
@@ -22591,8 +23982,11 @@
       <c r="L256" s="1" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="257" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M256" s="1" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>47</v>
       </c>
@@ -22623,8 +24017,11 @@
       <c r="L257" s="1" t="s">
         <v>1203</v>
       </c>
-    </row>
-    <row r="258" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M257" s="1" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>47</v>
       </c>
@@ -22655,13 +24052,16 @@
       <c r="L258" s="1" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M258" s="1" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D259" s="7"/>
       <c r="K259" s="1"/>
       <c r="L259" s="1"/>
     </row>
-    <row r="260" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>53</v>
       </c>
@@ -22692,24 +24092,29 @@
       <c r="L260" s="1" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="261" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M260" s="1" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E261" s="13"/>
       <c r="H261" s="14"/>
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
       <c r="K261" s="14"/>
       <c r="L261" s="14"/>
-    </row>
-    <row r="262" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M261" s="14"/>
+    </row>
+    <row r="262" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E262" s="13"/>
       <c r="H262" s="14"/>
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
       <c r="K262" s="14"/>
       <c r="L262" s="14"/>
-    </row>
-    <row r="263" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M262" s="14"/>
+    </row>
+    <row r="263" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>7</v>
       </c>
@@ -22740,12 +24145,15 @@
       <c r="L263" s="1" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M263" s="1" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D264" s="9"/>
       <c r="L264" s="1"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>7</v>
       </c>
@@ -22776,13 +24184,16 @@
       <c r="L265" s="1" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M265" s="1" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D266" s="9"/>
       <c r="K266" s="1"/>
       <c r="L266" s="1"/>
     </row>
-    <row r="267" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A267" s="8" t="s">
         <v>7</v>
       </c>
@@ -22813,15 +24224,18 @@
       <c r="L267" s="1" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M267" s="1" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="D268" s="9"/>
       <c r="K268" s="1"/>
       <c r="L268" s="1"/>
     </row>
-    <row r="269" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>7</v>
       </c>
@@ -22852,13 +24266,16 @@
       <c r="L269" s="1" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M269" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D270" s="9"/>
       <c r="K270" s="1"/>
       <c r="L270" s="1"/>
     </row>
-    <row r="271" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>47</v>
       </c>
@@ -22886,8 +24303,11 @@
       <c r="L271" s="1" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="272" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M271" s="1" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>47</v>
       </c>
@@ -22915,8 +24335,11 @@
       <c r="L272" s="1" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="273" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M272" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>47</v>
       </c>
@@ -22944,8 +24367,11 @@
       <c r="L273" s="1" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="274" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M273" s="1" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>47</v>
       </c>
@@ -22973,13 +24399,16 @@
       <c r="L274" s="1" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M274" s="1" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D275" s="9"/>
       <c r="K275" s="1"/>
       <c r="L275" s="1"/>
     </row>
-    <row r="276" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>53</v>
       </c>
@@ -23007,24 +24436,29 @@
       <c r="L276" s="1" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="277" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M276" s="1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E277" s="13"/>
       <c r="H277" s="14"/>
       <c r="I277" s="14"/>
       <c r="J277" s="14"/>
       <c r="K277" s="14"/>
       <c r="L277" s="14"/>
-    </row>
-    <row r="278" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M277" s="14"/>
+    </row>
+    <row r="278" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E278" s="13"/>
       <c r="H278" s="14"/>
       <c r="I278" s="14"/>
       <c r="J278" s="14"/>
       <c r="K278" s="14"/>
       <c r="L278" s="14"/>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M278" s="14"/>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>7</v>
       </c>
@@ -23055,13 +24489,16 @@
       <c r="L279" s="1" t="s">
         <v>1215</v>
       </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M279" s="1" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D280" s="10"/>
       <c r="K280" s="1"/>
       <c r="L280" s="1"/>
     </row>
-    <row r="281" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>7</v>
       </c>
@@ -23092,13 +24529,16 @@
       <c r="L281" s="1" t="s">
         <v>1216</v>
       </c>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M281" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D282" s="10"/>
       <c r="K282" s="1"/>
       <c r="L282" s="1"/>
     </row>
-    <row r="283" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>7</v>
       </c>
@@ -23129,13 +24569,16 @@
       <c r="L283" s="1" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M283" s="1" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D284" s="10"/>
       <c r="K284" s="1"/>
       <c r="L284" s="1"/>
     </row>
-    <row r="285" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>7</v>
       </c>
@@ -23166,13 +24609,16 @@
       <c r="L285" s="1" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M285" s="1" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D286" s="10"/>
       <c r="K286" s="1"/>
       <c r="L286" s="1"/>
     </row>
-    <row r="287" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>47</v>
       </c>
@@ -23200,8 +24646,11 @@
       <c r="L287" s="1" t="s">
         <v>1219</v>
       </c>
-    </row>
-    <row r="288" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M287" s="1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>47</v>
       </c>
@@ -23229,8 +24678,11 @@
       <c r="L288" s="1" t="s">
         <v>1220</v>
       </c>
-    </row>
-    <row r="289" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M288" s="1" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>47</v>
       </c>
@@ -23258,8 +24710,11 @@
       <c r="L289" s="1" t="s">
         <v>1221</v>
       </c>
-    </row>
-    <row r="290" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+      <c r="M289" s="1" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>47</v>
       </c>
@@ -23287,13 +24742,16 @@
       <c r="L290" s="1" t="s">
         <v>1222</v>
       </c>
-    </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M290" s="1" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D291" s="10"/>
       <c r="K291" s="1"/>
       <c r="L291" s="1"/>
     </row>
-    <row r="292" spans="1:12" ht="19" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:13" ht="19" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>53</v>
       </c>
@@ -23320,6 +24778,9 @@
       </c>
       <c r="L292" s="1" t="s">
         <v>1223</v>
+      </c>
+      <c r="M292" s="1" t="s">
+        <v>1441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>